<commit_message>
add '--update' to 'pip install' command; clean up text; add some todos
</commit_message>
<xml_diff>
--- a/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
+++ b/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25160" windowHeight="13600" tabRatio="993" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="37480" windowHeight="21140" tabRatio="993" firstSheet="1" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -236,10 +236,6 @@
     <t>hydrogenphosphate</t>
   </si>
   <si>
-    <t xml:space="preserve">InChI=1S/H3O4P/c1-5(2,3)4/h(H3,1,2,3,4)/p-2
-</t>
-  </si>
-  <si>
     <t>HO4P</t>
   </si>
   <si>
@@ -532,6 +528,9 @@
   </si>
   <si>
     <t>Rna</t>
+  </si>
+  <si>
+    <t>InChI=1S/H3O4P/c1-5(2,3)4/h(H3,1,2,3,4)/p-2</t>
   </si>
 </sst>
 </file>
@@ -609,7 +608,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -632,6 +631,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -1037,19 +1048,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="18" width="8.83203125" style="3"/>
+    <col min="1" max="1" width="8.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.1640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="42.5" style="3" customWidth="1"/>
+    <col min="6" max="6" width="6.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.5" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:18" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1060,119 +1088,119 @@
         <v>10</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>113</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>32</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>122</v>
       </c>
       <c r="R1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" ht="42" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>125</v>
       </c>
       <c r="G2" s="3">
         <v>2016</v>
       </c>
       <c r="H2" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>126</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>127</v>
       </c>
       <c r="L2" s="3">
         <v>44</v>
       </c>
       <c r="M2" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q2" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="Q2" s="3" t="s">
+    </row>
+    <row r="3" spans="1:18" ht="28" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>131</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>133</v>
       </c>
       <c r="G3" s="3">
         <v>2017</v>
       </c>
       <c r="H3" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>126</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>127</v>
       </c>
       <c r="L3" s="3">
         <v>45</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -1186,11 +1214,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="222" zoomScaleNormal="222" zoomScalePageLayoutView="222" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1200,39 +1228,39 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>137</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B2" s="1">
         <v>272634</v>
@@ -1246,10 +1274,10 @@
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>144</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>15</v>
@@ -1259,10 +1287,10 @@
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>18</v>
@@ -1272,10 +1300,10 @@
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>147</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>22</v>
@@ -1284,10 +1312,10 @@
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>25</v>
@@ -1296,10 +1324,10 @@
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>150</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>38</v>
@@ -1307,10 +1335,10 @@
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>54</v>
@@ -1318,10 +1346,10 @@
     </row>
     <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>33</v>
@@ -1329,10 +1357,10 @@
     </row>
     <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>42</v>
@@ -1340,10 +1368,10 @@
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>57</v>
@@ -1351,10 +1379,10 @@
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>50</v>
@@ -1362,13 +1390,13 @@
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>157</v>
-      </c>
       <c r="H13" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1381,14 +1409,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -1423,12 +1452,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="28" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="28" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -1443,16 +1472,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="210" zoomScaleNormal="210" zoomScalePageLayoutView="210" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="6" width="8.83203125" style="3"/>
+    <col min="1" max="1" width="15.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1513,19 +1547,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="218" zoomScaleNormal="218" zoomScalePageLayoutView="218" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="6" width="8.83203125" style="3"/>
+    <col min="1" max="1" width="5.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.1640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="11" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1545,7 +1584,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="42" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
@@ -1562,7 +1601,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="28" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>25</v>
       </c>
@@ -1590,276 +1629,302 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="10" width="8.83203125" style="3"/>
+    <col min="1" max="1" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="59.5" style="3" customWidth="1"/>
+    <col min="5" max="5" width="20" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" ht="42" x14ac:dyDescent="0.15">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:10" s="4" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:10" ht="42" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="11">
         <v>424.1773</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="12">
         <v>-3</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="6"/>
-    </row>
-    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="I2" s="13"/>
+      <c r="J2" s="12"/>
+    </row>
+    <row r="3" spans="1:10" ht="42" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="12">
         <v>345.20530000000002</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="12">
         <v>-2</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="6"/>
-    </row>
-    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="I3" s="13"/>
+      <c r="J3" s="12"/>
+    </row>
+    <row r="4" spans="1:10" ht="56" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="11">
         <v>503.14945999999998</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="12">
         <v>-4</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="6"/>
-    </row>
-    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="I4" s="13"/>
+      <c r="J4" s="12"/>
+    </row>
+    <row r="5" spans="1:10" ht="42" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="11">
         <v>180.15588</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="12">
         <v>0</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="I5" s="6"/>
-    </row>
-    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="I5" s="13"/>
+      <c r="J5" s="12"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="11">
         <v>1.00783</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="12">
         <v>1</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="I6" s="6"/>
-    </row>
-    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="I6" s="13"/>
+      <c r="J6" s="12"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="11">
         <v>18.0153</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="12">
         <v>0</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="12" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="E8" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="12">
+        <v>95.979299999999995</v>
+      </c>
+      <c r="G8" s="12">
+        <v>-2</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F8" s="3">
-        <v>95.979299999999995</v>
-      </c>
-      <c r="G8" s="3">
-        <v>-2</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="B9" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="E9" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="12">
+        <v>3298.9857699999998</v>
+      </c>
+      <c r="G9" s="12">
+        <v>-11</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F9" s="3">
-        <v>3298.9857699999998</v>
-      </c>
-      <c r="G9" s="3">
-        <v>-11</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>67</v>
-      </c>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J6"/>
@@ -1872,24 +1937,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="180" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="8.83203125" style="3"/>
+    <col min="1" max="1" width="10.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>7</v>
@@ -1900,7 +1968,7 @@
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B2" s="6">
         <v>5.0000000000000001E-3</v>
@@ -1908,7 +1976,7 @@
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B3" s="6">
         <v>5.0000000000000001E-3</v>
@@ -1916,7 +1984,7 @@
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B4" s="6">
         <v>5.0000000000000001E-3</v>
@@ -1924,7 +1992,7 @@
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B5" s="6">
         <v>0.01</v>
@@ -1932,7 +2000,7 @@
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B6" s="3">
         <v>9.9999999999999995E-8</v>
@@ -1940,7 +2008,7 @@
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B7" s="6">
         <v>55</v>
@@ -1948,7 +2016,7 @@
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B8" s="5">
         <v>5.0000000000000001E-3</v>
@@ -1965,11 +2033,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="142" zoomScaleNormal="142" zoomScalePageLayoutView="142" workbookViewId="0">
+    <sheetView zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="180" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A1:G5"/>
+      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1991,13 +2059,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>7</v>
@@ -2008,16 +2076,16 @@
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E2" s="8">
         <v>0</v>
@@ -2027,16 +2095,16 @@
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>84</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E3" s="8">
         <v>0</v>
@@ -2046,16 +2114,16 @@
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>87</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E4" s="8">
         <v>0</v>
@@ -2065,16 +2133,16 @@
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>90</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E5" s="3">
         <v>0</v>
@@ -2110,19 +2178,19 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>7</v>
@@ -2133,13 +2201,13 @@
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="D2" s="5">
         <v>2.9999999999999997E-4</v>
@@ -2150,13 +2218,13 @@
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="D3" s="5">
         <v>2.9999999999999997E-4</v>
@@ -2167,26 +2235,26 @@
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D4"/>
       <c r="E4"/>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D5" s="5">
         <v>2000</v>
@@ -2197,13 +2265,13 @@
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D6" s="5">
         <v>2.9999999999999997E-4</v>
@@ -2221,16 +2289,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="195" zoomScaleNormal="195" zoomScalePageLayoutView="195" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="8" width="8.83203125" style="3"/>
+    <col min="1" max="1" width="15.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -2244,13 +2319,13 @@
         <v>10</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>7</v>
@@ -2261,10 +2336,10 @@
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>1</v>
@@ -2273,10 +2348,10 @@
         <v>0.3</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rename wc_lang.core.CrossReference to wc_lang.core.DatabaseReference to replace an ambiguous name with a clear one
</commit_message>
<xml_diff>
--- a/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
+++ b/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
@@ -22,7 +22,7 @@
     <sheet name="Rate laws" sheetId="8" r:id="rId8"/>
     <sheet name="Parameters" sheetId="9" r:id="rId9"/>
     <sheet name="References" sheetId="10" r:id="rId10"/>
-    <sheet name="Cross references" sheetId="11" r:id="rId11"/>
+    <sheet name="Database references" sheetId="11" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3">Compartments!$A$1:$E$3</definedName>
@@ -1218,7 +1218,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O25" sqref="O25"/>
+      <selection pane="bottomRight" activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updating for revised wc_lang
</commit_message>
<xml_diff>
--- a/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
+++ b/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,27 +26,34 @@
     <sheet name="Database references" sheetId="16" state="visible" r:id="rId17"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
+    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
     <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">Concentrations!$A$1:$D$8</definedName>
     <definedName function="false" hidden="true" localSheetId="12" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
     <definedName function="false" hidden="true" localSheetId="9" name="_xlnm._FilterDatabase" vbProcedure="false">'Rate laws'!$A$1:$G$6</definedName>
     <definedName function="false" hidden="true" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="true" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
+    <definedName function="false" hidden="true" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_FilterDatabase_0" vbProcedure="false">submodels!#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Submodels!$A$1:$I$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Submodels!$A$1:$H$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">Concentrations!$A$1:$D$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0" vbProcedure="false">Concentrations!$A$1:$D$8</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase" vbProcedure="false">'Rate laws'!$A$1:$G$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Rate laws'!$A$1:$G$6</definedName>
     <definedName function="false" hidden="false" localSheetId="12" name="_FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
     <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0" vbProcedure="false">References!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0" vbProcedure="false">References!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -58,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="170">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -106,9 +113,6 @@
   </si>
   <si>
     <t xml:space="preserve">Mycoplasma pneumoniae M129</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Model</t>
   </si>
   <si>
     <t xml:space="preserve">Rank</t>
@@ -416,6 +420,9 @@
   </si>
   <si>
     <t xml:space="preserve">Species type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model</t>
   </si>
   <si>
     <t xml:space="preserve">Submodels</t>
@@ -944,48 +951,48 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.6720647773279"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="25.7085020242915"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="8.46153846153846"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.2834008097166"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.7125506072874"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>109</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B2" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="D2" s="5" t="n">
         <v>0.0003</v>
@@ -996,13 +1003,13 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="D3" s="5" t="n">
         <v>0.0003</v>
@@ -1013,26 +1020,26 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D4" s="0"/>
       <c r="E4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D5" s="5" t="n">
         <v>2000</v>
@@ -1043,13 +1050,13 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D6" s="5" t="n">
         <v>0.0003</v>
@@ -1082,7 +1089,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1093,19 +1100,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="E1" s="0" t="s">
         <v>117</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>118</v>
       </c>
       <c r="F1" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1132,7 +1139,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1143,13 +1150,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1175,17 +1182,17 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="33.7408906882591"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="34.0647773279352"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="20.5668016194332"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="3" width="13.7125506072874"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="3" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="12.8542510121458"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="3" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="3" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.78542510121457"/>
@@ -1199,13 +1206,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>118</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>119</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>120</v>
@@ -1214,7 +1221,7 @@
         <v>13</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1255,18 +1262,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -1274,12 +1281,9 @@
         <v>2</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>16</v>
+        <v>86</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="E1" s="0" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1299,40 +1303,39 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R3"/>
+  <dimension ref="1:3"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="bottomRight" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="3" width="8.35627530364373"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="29.3522267206478"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="42.7408906882591"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="6.31983805668016"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="5.1417004048583"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="3" width="6"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="3" width="15.8542510121457"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="3" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="3" width="6.63967611336032"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="3" width="7.71255060728745"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="3" width="8.03238866396761"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="3" width="5.78542510121457"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="3" width="7.39271255060729"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="3" width="8.03238866396761"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="3" width="12.5344129554656"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="3" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="43.17004048583"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="6.31983805668016"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="5.1417004048583"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="6"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="3" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="3" width="9.4251012145749"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="3" width="6.63967611336032"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="3" width="7.71255060728745"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="3" width="8.03238866396761"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="3" width="5.78542510121457"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="3" width="7.49797570850202"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="3" width="8.03238866396761"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="3" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="3" width="10.497975708502"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="4" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1340,126 +1343,118 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>125</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>128</v>
+        <v>40</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>41</v>
+        <v>129</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="R1" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>124</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
+      <c r="C2" s="3" t="s">
+        <v>139</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="E2" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="G2" s="3" t="n">
+      <c r="F2" s="3" t="n">
         <v>2016</v>
       </c>
+      <c r="G2" s="3" t="s">
+        <v>141</v>
+      </c>
       <c r="H2" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="I2" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="L2" s="3" t="n">
+      <c r="K2" s="3" t="n">
         <v>44</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>145</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>1</v>
+      <c r="C3" s="3" t="s">
+        <v>147</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="E3" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="G3" s="3" t="n">
+      <c r="F3" s="3" t="n">
         <v>2017</v>
       </c>
+      <c r="G3" s="3" t="s">
+        <v>141</v>
+      </c>
       <c r="H3" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="I3" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="L3" s="3" t="n">
+      <c r="K3" s="3" t="n">
         <v>45</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>149</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1"/>
+  <autoFilter ref="A1:D1"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1503,22 +1498,22 @@
         <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>16</v>
+        <v>118</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>152</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>153</v>
@@ -1546,7 +1541,7 @@
         <v>156</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G3" s="0"/>
       <c r="H3" s="0"/>
@@ -1559,7 +1554,7 @@
         <v>157</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G4" s="0"/>
       <c r="H4" s="0"/>
@@ -1572,7 +1567,7 @@
         <v>159</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H5" s="0"/>
     </row>
@@ -1584,7 +1579,7 @@
         <v>160</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H6" s="0"/>
     </row>
@@ -1596,7 +1591,7 @@
         <v>162</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1607,7 +1602,7 @@
         <v>163</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1618,7 +1613,7 @@
         <v>164</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1629,7 +1624,7 @@
         <v>165</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1640,7 +1635,7 @@
         <v>166</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1651,7 +1646,7 @@
         <v>167</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1662,7 +1657,7 @@
         <v>169</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1681,18 +1676,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.6356275303644"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.8502024291498"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -1717,25 +1712,17 @@
         <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1754,25 +1741,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="210" zoomScaleNormal="210" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="bottomRight" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="9.74898785425101"/>
-    <col collapsed="false" hidden="false" max="8" min="5" style="3" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="3" width="11.0323886639676"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="9.85425101214575"/>
+    <col collapsed="false" hidden="false" max="7" min="4" style="3" width="10.497975708502"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="3" width="11.0323886639676"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1783,7 +1769,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>20</v>
@@ -1795,41 +1781,32 @@
         <v>22</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1848,28 +1825,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="1:3"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="218" zoomScaleNormal="218" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="3" width="5.35627530364372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="16.8178137651822"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="15.5303643724696"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="56.5587044534413"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="11.0323886639676"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="16.9230769230769"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="56.9878542510121"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="11.0323886639676"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="4" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1877,54 +1853,46 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="B2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="5" t="n">
+        <v>4.58E-017</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="5" t="n">
-        <v>4.58E-017</v>
-      </c>
-      <c r="E2" s="3" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="5" t="n">
+        <v>1E-012</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="5" t="n">
-        <v>1E-012</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>36</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E3"/>
+  <autoFilter ref="A1:D3"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1941,32 +1909,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="1:10"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="bottomRight" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="9.74898785425101"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="17.4615384615385"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="59.9878542510121"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="10.0688259109312"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="3" width="14.4615384615385"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="3" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="3" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="9.85425101214575"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="60.5222672064777"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="10.8178137651822"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="3" width="10.497975708502"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="3" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="4" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1974,7 +1941,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>37</v>
@@ -1989,261 +1956,232 @@
         <v>40</v>
       </c>
       <c r="H1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+      <c r="B2" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>43</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>1</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="n">
+        <v>424.1773</v>
+      </c>
+      <c r="F2" s="8" t="n">
+        <v>-3</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="7" t="n">
-        <v>424.1773</v>
-      </c>
-      <c r="G2" s="8" t="n">
-        <v>-3</v>
-      </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="9"/>
+      <c r="I2" s="8"/>
+    </row>
+    <row r="3" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="I2" s="9"/>
-      <c r="J2" s="8"/>
-    </row>
-    <row r="3" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+      <c r="B3" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="C3" s="8" t="s">
         <v>48</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>1</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="8" t="n">
+        <v>345.2053</v>
+      </c>
+      <c r="F3" s="8" t="n">
+        <v>-2</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="9"/>
+      <c r="I3" s="8"/>
+    </row>
+    <row r="4" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="8" t="n">
-        <v>345.2053</v>
-      </c>
-      <c r="G3" s="8" t="n">
-        <v>-2</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="I3" s="9"/>
-      <c r="J3" s="8"/>
-    </row>
-    <row r="4" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
+      <c r="B4" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="C4" s="8" t="s">
         <v>52</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>1</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="7" t="n">
+        <v>503.14946</v>
+      </c>
+      <c r="F4" s="8" t="n">
+        <v>-4</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="9"/>
+      <c r="I4" s="8"/>
+    </row>
+    <row r="5" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="7" t="n">
-        <v>503.14946</v>
-      </c>
-      <c r="G4" s="8" t="n">
-        <v>-4</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="I4" s="9"/>
-      <c r="J4" s="8"/>
-    </row>
-    <row r="5" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
+      <c r="B5" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="C5" s="8" t="s">
         <v>56</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>1</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="n">
+        <v>180.15588</v>
+      </c>
+      <c r="F5" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" s="9"/>
+      <c r="I5" s="8"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="7" t="n">
-        <v>180.15588</v>
-      </c>
-      <c r="G5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="I5" s="9"/>
-      <c r="J5" s="8"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
+      <c r="B6" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="8" t="s">
         <v>60</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>1</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="7" t="n">
+        <v>1.00783</v>
+      </c>
+      <c r="F6" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="9"/>
+      <c r="I6" s="8"/>
+    </row>
+    <row r="7" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="F6" s="7" t="n">
-        <v>1.00783</v>
-      </c>
-      <c r="G6" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="I6" s="9"/>
-      <c r="J6" s="8"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="s">
+      <c r="B7" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="C7" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>1</v>
-      </c>
       <c r="D7" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="7" t="n">
+        <v>18.0153</v>
+      </c>
+      <c r="F7" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F7" s="7" t="n">
-        <v>18.0153</v>
-      </c>
-      <c r="G7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
+      <c r="B8" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="C8" s="8" t="s">
         <v>67</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>1</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="8" t="n">
+        <v>95.9793</v>
+      </c>
+      <c r="F8" s="8" t="n">
+        <v>-2</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+    </row>
+    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F8" s="8" t="n">
-        <v>95.9793</v>
-      </c>
-      <c r="G8" s="8" t="n">
-        <v>-2</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
+      <c r="B9" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="C9" s="8" t="s">
         <v>71</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>1</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="8" t="n">
+        <v>3298.98577</v>
+      </c>
+      <c r="F9" s="8" t="n">
+        <v>-11</v>
+      </c>
+      <c r="G9" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="F9" s="8" t="n">
-        <v>3298.98577</v>
-      </c>
-      <c r="G9" s="8" t="n">
-        <v>-11</v>
-      </c>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+    </row>
+    <row r="10" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
-        <v>75</v>
-      </c>
       <c r="B10" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>1</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="9" t="s">
-        <v>76</v>
-      </c>
+      <c r="G10" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="H10" s="8"/>
       <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J6"/>
+  <autoFilter ref="A1:I6"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2273,29 +2211,29 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="3" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="10.0688259109312"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="13.2834008097166"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="3" width="13.7125506072874"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B2" s="10" t="n">
         <v>0.005</v>
@@ -2303,7 +2241,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" s="10" t="n">
         <v>0.005</v>
@@ -2311,7 +2249,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4" s="10" t="n">
         <v>0.005</v>
@@ -2319,7 +2257,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5" s="10" t="n">
         <v>0.01</v>
@@ -2327,7 +2265,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B6" s="3" t="n">
         <v>1E-007</v>
@@ -2335,7 +2273,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B7" s="10" t="n">
         <v>55</v>
@@ -2343,7 +2281,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B8" s="5" t="n">
         <v>0.005</v>
@@ -2367,18 +2305,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -2386,15 +2324,12 @@
         <v>2</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>16</v>
+        <v>76</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="F1" s="0" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2414,18 +2349,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -2433,12 +2368,9 @@
         <v>2</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>16</v>
+        <v>86</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="E1" s="0" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2460,7 +2392,7 @@
   </sheetPr>
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
@@ -2470,10 +2402,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="21.1012145748988"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="14.7813765182186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="46.7044534412956"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="14.8906882591093"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="47.0242914979757"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="3" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="8" min="6" style="3" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="3" width="11.1417004048583"/>
@@ -2488,39 +2420,39 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>94</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>95</v>
       </c>
       <c r="E2" s="12" t="n">
         <v>0</v>
@@ -2532,16 +2464,16 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="E3" s="12" t="n">
         <v>0</v>
@@ -2553,16 +2485,16 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>100</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>101</v>
       </c>
       <c r="E4" s="12" t="n">
         <v>0</v>
@@ -2574,16 +2506,16 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>104</v>
       </c>
       <c r="E5" s="3" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
updating for addition of wc_lang.Concentration.units
</commit_message>
<xml_diff>
--- a/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
+++ b/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="14"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
-    <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">Concentrations!$A$1:$D$8</definedName>
+    <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">Concentrations!$A$1:$E$8</definedName>
     <definedName function="false" hidden="true" localSheetId="12" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
     <definedName function="false" hidden="true" localSheetId="9" name="_xlnm._FilterDatabase" vbProcedure="false">'Rate laws'!$A$1:$G$6</definedName>
     <definedName function="false" hidden="true" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
@@ -38,22 +38,29 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">Concentrations!$A$1:$D$8</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0" vbProcedure="false">Concentrations!$A$1:$D$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">Concentrations!$A$1:$E$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0" vbProcedure="false">Concentrations!$A$1:$E$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Concentrations!$A$1:$E$8</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase" vbProcedure="false">'Rate laws'!$A$1:$G$6</definedName>
     <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Rate laws'!$A$1:$G$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Rate laws'!$A$1:$G$6</definedName>
     <definedName function="false" hidden="false" localSheetId="12" name="_FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
     <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
     <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -65,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="171">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -302,9 +309,15 @@
     <t xml:space="preserve">Value</t>
   </si>
   <si>
+    <t xml:space="preserve">Units</t>
+  </si>
+  <si>
     <t xml:space="preserve">adp[c]</t>
   </si>
   <si>
+    <t xml:space="preserve">M</t>
+  </si>
+  <si>
     <t xml:space="preserve">atp[c]</t>
   </si>
   <si>
@@ -426,9 +439,6 @@
   </si>
   <si>
     <t xml:space="preserve">Submodels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Units</t>
   </si>
   <si>
     <t xml:space="preserve">fractionDryWeight</t>
@@ -951,31 +961,31 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.7813765182186"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="25.8137651821862"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="8.46153846153846"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.7125506072874"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>13</v>
@@ -986,13 +996,13 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D2" s="5" t="n">
         <v>0.0003</v>
@@ -1003,13 +1013,13 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D3" s="5" t="n">
         <v>0.0003</v>
@@ -1020,26 +1030,26 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D4" s="0"/>
       <c r="E4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D5" s="5" t="n">
         <v>2000</v>
@@ -1050,13 +1060,13 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D6" s="5" t="n">
         <v>0.0003</v>
@@ -1103,10 +1113,10 @@
         <v>21</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="F1" s="0" t="s">
         <v>13</v>
@@ -1187,12 +1197,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="15.8542510121457"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="34.0647773279352"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="34.3846153846154"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="20.6720647773279"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="3" width="13.7125506072874"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="3" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="12.9595141700405"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="3" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="3" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.78542510121457"/>
@@ -1206,16 +1216,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>77</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>120</v>
+        <v>78</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>13</v>
@@ -1226,10 +1236,10 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>1</v>
@@ -1238,10 +1248,10 @@
         <v>0.3</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1281,7 +1291,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>13</v>
@@ -1305,7 +1315,7 @@
   </sheetPr>
   <dimension ref="1:3"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -1316,13 +1326,13 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="3" width="8.35627530364373"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="17.995951417004"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="29.5668016194332"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="43.17004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="29.7773279352227"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="43.5991902834008"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="3" width="6.31983805668016"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="3" width="5.1417004048583"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="3" width="6"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="3" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="3" width="16.0688259109312"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="3" width="9.4251012145749"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="3" width="6.63967611336032"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="3" width="7.71255060728745"/>
@@ -1330,7 +1340,7 @@
     <col collapsed="false" hidden="false" max="13" min="13" style="3" width="5.78542510121457"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="3" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="3" width="8.03238866396761"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="3" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="3" width="12.748987854251"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="3" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="8.78542510121457"/>
   </cols>
@@ -1343,46 +1353,46 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>13</v>
@@ -1391,66 +1401,66 @@
     </row>
     <row r="2" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F2" s="3" t="n">
         <v>2016</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="K2" s="3" t="n">
         <v>44</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F3" s="3" t="n">
         <v>2017</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="K3" s="3" t="n">
         <v>45</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -1489,39 +1499,39 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>20</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>272634</v>
@@ -1535,10 +1545,10 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>23</v>
@@ -1548,10 +1558,10 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>26</v>
@@ -1561,10 +1571,10 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>30</v>
@@ -1573,10 +1583,10 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>33</v>
@@ -1585,10 +1595,10 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>46</v>
@@ -1596,10 +1606,10 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>62</v>
@@ -1607,10 +1617,10 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>41</v>
@@ -1618,10 +1628,10 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>50</v>
@@ -1629,10 +1639,10 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>65</v>
@@ -1640,10 +1650,10 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>58</v>
@@ -1651,10 +1661,10 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>69</v>
@@ -1687,7 +1697,7 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.8502024291498"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="28.0647773279352"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -1753,9 +1763,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="15.5303643724696"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="15.3198380566802"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="9.85425101214575"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="9.96356275303644"/>
     <col collapsed="false" hidden="false" max="7" min="4" style="3" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="3" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.78542510121457"/>
@@ -1838,9 +1848,9 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="3" width="5.35627530364372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="16.9230769230769"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="56.9878542510121"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="17.0323886639676"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="57.5222672064777"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="3" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.78542510121457"/>
   </cols>
@@ -1921,15 +1931,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="9.85425101214575"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="17.5668016194332"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="60.5222672064777"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="61.0566801619433"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="20.3522267206478"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="3" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="10.1781376518219"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="14.6761133603239"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="3" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="3" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="3" width="12.9595141700405"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -2198,23 +2208,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="bottomRight" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="3" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="10.1781376518219"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="13.2834008097166"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="3" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="13.7125506072874"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2225,70 +2235,94 @@
         <v>77</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B2" s="10" t="n">
         <v>0.005</v>
       </c>
+      <c r="C2" s="10" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B3" s="10" t="n">
         <v>0.005</v>
       </c>
+      <c r="C3" s="10" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B4" s="10" t="n">
         <v>0.005</v>
       </c>
+      <c r="C4" s="10" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B5" s="10" t="n">
         <v>0.01</v>
       </c>
+      <c r="C5" s="10" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B6" s="3" t="n">
         <v>1E-007</v>
       </c>
+      <c r="C6" s="10" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B7" s="10" t="n">
         <v>55</v>
       </c>
+      <c r="C7" s="10" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B8" s="5" t="n">
         <v>0.005</v>
       </c>
+      <c r="C8" s="10" t="s">
+        <v>80</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D8"/>
+  <autoFilter ref="A1:E8"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2327,7 +2361,7 @@
         <v>76</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>13</v>
@@ -2368,7 +2402,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>13</v>
@@ -2402,10 +2436,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="14.8906882591093"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="47.0242914979757"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="47.3481781376518"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="3" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="8" min="6" style="3" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="3" width="11.1417004048583"/>
@@ -2420,19 +2454,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>13</v>
@@ -2443,16 +2477,16 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E2" s="12" t="n">
         <v>0</v>
@@ -2464,16 +2498,16 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E3" s="12" t="n">
         <v>0</v>
@@ -2485,16 +2519,16 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E4" s="12" t="n">
         <v>0</v>
@@ -2506,16 +2540,16 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E5" s="3" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
updating for new Species table in wc_lang (Species definied explicitly rather than inline)
</commit_message>
<xml_diff>
--- a/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
+++ b/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,25 +13,26 @@
     <sheet name="Submodels" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Compartments" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Species types" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Concentrations" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Observables" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="Functions" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="Reactions" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="Rate laws" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="Biomass components" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="Biomass reactions" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="Parameters" sheetId="13" state="visible" r:id="rId14"/>
-    <sheet name="Stop conditions" sheetId="14" state="visible" r:id="rId15"/>
-    <sheet name="References" sheetId="15" state="visible" r:id="rId16"/>
-    <sheet name="Database references" sheetId="16" state="visible" r:id="rId17"/>
+    <sheet name="Species" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Concentrations" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Observables" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Functions" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Reactions" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Rate laws" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="Biomass components" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="Biomass reactions" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="Parameters" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="Stop conditions" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="References" sheetId="16" state="visible" r:id="rId17"/>
+    <sheet name="Database references" sheetId="17" state="visible" r:id="rId18"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
-    <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">Concentrations!$A$1:$E$8</definedName>
-    <definedName function="false" hidden="true" localSheetId="12" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="true" localSheetId="9" name="_xlnm._FilterDatabase" vbProcedure="false">'Rate laws'!$A$1:$G$6</definedName>
-    <definedName function="false" hidden="true" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="true" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="6" name="_xlnm._FilterDatabase" vbProcedure="false">Concentrations!$A$1:$E$8</definedName>
+    <definedName function="false" hidden="true" localSheetId="13" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="10" name="_xlnm._FilterDatabase" vbProcedure="false">'Rate laws'!$A$1:$G$6</definedName>
+    <definedName function="false" hidden="true" localSheetId="9" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="true" localSheetId="15" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_FilterDatabase_0" vbProcedure="false">submodels!#REF!</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Submodels!$A$1:$G$3</definedName>
@@ -39,28 +40,35 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="excel_is_bugging_me" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_FilterDatabase_0" vbProcedure="false">Concentrations!$A$1:$E$8</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_FilterDatabase_0_0" vbProcedure="false">Concentrations!$A$1:$E$8</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">Concentrations!$A$1:$E$8</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="excel_is_bugging_me" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="9" name="_FilterDatabase_0" vbProcedure="false">'Rate laws'!$A$1:$G$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="9" name="_FilterDatabase_0_0" vbProcedure="false">'Rate laws'!$A$1:$G$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase" vbProcedure="false">'Rate laws'!$A$1:$G$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="12" name="excel_is_bugging_me" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="12" name="_FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="12" name="_FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="excel_is_bugging_me" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_FilterDatabase_0" vbProcedure="false">Concentrations!$A$1:$E$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_FilterDatabase_0_0" vbProcedure="false">Concentrations!$A$1:$E$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase" vbProcedure="false">Concentrations!$A$1:$E$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0" vbProcedure="false">Concentrations!$A$1:$E$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="excel_is_bugging_me" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0" vbProcedure="false">'Rate laws'!$A$1:$G$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0_0" vbProcedure="false">'Rate laws'!$A$1:$G$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase" vbProcedure="false">'Rate laws'!$A$1:$G$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Rate laws'!$A$1:$G$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="13" name="excel_is_bugging_me" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="13" name="_FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="13" name="_FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="15" name="excel_is_bugging_me" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="15" name="_FilterDatabase_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="15" name="_FilterDatabase_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0" vbProcedure="false">References!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -72,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="173">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -300,6 +308,42 @@
     <t xml:space="preserve">pseudo_species</t>
   </si>
   <si>
+    <t xml:space="preserve">Species type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compartment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adp[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">amp[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">atp[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biomass[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">glc[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">glc[e]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h2o[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pi[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rna_dec_a[c]</t>
+  </si>
+  <si>
     <t xml:space="preserve">Species</t>
   </si>
   <si>
@@ -309,30 +353,9 @@
     <t xml:space="preserve">Units</t>
   </si>
   <si>
-    <t xml:space="preserve">adp[c]</t>
-  </si>
-  <si>
     <t xml:space="preserve">M</t>
   </si>
   <si>
-    <t xml:space="preserve">atp[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">glc[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">glc[e]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">h[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">h2o[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pi[c]</t>
-  </si>
-  <si>
     <t xml:space="preserve">Expression</t>
   </si>
   <si>
@@ -424,12 +447,6 @@
   </si>
   <si>
     <t xml:space="preserve">Coefficient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Species type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Compartment</t>
   </si>
   <si>
     <t xml:space="preserve">Model</t>
@@ -589,13 +606,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
     <numFmt numFmtId="166" formatCode="0.000E+00"/>
     <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -630,6 +648,14 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -693,7 +719,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -718,24 +744,20 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -746,7 +768,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -950,10 +972,155 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D2" activeCellId="0" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="9" min="1" style="3" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.78542510121457"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="4" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="12"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E3" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="12"/>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="E4" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D5"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -964,19 +1131,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>13</v>
@@ -987,13 +1154,13 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>109</v>
+        <v>97</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>114</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="D2" s="5" t="n">
         <v>0.0003</v>
@@ -1004,13 +1171,13 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>111</v>
+        <v>97</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>116</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="D3" s="5" t="n">
         <v>0.0003</v>
@@ -1021,26 +1188,26 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>111</v>
+        <v>100</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>116</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="D4" s="0"/>
       <c r="E4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>111</v>
+        <v>103</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>116</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="D5" s="5" t="n">
         <v>2000</v>
@@ -1051,13 +1218,13 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>111</v>
+        <v>106</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>116</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="D6" s="5" t="n">
         <v>0.0003</v>
@@ -1077,7 +1244,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1104,10 +1271,10 @@
         <v>20</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>117</v>
+        <v>75</v>
       </c>
       <c r="F1" s="0" t="s">
         <v>13</v>
@@ -1127,7 +1294,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1151,7 +1318,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>118</v>
+        <v>76</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>13</v>
@@ -1171,14 +1338,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="195" zoomScaleNormal="195" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -1200,16 +1367,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>13</v>
@@ -1220,10 +1387,10 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>1</v>
@@ -1232,10 +1399,10 @@
         <v>0.3</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1251,7 +1418,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1275,7 +1442,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>13</v>
@@ -1292,14 +1459,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -1321,46 +1488,46 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>39</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>13</v>
@@ -1368,66 +1535,66 @@
     </row>
     <row r="2" customFormat="false" ht="224" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="F2" s="3" t="n">
         <v>2016</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="K2" s="3" t="n">
         <v>44</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="168" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F3" s="3" t="n">
         <v>2017</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="K3" s="3" t="n">
         <v>45</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -1443,14 +1610,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="222" zoomScaleNormal="222" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
@@ -1466,39 +1633,39 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>118</v>
+        <v>76</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>117</v>
+        <v>75</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>272634</v>
@@ -1512,10 +1679,10 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>22</v>
@@ -1525,10 +1692,10 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>25</v>
@@ -1538,10 +1705,10 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>29</v>
@@ -1550,10 +1717,10 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>32</v>
@@ -1562,10 +1729,10 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>45</v>
@@ -1573,10 +1740,10 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>61</v>
@@ -1584,10 +1751,10 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>40</v>
@@ -1595,10 +1762,10 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>49</v>
@@ -1606,10 +1773,10 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>64</v>
@@ -1617,10 +1784,10 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>57</v>
@@ -1628,10 +1795,10 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>68</v>
@@ -1655,7 +1822,7 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="A3" activeCellId="0" sqref="A3"/>
@@ -1719,7 +1886,7 @@
   </sheetPr>
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="210" zoomScaleNormal="210" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -1796,7 +1963,7 @@
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="218" zoomScaleNormal="218" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -1875,265 +2042,248 @@
   </sheetPr>
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomRight" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.7"/>
   <cols>
     <col collapsed="false" hidden="false" max="9" min="1" style="3" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="6" width="8.78542510121457"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
+    <row r="1" s="3" customFormat="true" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="350" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+    <row r="2" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="7" t="n">
+      <c r="E2" s="3" t="n">
         <v>424.1773</v>
       </c>
-      <c r="F2" s="8" t="n">
+      <c r="F2" s="3" t="n">
         <v>-3</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="9"/>
-      <c r="I2" s="8"/>
-    </row>
-    <row r="3" customFormat="false" ht="308" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+      <c r="H2" s="7"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E3" s="8" t="n">
+      <c r="E3" s="3" t="n">
         <v>345.2053</v>
       </c>
-      <c r="F3" s="8" t="n">
+      <c r="F3" s="3" t="n">
         <v>-2</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="8"/>
-    </row>
-    <row r="4" customFormat="false" ht="392" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="7" t="n">
+      <c r="E4" s="3" t="n">
         <v>503.14946</v>
       </c>
-      <c r="F4" s="8" t="n">
+      <c r="F4" s="3" t="n">
         <v>-4</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H4" s="9"/>
-      <c r="I4" s="8"/>
-    </row>
-    <row r="5" customFormat="false" ht="168" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E5" s="7" t="n">
+      <c r="E5" s="3" t="n">
         <v>180.15588</v>
       </c>
-      <c r="F5" s="8" t="n">
+      <c r="F5" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H5" s="9"/>
-      <c r="I5" s="8"/>
-    </row>
-    <row r="6" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E6" s="7" t="n">
+      <c r="E6" s="3" t="n">
         <v>1.00783</v>
       </c>
-      <c r="F6" s="8" t="n">
+      <c r="F6" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H6" s="9"/>
-      <c r="I6" s="8"/>
-    </row>
-    <row r="7" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="s">
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E7" s="7" t="n">
+      <c r="E7" s="3" t="n">
         <v>18.0153</v>
       </c>
-      <c r="F7" s="8" t="n">
+      <c r="F7" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-    </row>
-    <row r="8" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E8" s="8" t="n">
+      <c r="E8" s="3" t="n">
         <v>95.9793</v>
       </c>
-      <c r="F8" s="8" t="n">
+      <c r="F8" s="3" t="n">
         <v>-2</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-    </row>
-    <row r="9" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E9" s="8" t="n">
+      <c r="E9" s="3" t="n">
         <v>3298.98577</v>
       </c>
-      <c r="F9" s="8" t="n">
+      <c r="F9" s="3" t="n">
         <v>-11</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-    </row>
-    <row r="10" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I6"/>
@@ -2153,14 +2303,186 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="bottomRight" activeCell="B20" activeCellId="0" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.1417004048583"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2171,13 +2493,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>13</v>
@@ -2188,46 +2510,46 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2" s="10" t="n">
+        <v>77</v>
+      </c>
+      <c r="B2" s="7" t="n">
         <v>0.005</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>79</v>
+      <c r="C2" s="7" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B3" s="10" t="n">
+        <v>79</v>
+      </c>
+      <c r="B3" s="7" t="n">
         <v>0.005</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>79</v>
+      <c r="C3" s="7" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="10" t="n">
+      <c r="B4" s="7" t="n">
         <v>0.005</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>79</v>
+      <c r="C4" s="7" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B5" s="10" t="n">
+      <c r="B5" s="7" t="n">
         <v>0.01</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>79</v>
+      <c r="C5" s="7" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2237,19 +2559,19 @@
       <c r="B6" s="3" t="n">
         <v>1E-007</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>79</v>
+      <c r="C6" s="7" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="10" t="n">
+      <c r="B7" s="7" t="n">
         <v>55</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>79</v>
+      <c r="C7" s="7" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2259,8 +2581,8 @@
       <c r="B8" s="5" t="n">
         <v>0.005</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>79</v>
+      <c r="C8" s="7" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2276,7 +2598,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -2300,7 +2622,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>13</v>
@@ -2317,7 +2639,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -2341,7 +2663,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>13</v>
@@ -2356,149 +2678,4 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:I5"/>
-  <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F2" activeCellId="0" sqref="F2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="9" min="1" style="3" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.78542510121457"/>
-  </cols>
-  <sheetData>
-    <row r="1" s="4" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="E2" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="13"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E3" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="13"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="E4" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:D5"/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
updating for revisions to wc-lang
</commit_message>
<xml_diff>
--- a/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
+++ b/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,8 +19,8 @@
     <sheet name="Functions" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="Reactions" sheetId="10" state="visible" r:id="rId11"/>
     <sheet name="Rate laws" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="Biomass components" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="Biomass reactions" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="Biomass reactions" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="Biomass components" sheetId="13" state="visible" r:id="rId14"/>
     <sheet name="Parameters" sheetId="14" state="visible" r:id="rId15"/>
     <sheet name="Stop conditions" sheetId="15" state="visible" r:id="rId16"/>
     <sheet name="References" sheetId="16" state="visible" r:id="rId17"/>
@@ -35,40 +35,47 @@
     <definedName function="false" hidden="true" localSheetId="15" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_FilterDatabase_0" vbProcedure="false">submodels!#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Submodels!$A$1:$G$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Submodels!$A$1:$F$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="excel_is_bugging_me" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="excel_is_bugging_me" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_FilterDatabase_0" vbProcedure="false">Concentrations!$A$1:$E$8</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_FilterDatabase_0_0" vbProcedure="false">Concentrations!$A$1:$E$8</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase" vbProcedure="false">Concentrations!$A$1:$E$8</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0" vbProcedure="false">Concentrations!$A$1:$E$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Concentrations!$A$1:$E$8</definedName>
     <definedName function="false" hidden="false" localSheetId="9" name="excel_is_bugging_me" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="9" name="_FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="9" name="_FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0" vbProcedure="false">'Rate laws'!$A$1:$G$6</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0_0" vbProcedure="false">'Rate laws'!$A$1:$G$6</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase" vbProcedure="false">'Rate laws'!$A$1:$G$6</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Rate laws'!$A$1:$G$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Rate laws'!$A$1:$G$6</definedName>
     <definedName function="false" hidden="false" localSheetId="13" name="excel_is_bugging_me" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
     <definedName function="false" hidden="false" localSheetId="13" name="_FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
     <definedName function="false" hidden="false" localSheetId="13" name="_FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
     <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
     <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
     <definedName function="false" hidden="false" localSheetId="15" name="excel_is_bugging_me" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="15" name="_FilterDatabase_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="15" name="_FilterDatabase_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -80,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="173">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -140,9 +147,6 @@
   </si>
   <si>
     <t xml:space="preserve">Algorithm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Biomass reaction</t>
   </si>
   <si>
     <t xml:space="preserve">Objective function</t>
@@ -444,6 +448,9 @@
   </si>
   <si>
     <t xml:space="preserve">k_cat * rna_dec_a[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biomass reaction</t>
   </si>
   <si>
     <t xml:space="preserve">Coefficient</t>
@@ -606,12 +613,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
     <numFmt numFmtId="166" formatCode="0.000E+00"/>
     <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
-    <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -768,7 +774,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -996,19 +1002,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>13</v>
@@ -1019,16 +1025,16 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>98</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>99</v>
       </c>
       <c r="E2" s="11" t="n">
         <v>0</v>
@@ -1040,16 +1046,16 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>102</v>
       </c>
       <c r="E3" s="11" t="n">
         <v>0</v>
@@ -1061,16 +1067,16 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>104</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>105</v>
       </c>
       <c r="E4" s="11" t="n">
         <v>0</v>
@@ -1082,16 +1088,16 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>108</v>
       </c>
       <c r="E5" s="3" t="n">
         <v>0</v>
@@ -1131,19 +1137,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>113</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>13</v>
@@ -1154,13 +1160,13 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B2" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>115</v>
       </c>
       <c r="D2" s="5" t="n">
         <v>0.0003</v>
@@ -1171,13 +1177,13 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="D3" s="5" t="n">
         <v>0.0003</v>
@@ -1188,26 +1194,26 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D4" s="0"/>
       <c r="E4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D5" s="5" t="n">
         <v>2000</v>
@@ -1218,13 +1224,13 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D6" s="5" t="n">
         <v>0.0003</v>
@@ -1249,10 +1255,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1268,18 +1278,12 @@
         <v>2</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>121</v>
+        <v>13</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="0" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1299,10 +1303,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1318,12 +1326,18 @@
         <v>2</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>76</v>
+        <v>120</v>
       </c>
       <c r="D1" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1373,10 +1387,10 @@
         <v>123</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>13</v>
@@ -1442,7 +1456,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>13</v>
@@ -1500,7 +1514,7 @@
         <v>131</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>132</v>
@@ -1648,16 +1662,16 @@
         <v>155</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>156</v>
@@ -1685,7 +1699,7 @@
         <v>159</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G3" s="0"/>
       <c r="H3" s="0"/>
@@ -1698,7 +1712,7 @@
         <v>160</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G4" s="0"/>
       <c r="H4" s="0"/>
@@ -1711,7 +1725,7 @@
         <v>162</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H5" s="0"/>
     </row>
@@ -1723,7 +1737,7 @@
         <v>163</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H6" s="0"/>
     </row>
@@ -1735,7 +1749,7 @@
         <v>165</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1746,7 +1760,7 @@
         <v>166</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1757,7 +1771,7 @@
         <v>167</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1768,7 +1782,7 @@
         <v>168</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1779,7 +1793,7 @@
         <v>169</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1790,7 +1804,7 @@
         <v>170</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1801,7 +1815,7 @@
         <v>172</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1884,20 +1898,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="bottomRight" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="7" min="1" style="3" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="3" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1914,35 +1928,32 @@
         <v>20</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1985,7 +1996,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>13</v>
@@ -1996,30 +2007,30 @@
     </row>
     <row r="2" customFormat="false" ht="252" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="C2" s="5" t="n">
         <v>4.58E-017</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="168" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="C3" s="5" t="n">
         <v>1E-012</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2064,19 +2075,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>13</v>
@@ -2087,16 +2098,16 @@
     </row>
     <row r="2" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="E2" s="3" t="n">
         <v>424.1773</v>
@@ -2105,22 +2116,22 @@
         <v>-3</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="E3" s="3" t="n">
         <v>345.2053</v>
@@ -2129,22 +2140,22 @@
         <v>-2</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="E4" s="3" t="n">
         <v>503.14946</v>
@@ -2153,22 +2164,22 @@
         <v>-4</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="E5" s="3" t="n">
         <v>180.15588</v>
@@ -2177,22 +2188,22 @@
         <v>0</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="E6" s="3" t="n">
         <v>1.00783</v>
@@ -2201,22 +2212,22 @@
         <v>1</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>63</v>
-      </c>
       <c r="D7" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E7" s="3" t="n">
         <v>18.0153</v>
@@ -2225,21 +2236,21 @@
         <v>0</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="E8" s="3" t="n">
         <v>95.9793</v>
@@ -2248,21 +2259,21 @@
         <v>-2</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="E9" s="3" t="n">
         <v>3298.98577</v>
@@ -2271,18 +2282,18 @@
         <v>-11</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="7" t="s">
         <v>73</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -2305,7 +2316,7 @@
   </sheetPr>
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -2315,8 +2326,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2327,10 +2338,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>75</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>76</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>13</v>
@@ -2341,122 +2352,122 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="0" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2493,13 +2504,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>13</v>
@@ -2510,79 +2521,79 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" s="7" t="n">
         <v>0.005</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3" s="7" t="n">
         <v>0.005</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4" s="7" t="n">
         <v>0.005</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5" s="7" t="n">
         <v>0.01</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B6" s="3" t="n">
         <v>1E-007</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B7" s="7" t="n">
         <v>55</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B8" s="5" t="n">
         <v>0.005</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -2622,7 +2633,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>13</v>
@@ -2663,7 +2674,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
updating fixture for updates to wc_lang
</commit_message>
<xml_diff>
--- a/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
+++ b/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13965" tabRatio="993" activeTab="6"/>
+    <workbookView windowWidth="19800" windowHeight="6945" tabRatio="993" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="221">
   <si>
     <t>Id</t>
   </si>
@@ -212,18 +212,27 @@
     <t>Type</t>
   </si>
   <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>Initial volume, distribution</t>
+  </si>
+  <si>
+    <t>Initial volume, mean</t>
+  </si>
+  <si>
+    <t>Initial volume, standard deviation</t>
+  </si>
+  <si>
+    <t>Volume units</t>
+  </si>
+  <si>
     <t>Density</t>
   </si>
   <si>
     <t>Density units</t>
   </si>
   <si>
-    <t>Volume</t>
-  </si>
-  <si>
-    <t>Volume units</t>
-  </si>
-  <si>
     <t>c</t>
   </si>
   <si>
@@ -233,13 +242,19 @@
     <t>physical_3d</t>
   </si>
   <si>
+    <t>mass * density</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>init_mass / init_volume</t>
+  </si>
+  <si>
     <t>g ml^-1</t>
-  </si>
-  <si>
-    <t>mass * density</t>
-  </si>
-  <si>
-    <t>l</t>
   </si>
   <si>
     <t>cco: CCO-CYTOPLASM</t>
@@ -472,9 +487,6 @@
   </si>
   <si>
     <t>dist-init-conc-adp[c]</t>
-  </si>
-  <si>
-    <t>normal</t>
   </si>
   <si>
     <t>M</t>
@@ -754,10 +766,10 @@
   <numFmts count="6">
     <numFmt numFmtId="176" formatCode="0.000E+00"/>
     <numFmt numFmtId="177" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -800,9 +812,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -813,53 +827,20 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
+      <sz val="10"/>
+      <name val="Arial"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -872,16 +853,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -896,7 +869,61 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -911,30 +938,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -955,13 +967,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -973,7 +1009,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -985,13 +1093,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1003,139 +1141,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1175,41 +1187,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -1241,6 +1218,32 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1255,138 +1258,147 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1557,7 +1569,14 @@
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="#REF"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
 </externalLink>
 </file>
 
@@ -1974,22 +1993,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>18</v>
@@ -2006,16 +2025,16 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:9">
       <c r="A2" s="1" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="E2" s="6">
         <v>1</v>
@@ -2026,16 +2045,16 @@
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:9">
       <c r="A3" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="E3" s="6">
         <v>0</v>
@@ -2046,16 +2065,16 @@
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="E4" s="6">
         <v>0</v>
@@ -2065,16 +2084,16 @@
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>34</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="E5" s="1">
         <v>0</v>
@@ -2118,19 +2137,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>38</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
@@ -2147,102 +2166,102 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>157</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:7">
       <c r="A4" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:7">
       <c r="A5" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D5" s="6" t="s">
+      <c r="E5" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>157</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="D6" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>157</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -2281,13 +2300,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>18</v>
@@ -2304,16 +2323,16 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -2352,13 +2371,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>18</v>
@@ -2409,16 +2428,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>18</v>
@@ -2472,13 +2491,13 @@
         <v>38</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>18</v>
@@ -2495,134 +2514,134 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="D2" s="1">
         <v>0.3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D3" s="1">
         <v>0.0003</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D4" s="1">
         <v>0.0003</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:6">
       <c r="A6" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>179</v>
       </c>
       <c r="D6" s="1">
         <v>2000</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D7" s="1">
         <v>0.0003</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" ht="15.1" customHeight="1" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="D8" s="1">
         <v>0.001</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" ht="15.1" customHeight="1" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="D9" s="1">
         <v>0.001</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" ht="15.1" customHeight="1" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="D10" s="1">
         <v>0.01</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -2661,10 +2680,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>18</v>
@@ -2715,28 +2734,28 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>38</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>18</v>
@@ -2787,46 +2806,46 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>38</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>18</v>
@@ -2837,66 +2856,66 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:16">
       <c r="A2" s="1" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="F2" s="1">
         <v>2016</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="K2" s="1">
         <v>44</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:16">
       <c r="A3" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="F3" s="1">
         <v>2017</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="K3" s="1">
         <v>45</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -3056,22 +3075,22 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E36" sqref="E36"/>
+      <selection pane="bottomRight" activeCell="D1" sqref="D1:J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1025" width="8.78333333333333" style="1"/>
+    <col min="1" max="1028" width="8.78333333333333" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:11">
+    <row r="1" ht="15.1" customHeight="1" spans="1:14">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -3094,74 +3113,101 @@
         <v>42</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:10">
+    <row r="2" ht="15.1" customHeight="1" spans="1:13">
       <c r="A2" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" s="1">
-        <v>1.09</v>
+        <v>48</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="10">
+        <v>4.58e-17</v>
+      </c>
+      <c r="G2" s="1">
+        <v>4.58e-18</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" ht="15.1" customHeight="1" spans="1:13">
+      <c r="A3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" ht="15.1" customHeight="1" spans="1:10">
-      <c r="A3" s="1" t="s">
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0.99318</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>54</v>
+      <c r="K3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -3202,16 +3248,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>38</v>
@@ -3231,16 +3277,16 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="E2" s="1">
         <v>424.1773</v>
@@ -3249,25 +3295,25 @@
         <v>-3</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="J2" s="9"/>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E3" s="1">
         <v>345.2053</v>
@@ -3276,25 +3322,25 @@
         <v>-2</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="J3" s="9"/>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="E4" s="1">
         <v>503.14946</v>
@@ -3303,25 +3349,25 @@
         <v>-4</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="J4" s="9"/>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E5" s="1">
         <v>180.15588</v>
@@ -3330,22 +3376,22 @@
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="J5" s="9"/>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:10">
       <c r="A6" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="E6" s="1">
         <v>1.00783</v>
@@ -3354,25 +3400,25 @@
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="J6" s="9"/>
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="E7" s="1">
         <v>18.0153</v>
@@ -3381,24 +3427,24 @@
         <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" ht="15.1" customHeight="1" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="E8" s="1">
         <v>95.9793</v>
@@ -3407,24 +3453,24 @@
         <v>-2</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" ht="15.1" customHeight="1" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E9" s="1">
         <v>174.95</v>
@@ -3433,21 +3479,21 @@
         <v>-4</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" ht="15.1" customHeight="1" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="E10" s="1">
         <v>3298.98577</v>
@@ -3456,21 +3502,21 @@
         <v>-11</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" ht="15.1" customHeight="1" spans="1:9">
       <c r="A11" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="E11" s="1">
         <v>1042.32919</v>
@@ -3479,7 +3525,7 @@
         <v>-8</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
@@ -3521,13 +3567,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>18</v>
@@ -3544,152 +3590,152 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="1" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="1" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" ht="15.1" customHeight="1" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" ht="15.1" customHeight="1" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" ht="15.1" customHeight="1" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="1" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" ht="15.1" customHeight="1" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="1" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -3707,7 +3753,7 @@
   <sheetPr/>
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
@@ -3729,19 +3775,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
@@ -3758,13 +3804,13 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>126</v>
+        <v>50</v>
       </c>
       <c r="E2" s="9">
         <v>0.005</v>
@@ -3773,125 +3819,125 @@
         <v>0.0121655250605964</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:9">
       <c r="A3" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>126</v>
+        <v>50</v>
       </c>
       <c r="E3" s="9">
         <v>0.005</v>
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="9" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:9">
       <c r="A4" s="1" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>126</v>
+        <v>50</v>
       </c>
       <c r="E4" s="9">
         <v>0.005</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="9" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:9">
       <c r="A5" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>126</v>
+        <v>50</v>
       </c>
       <c r="E5" s="9">
         <v>0.01</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="9" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:9">
       <c r="A6" s="1" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>126</v>
+        <v>50</v>
       </c>
       <c r="E6" s="1">
         <v>1e-7</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="9" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:9">
       <c r="A7" s="1" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>126</v>
+        <v>50</v>
       </c>
       <c r="E7" s="9">
         <v>55</v>
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="9" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
     </row>
     <row r="8" ht="15.1" customHeight="1" spans="1:9">
       <c r="A8" s="1" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>126</v>
+        <v>50</v>
       </c>
       <c r="E8" s="10">
         <v>0.005</v>
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="9" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
@@ -3932,10 +3978,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>18</v>
@@ -3986,10 +4032,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
updating for changes to wc_lang compartments
</commit_message>
<xml_diff>
--- a/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
+++ b/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="19800" windowHeight="6945" tabRatio="993" activeTab="3"/>
+    <workbookView windowWidth="28200" windowHeight="14070" tabRatio="993" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <externalReference r:id="rId19"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Compartments!$A$1:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Compartments!$A$1:$G$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Species types'!$A$1:$K$11</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Initial species concentrations'!$C$1:$K$8</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Reactions!$A$1:$D$5</definedName>
@@ -40,13 +40,13 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">References!$A$1:$D$3</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="2">Submodels!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2">Submodels!$A$1:$G$3</definedName>
-    <definedName name="excel_is_bugging_me" localSheetId="3">Compartments!$A$1:$D$3</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="3">Compartments!$A$1:$D$3</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="3">Compartments!$A$1:$D$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="3">Compartments!$A$1:$D$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="3">Compartments!$A$1:$D$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$D$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$D$3</definedName>
+    <definedName name="excel_is_bugging_me" localSheetId="3">Compartments!$A$1:$G$3</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="3">Compartments!$A$1:$G$3</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="3">Compartments!$A$1:$G$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="3">Compartments!$A$1:$G$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="3">Compartments!$A$1:$G$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$G$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$G$3</definedName>
     <definedName name="excel_is_bugging_me" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="228">
   <si>
     <t>Id</t>
   </si>
@@ -209,82 +209,103 @@
     <t>go: GO:0006401</t>
   </si>
   <si>
+    <t>Biological type</t>
+  </si>
+  <si>
+    <t>Physical type</t>
+  </si>
+  <si>
+    <t>Geometry</t>
+  </si>
+  <si>
+    <t>Parent compartment</t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>Initial volume, distribution</t>
+  </si>
+  <si>
+    <t>Initial volume, mean</t>
+  </si>
+  <si>
+    <t>Initial volume, standard deviation</t>
+  </si>
+  <si>
+    <t>Volume units</t>
+  </si>
+  <si>
+    <t>Density</t>
+  </si>
+  <si>
+    <t>Density units</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>Cell</t>
+  </si>
+  <si>
+    <t>cellular</t>
+  </si>
+  <si>
+    <t>fluid</t>
+  </si>
+  <si>
+    <t>3d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>mass * density</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>init_mass / init_volume</t>
+  </si>
+  <si>
+    <t>g ml^-1</t>
+  </si>
+  <si>
+    <t>cco: CCO-CYTOPLASM</t>
+  </si>
+  <si>
+    <t>Average volume of Mycoplasma pneumoniae is 66 aL [Ref-0001]. This equates to 45.8 aL at the beginning of the cell cycle (66 aL * ln(2)).</t>
+  </si>
+  <si>
+    <t>Extracellular space</t>
+  </si>
+  <si>
+    <t>extracellular</t>
+  </si>
+  <si>
+    <t>cco: CCO-EXTRACELLULAR</t>
+  </si>
+  <si>
+    <t>Typical density of Mycoplasma pneumoniae cells in culture is 1e-9 cells/mL [Ref-0002].</t>
+  </si>
+  <si>
+    <t>Structure</t>
+  </si>
+  <si>
+    <t>Empirical formula</t>
+  </si>
+  <si>
+    <t>Molecular weight</t>
+  </si>
+  <si>
+    <t>Charge</t>
+  </si>
+  <si>
     <t>Type</t>
-  </si>
-  <si>
-    <t>Volume</t>
-  </si>
-  <si>
-    <t>Initial volume, distribution</t>
-  </si>
-  <si>
-    <t>Initial volume, mean</t>
-  </si>
-  <si>
-    <t>Initial volume, standard deviation</t>
-  </si>
-  <si>
-    <t>Volume units</t>
-  </si>
-  <si>
-    <t>Density</t>
-  </si>
-  <si>
-    <t>Density units</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>Cell</t>
-  </si>
-  <si>
-    <t>physical_3d</t>
-  </si>
-  <si>
-    <t>mass * density</t>
-  </si>
-  <si>
-    <t>normal</t>
-  </si>
-  <si>
-    <t>l</t>
-  </si>
-  <si>
-    <t>init_mass / init_volume</t>
-  </si>
-  <si>
-    <t>g ml^-1</t>
-  </si>
-  <si>
-    <t>cco: CCO-CYTOPLASM</t>
-  </si>
-  <si>
-    <t>Average volume of Mycoplasma pneumoniae is 66 aL [Ref-0001]. This equates to 45.8 aL at the beginning of the cell cycle (66 aL * ln(2)).</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>Extracellular space</t>
-  </si>
-  <si>
-    <t>cco: CCO-EXTRACELLULAR</t>
-  </si>
-  <si>
-    <t>Typical density of Mycoplasma pneumoniae cells in culture is 1e-9 cells/mL [Ref-0002].</t>
-  </si>
-  <si>
-    <t>Structure</t>
-  </si>
-  <si>
-    <t>Empirical formula</t>
-  </si>
-  <si>
-    <t>Molecular weight</t>
-  </si>
-  <si>
-    <t>Charge</t>
   </si>
   <si>
     <t>adp</t>
@@ -764,12 +785,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="0.000E+00"/>
     <numFmt numFmtId="177" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -812,11 +833,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -827,27 +846,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -861,7 +870,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -869,53 +885,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -930,10 +899,18 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -945,10 +922,54 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -967,19 +988,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -991,37 +1048,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1033,19 +1066,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1057,7 +1078,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1075,25 +1096,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1117,19 +1132,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1141,7 +1150,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1188,17 +1209,34 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1220,26 +1258,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1262,143 +1283,143 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1993,22 +2014,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>18</v>
@@ -2025,16 +2046,16 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:9">
       <c r="A2" s="1" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="E2" s="6">
         <v>1</v>
@@ -2045,16 +2066,16 @@
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:9">
       <c r="A3" s="1" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="E3" s="6">
         <v>0</v>
@@ -2065,16 +2086,16 @@
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="E4" s="6">
         <v>0</v>
@@ -2084,16 +2105,16 @@
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>34</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="E5" s="1">
         <v>0</v>
@@ -2137,19 +2158,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
@@ -2166,102 +2187,102 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -2300,13 +2321,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>18</v>
@@ -2323,16 +2344,16 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -2371,13 +2392,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>18</v>
@@ -2428,16 +2449,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>18</v>
@@ -2488,16 +2509,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>18</v>
@@ -2514,134 +2535,134 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="D2" s="1">
         <v>0.3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="D3" s="1">
         <v>0.0003</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="D4" s="1">
         <v>0.0003</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="D6" s="1">
         <v>2000</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="D7" s="1">
         <v>0.0003</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" ht="15.1" customHeight="1" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="D8" s="1">
         <v>0.001</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" ht="15.1" customHeight="1" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="D9" s="1">
         <v>0.001</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" ht="15.1" customHeight="1" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="D10" s="1">
         <v>0.01</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -2680,10 +2701,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>18</v>
@@ -2734,28 +2755,28 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>18</v>
@@ -2806,46 +2827,46 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>18</v>
@@ -2856,66 +2877,66 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:16">
       <c r="A2" s="1" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="F2" s="1">
         <v>2016</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="K2" s="1">
         <v>44</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:16">
       <c r="A3" s="1" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="F3" s="1">
         <v>2017</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="K3" s="1">
         <v>45</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -3075,29 +3096,29 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D1" sqref="D1:J3"/>
+      <selection pane="bottomRight" activeCell="F1" sqref="F$1:F$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1028" width="8.78333333333333" style="1"/>
+    <col min="1" max="1031" width="8.78333333333333" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:14">
+    <row r="1" ht="15.1" customHeight="1" spans="1:17">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -3122,96 +3143,120 @@
         <v>45</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:13">
+    <row r="2" ht="15.1" customHeight="1" spans="1:16">
       <c r="A2" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F2" s="10">
+        <v>53</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" s="10">
         <v>4.58e-17</v>
       </c>
-      <c r="G2" s="1">
+      <c r="J2" s="1">
         <v>4.58e-18</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="K2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" ht="15.1" customHeight="1" spans="1:16">
+      <c r="A3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="M2" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="3" ht="15.1" customHeight="1" spans="1:13">
-      <c r="A3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" s="1">
-        <v>1</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>58</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>59</v>
       </c>
+      <c r="N3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D3">
+  <autoFilter ref="A1:G3">
     <extLst/>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3248,19 +3293,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
@@ -3277,16 +3322,16 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="E2" s="1">
         <v>424.1773</v>
@@ -3295,25 +3340,25 @@
         <v>-3</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="J2" s="9"/>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="E3" s="1">
         <v>345.2053</v>
@@ -3322,25 +3367,25 @@
         <v>-2</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="J3" s="9"/>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="E4" s="1">
         <v>503.14946</v>
@@ -3349,25 +3394,25 @@
         <v>-4</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="J4" s="9"/>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="E5" s="1">
         <v>180.15588</v>
@@ -3376,22 +3421,22 @@
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="J5" s="9"/>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:10">
       <c r="A6" s="1" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="E6" s="1">
         <v>1.00783</v>
@@ -3400,25 +3445,25 @@
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="J6" s="9"/>
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="E7" s="1">
         <v>18.0153</v>
@@ -3427,24 +3472,24 @@
         <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" ht="15.1" customHeight="1" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="E8" s="1">
         <v>95.9793</v>
@@ -3453,24 +3498,24 @@
         <v>-2</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" ht="15.1" customHeight="1" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E9" s="1">
         <v>174.95</v>
@@ -3479,21 +3524,21 @@
         <v>-4</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" ht="15.1" customHeight="1" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="E10" s="1">
         <v>3298.98577</v>
@@ -3502,21 +3547,21 @@
         <v>-11</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" ht="15.1" customHeight="1" spans="1:9">
       <c r="A11" s="1" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E11" s="1">
         <v>1042.32919</v>
@@ -3525,7 +3570,7 @@
         <v>-8</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
@@ -3567,13 +3612,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>18</v>
@@ -3590,152 +3635,152 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="1" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="1" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="1" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="1" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="1" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="1" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" ht="15.1" customHeight="1" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="1" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" ht="15.1" customHeight="1" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="1" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" ht="15.1" customHeight="1" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="1" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" ht="15.1" customHeight="1" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="1" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -3775,19 +3820,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
@@ -3804,13 +3849,13 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="E2" s="9">
         <v>0.005</v>
@@ -3819,125 +3864,125 @@
         <v>0.0121655250605964</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:9">
       <c r="A3" s="1" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="E3" s="9">
         <v>0.005</v>
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="9" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:9">
       <c r="A4" s="1" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="E4" s="9">
         <v>0.005</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="9" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:9">
       <c r="A5" s="1" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="E5" s="9">
         <v>0.01</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="9" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:9">
       <c r="A6" s="1" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="E6" s="1">
         <v>1e-7</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="9" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:9">
       <c r="A7" s="1" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="E7" s="9">
         <v>55</v>
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="9" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
     </row>
     <row r="8" ht="15.1" customHeight="1" spans="1:9">
       <c r="A8" s="1" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="E8" s="10">
         <v>0.005</v>
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="9" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
@@ -3978,10 +4023,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>18</v>
@@ -4032,10 +4077,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
updating for changing reaction rate units in wc_lang
</commit_message>
<xml_diff>
--- a/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
+++ b/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28200" windowHeight="14070" tabRatio="993" activeTab="3"/>
+    <workbookView windowWidth="28200" windowHeight="13965" tabRatio="993" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="230">
   <si>
     <t>Id</t>
   </si>
@@ -549,7 +549,7 @@
     <t>Flux max</t>
   </si>
   <si>
-    <t>Flux units</t>
+    <t>Flux bound units</t>
   </si>
   <si>
     <t>atp_hydrolysis</t>
@@ -634,6 +634,12 @@
   </si>
   <si>
     <t>k_cat_rna_deg_for * rna_dec_a[c]</t>
+  </si>
+  <si>
+    <t>Reaction rate units</t>
+  </si>
+  <si>
+    <t>Coefficient units</t>
   </si>
   <si>
     <t>dfba-obj-metabolism</t>
@@ -785,12 +791,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="0.000E+00"/>
     <numFmt numFmtId="177" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -838,46 +844,16 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -892,6 +868,29 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -899,10 +898,17 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -915,15 +921,28 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -937,37 +956,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -988,7 +994,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1000,7 +1012,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1012,7 +1024,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1024,7 +1102,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1036,19 +1114,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1060,49 +1156,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1114,55 +1168,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1191,6 +1197,39 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1206,11 +1245,28 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1232,56 +1288,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -1291,132 +1297,132 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1994,7 +2000,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4"/>
@@ -2298,22 +2304,25 @@
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1025" width="9.10833333333333" style="1"/>
+    <col min="1" max="1" width="17" style="1" customWidth="1"/>
+    <col min="2" max="4" width="9.10833333333333" style="1"/>
+    <col min="5" max="6" width="12.25" style="1" customWidth="1"/>
+    <col min="7" max="1027" width="9.10833333333333" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:9">
+    <row r="1" ht="15.1" customHeight="1" spans="1:11">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2330,21 +2339,27 @@
         <v>121</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:5">
+    <row r="2" ht="15.1" customHeight="1" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>30</v>
@@ -2353,7 +2368,13 @@
         <v>155</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>181</v>
+        <v>183</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -2398,7 +2419,7 @@
         <v>121</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>18</v>
@@ -2449,13 +2470,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>133</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>121</v>
@@ -2512,10 +2533,10 @@
         <v>70</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>121</v>
@@ -2535,10 +2556,10 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>168</v>
@@ -2547,18 +2568,18 @@
         <v>0.3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D3" s="1">
         <v>0.0003</v>
@@ -2569,10 +2590,10 @@
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D4" s="1">
         <v>0.0003</v>
@@ -2583,24 +2604,24 @@
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:6">
       <c r="A5" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>190</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D6" s="1">
         <v>2000</v>
@@ -2611,24 +2632,24 @@
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D7" s="1">
         <v>0.0003</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" ht="15.1" customHeight="1" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D8" s="1">
         <v>0.001</v>
@@ -2639,10 +2660,10 @@
     </row>
     <row r="9" ht="15.1" customHeight="1" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D9" s="1">
         <v>0.001</v>
@@ -2653,10 +2674,10 @@
     </row>
     <row r="10" ht="15.1" customHeight="1" spans="1:6">
       <c r="A10" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="D10" s="1">
         <v>0.01</v>
@@ -2755,7 +2776,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>121</v>
@@ -2764,19 +2785,19 @@
         <v>70</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>18</v>
@@ -2827,46 +2848,46 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>70</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>42</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>18</v>
@@ -2877,66 +2898,66 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:16">
       <c r="A2" s="1" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="F2" s="1">
         <v>2016</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="K2" s="1">
         <v>44</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:16">
       <c r="A3" s="1" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="F3" s="1">
         <v>2017</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="K3" s="1">
         <v>45</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -3098,7 +3119,7 @@
   <sheetPr/>
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>

</xml_diff>

<commit_message>
updating for changes to wc_lang compartment mass, density, and volume
</commit_message>
<xml_diff>
--- a/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
+++ b/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28200" windowHeight="13965" tabRatio="993" activeTab="11"/>
+    <workbookView windowWidth="28200" windowHeight="13965" tabRatio="993" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="237">
   <si>
     <t>Id</t>
   </si>
@@ -221,25 +221,22 @@
     <t>Parent compartment</t>
   </si>
   <si>
-    <t>Volume</t>
-  </si>
-  <si>
-    <t>Initial volume, distribution</t>
-  </si>
-  <si>
-    <t>Initial volume, mean</t>
-  </si>
-  <si>
-    <t>Initial volume, standard deviation</t>
-  </si>
-  <si>
-    <t>Volume units</t>
-  </si>
-  <si>
-    <t>Density</t>
-  </si>
-  <si>
-    <t>Density units</t>
+    <t>Mass units</t>
+  </si>
+  <si>
+    <t>Initial volume distribution</t>
+  </si>
+  <si>
+    <t>Initial volume mean</t>
+  </si>
+  <si>
+    <t>Initial volume standard deviation</t>
+  </si>
+  <si>
+    <t>Initial volume units</t>
+  </si>
+  <si>
+    <t>Initial density</t>
   </si>
   <si>
     <t>c</t>
@@ -260,7 +257,7 @@
     <t>e</t>
   </si>
   <si>
-    <t>mass * density</t>
+    <t>g</t>
   </si>
   <si>
     <t>normal</t>
@@ -269,10 +266,7 @@
     <t>l</t>
   </si>
   <si>
-    <t>init_mass / init_volume</t>
-  </si>
-  <si>
-    <t>g ml^-1</t>
+    <t>density_c</t>
   </si>
   <si>
     <t>cco: CCO-CYTOPLASM</t>
@@ -285,6 +279,9 @@
   </si>
   <si>
     <t>extracellular</t>
+  </si>
+  <si>
+    <t>density_e</t>
   </si>
   <si>
     <t>cco: CCO-EXTRACELLULAR</t>
@@ -534,6 +531,18 @@
     <t>Expression</t>
   </si>
   <si>
+    <t>volume_c</t>
+  </si>
+  <si>
+    <t>c / density_c</t>
+  </si>
+  <si>
+    <t>volume_e</t>
+  </si>
+  <si>
+    <t>e / density_e</t>
+  </si>
+  <si>
     <t>Submodel</t>
   </si>
   <si>
@@ -603,7 +612,7 @@
     <t>other</t>
   </si>
   <si>
-    <t>k_cat_atp_hyd_rev * atp[c] / (atp[c] + K_m_atp_hyd_rev)</t>
+    <t>k_cat_atp_hyd_rev * atp[c] / (atp[c] + K_m_atp_hyd_rev * Avogadro * volume_c)</t>
   </si>
   <si>
     <t>s^-1</t>
@@ -615,7 +624,7 @@
     <t>forward</t>
   </si>
   <si>
-    <t>k_cat_atp_hyd_rev * adp[c] / (adp[c] + K_m_atp_hyd_for)</t>
+    <t>k_cat_atp_hyd_rev * adp[c] / (adp[c] + K_m_atp_hyd_for * Avogadro * volume_c)</t>
   </si>
   <si>
     <t>biomass_production-forward</t>
@@ -627,7 +636,7 @@
     <t>glc_import-forward</t>
   </si>
   <si>
-    <t>k_cat_glc_import_for * glc[e] / (glc[e] + K_m_glc_import_for)</t>
+    <t>k_cat_glc_import_for * glc[e] / (glc[e] + K_m_glc_import_for * Avogadro * volume_c)</t>
   </si>
   <si>
     <t>rna_degradation_dec_a-forward</t>
@@ -702,6 +711,15 @@
     <t>K_m_glc_import_for</t>
   </si>
   <si>
+    <t>g l^-1</t>
+  </si>
+  <si>
+    <t>Avogadro</t>
+  </si>
+  <si>
+    <t>molecule mol^-1</t>
+  </si>
+  <si>
     <t>Taxon</t>
   </si>
   <si>
@@ -733,6 +751,9 @@
   </si>
   <si>
     <t>Series</t>
+  </si>
+  <si>
+    <t>Volume</t>
   </si>
   <si>
     <t>Number</t>
@@ -791,11 +812,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="0.000E+00"/>
-    <numFmt numFmtId="177" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="176" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="0.000E+00"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="25">
@@ -831,9 +852,23 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -844,16 +879,17 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -868,17 +904,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -891,24 +927,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -927,24 +956,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -956,24 +972,29 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -994,7 +1015,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1006,13 +1033,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1024,25 +1087,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1054,127 +1195,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1197,17 +1218,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1224,8 +1239,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1246,16 +1276,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1272,161 +1302,152 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1441,6 +1462,9 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="35" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1453,13 +1477,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2020,22 +2041,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>18</v>
@@ -2052,75 +2073,75 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:9">
       <c r="A2" s="1" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="E2" s="6">
+      <c r="D2" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E2" s="7">
         <v>1</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="I2" s="8"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="I2" s="9"/>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:9">
       <c r="A3" s="1" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E3" s="6">
+        <v>160</v>
+      </c>
+      <c r="E3" s="7">
         <v>0</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="I3" s="8"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="I3" s="9"/>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="E4" s="6">
+      <c r="D4" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="E4" s="7">
         <v>0</v>
       </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>34</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="E5" s="1">
         <v>0</v>
@@ -2152,7 +2173,7 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5"/>
   <cols>
     <col min="1" max="5" width="8.78333333333333" style="1"/>
-    <col min="6" max="6" width="44.775" style="1"/>
+    <col min="6" max="6" width="68.5" style="1" customWidth="1"/>
     <col min="7" max="1025" width="8.78333333333333" style="1"/>
   </cols>
   <sheetData>
@@ -2164,19 +2185,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
@@ -2193,102 +2214,102 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>168</v>
+        <v>155</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>171</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:7">
       <c r="A3" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>168</v>
-      </c>
       <c r="F3" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>168</v>
+        <v>158</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>171</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>168</v>
+        <v>161</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>171</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>168</v>
+        <v>164</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>171</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -2306,7 +2327,7 @@
   <sheetPr/>
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
@@ -2330,19 +2351,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
@@ -2359,19 +2380,19 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>155</v>
+      <c r="D2" s="6" t="s">
+        <v>158</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>17</v>
@@ -2413,13 +2434,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>18</v>
@@ -2463,34 +2484,34 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.1" customHeight="1" spans="1:10">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="G1" s="4" t="s">
+      <c r="C1" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>18</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="5" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2507,22 +2528,22 @@
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="O33" sqref="O33"/>
+      <selection pane="bottomRight" activeCell="F8" sqref="F8:F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1025" width="8.78333333333333" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:10">
+    <row r="1" customHeight="1" spans="1:10">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2530,16 +2551,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>18</v>
@@ -2554,136 +2575,178 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:10">
+    <row r="2" customHeight="1" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="D2" s="1">
         <v>0.3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="3" ht="15.1" customHeight="1" spans="1:6">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="3" customHeight="1" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="D3" s="1">
         <v>0.0003</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="4" ht="15.1" customHeight="1" spans="1:6">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" customHeight="1" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="D4" s="1">
         <v>0.0003</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="5" ht="15.1" customHeight="1" spans="1:6">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" customHeight="1" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="6" customHeight="1" spans="1:6">
+      <c r="A6" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>195</v>
-      </c>
-    </row>
-    <row r="6" ht="15.1" customHeight="1" spans="1:6">
-      <c r="A6" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>192</v>
       </c>
       <c r="D6" s="1">
         <v>2000</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="7" ht="15.1" customHeight="1" spans="1:6">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" customHeight="1" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="D7" s="1">
         <v>0.0003</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="8" ht="15.1" customHeight="1" spans="1:6">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="8" customHeight="1" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D8" s="1">
         <v>0.001</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="9" ht="15.1" customHeight="1" spans="1:6">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" customHeight="1" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D9" s="1">
         <v>0.001</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" ht="15.1" customHeight="1" spans="1:6">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" customHeight="1" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D10" s="1">
         <v>0.01</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>123</v>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="11" customHeight="1" spans="1:6">
+      <c r="A11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1100</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="12" customHeight="1" spans="1:6">
+      <c r="A12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="13" customHeight="1" spans="1:6">
+      <c r="A13" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D13" s="4">
+        <v>6.02214075862e+23</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -2722,10 +2785,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>18</v>
@@ -2776,28 +2839,28 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>18</v>
@@ -2848,46 +2911,46 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>42</v>
+        <v>219</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>18</v>
@@ -2898,66 +2961,66 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:16">
       <c r="A2" s="1" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="F2" s="1">
         <v>2016</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="K2" s="1">
         <v>44</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:16">
       <c r="A3" s="1" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="F3" s="1">
         <v>2017</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="K3" s="1">
         <v>45</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -3117,22 +3180,22 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F1" sqref="F$1:F$1048576"/>
+      <selection pane="bottomRight" activeCell="L2" sqref="L2:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1031" width="8.78333333333333" style="1"/>
+    <col min="1" max="1030" width="8.78333333333333" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:17">
+    <row r="1" ht="15.1" customHeight="1" spans="1:16">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -3170,89 +3233,83 @@
         <v>47</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" ht="15.1" customHeight="1" spans="1:15">
+      <c r="A2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:16">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I2" s="10">
+      <c r="I2" s="4">
         <v>4.58e-17</v>
       </c>
       <c r="J2" s="1">
         <v>4.58e-18</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="N2" s="1" t="s">
+    </row>
+    <row r="3" ht="15.1" customHeight="1" spans="1:15">
+      <c r="A3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="3" ht="15.1" customHeight="1" spans="1:16">
-      <c r="A3" s="1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="I3" s="1">
         <v>1</v>
@@ -3261,19 +3318,16 @@
         <v>0</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="N3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="O3" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -3314,19 +3368,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
@@ -3343,16 +3397,16 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:10">
       <c r="A2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="E2" s="1">
         <v>424.1773</v>
@@ -3361,25 +3415,25 @@
         <v>-3</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="J2" s="9"/>
+      <c r="J2" s="10"/>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:10">
       <c r="A3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="E3" s="1">
         <v>345.2053</v>
@@ -3388,25 +3442,25 @@
         <v>-2</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="J3" s="9"/>
+        <v>80</v>
+      </c>
+      <c r="J3" s="10"/>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:10">
       <c r="A4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="E4" s="1">
         <v>503.14946</v>
@@ -3415,25 +3469,25 @@
         <v>-4</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="J4" s="9"/>
+        <v>85</v>
+      </c>
+      <c r="J4" s="10"/>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:10">
       <c r="A5" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="E5" s="1">
         <v>180.15588</v>
@@ -3442,22 +3496,22 @@
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="J5" s="9"/>
+        <v>74</v>
+      </c>
+      <c r="J5" s="10"/>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:10">
       <c r="A6" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="E6" s="1">
         <v>1.00783</v>
@@ -3466,25 +3520,25 @@
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="J6" s="9"/>
+        <v>94</v>
+      </c>
+      <c r="J6" s="10"/>
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:8">
       <c r="A7" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="E7" s="1">
         <v>18.0153</v>
@@ -3493,24 +3547,24 @@
         <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" ht="15.1" customHeight="1" spans="1:8">
       <c r="A8" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="E8" s="1">
         <v>95.9793</v>
@@ -3519,24 +3573,24 @@
         <v>-2</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" ht="15.1" customHeight="1" spans="1:7">
       <c r="A9" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="E9" s="1">
         <v>174.95</v>
@@ -3545,21 +3599,21 @@
         <v>-4</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" ht="15.1" customHeight="1" spans="1:8">
       <c r="A10" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="E10" s="1">
         <v>3298.98577</v>
@@ -3568,21 +3622,21 @@
         <v>-11</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="11" ht="15.1" customHeight="1" spans="1:9">
       <c r="A11" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="E11" s="1">
         <v>1042.32919</v>
@@ -3590,11 +3644,11 @@
       <c r="F11" s="1">
         <v>-8</v>
       </c>
-      <c r="G11" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
+      <c r="G11" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:K11">
@@ -3633,13 +3687,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>18</v>
@@ -3656,152 +3710,152 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:5">
       <c r="A2" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B3" s="8"/>
+        <v>123</v>
+      </c>
+      <c r="B3" s="9"/>
       <c r="C3" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B4" s="8"/>
+        <v>124</v>
+      </c>
+      <c r="B4" s="9"/>
       <c r="C4" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B5" s="8"/>
+        <v>125</v>
+      </c>
+      <c r="B5" s="9"/>
       <c r="C5" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B6" s="8"/>
+        <v>126</v>
+      </c>
+      <c r="B6" s="9"/>
       <c r="C6" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B7" s="8"/>
+        <v>127</v>
+      </c>
+      <c r="B7" s="9"/>
       <c r="C7" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" ht="15.1" customHeight="1" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B8" s="8"/>
+        <v>128</v>
+      </c>
+      <c r="B8" s="9"/>
       <c r="C8" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" ht="15.1" customHeight="1" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B9" s="8"/>
+        <v>129</v>
+      </c>
+      <c r="B9" s="9"/>
       <c r="C9" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" ht="15.1" customHeight="1" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B10" s="8"/>
+        <v>130</v>
+      </c>
+      <c r="B10" s="9"/>
       <c r="C10" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" ht="15.1" customHeight="1" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B11" s="8"/>
+        <v>131</v>
+      </c>
+      <c r="B11" s="9"/>
       <c r="C11" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -3841,19 +3895,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>136</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
@@ -3870,143 +3924,143 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E2" s="9">
+        <v>55</v>
+      </c>
+      <c r="E2" s="10">
         <v>0.005</v>
       </c>
       <c r="F2" s="1">
         <v>0.0121655250605964</v>
       </c>
-      <c r="G2" s="9" t="s">
-        <v>138</v>
+      <c r="G2" s="10" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:9">
       <c r="A3" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E3" s="9">
+        <v>55</v>
+      </c>
+      <c r="E3" s="10">
         <v>0.005</v>
       </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:9">
       <c r="A4" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" s="9">
+        <v>55</v>
+      </c>
+      <c r="E4" s="10">
         <v>0.005</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:9">
       <c r="A5" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E5" s="9">
+        <v>55</v>
+      </c>
+      <c r="E5" s="10">
         <v>0.01</v>
       </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:9">
       <c r="A6" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E6" s="1">
         <v>1e-7</v>
       </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:9">
       <c r="A7" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E7" s="9">
         <v>55</v>
       </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
+      <c r="E7" s="10">
+        <v>55</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
     </row>
     <row r="8" ht="15.1" customHeight="1" spans="1:9">
       <c r="A8" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E8" s="10">
+        <v>55</v>
+      </c>
+      <c r="E8" s="4">
         <v>0.005</v>
       </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
     </row>
   </sheetData>
   <autoFilter ref="C1:K8">
@@ -4044,10 +4098,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>18</v>
@@ -4075,22 +4129,24 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K35" sqref="K35"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1025" width="8.78333333333333" style="1"/>
+    <col min="1" max="2" width="8.78333333333333" style="1"/>
+    <col min="3" max="3" width="11" style="1" customWidth="1"/>
+    <col min="4" max="1025" width="8.78333333333333" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:8">
+    <row r="1" customHeight="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4098,10 +4154,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>18</v>
@@ -4114,6 +4170,28 @@
       </c>
       <c r="H1" s="2" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="2" customHeight="1" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" customHeight="1" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating for refactoring of expressions to obj_model
</commit_message>
<xml_diff>
--- a/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
+++ b/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28200" windowHeight="13965" tabRatio="993" activeTab="14"/>
+    <workbookView windowWidth="19800" windowHeight="6840" tabRatio="993" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Initial species concentrations'!$C$1:$K$8</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Reactions!$A$1:$D$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'Rate laws'!$C$1:$H$6</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">Parameters!$A$1:$F$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">Parameters!$A$1:$F$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">References!$A$1:$D$3</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="2">Submodels!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2">Submodels!$A$1:$G$3</definedName>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="238">
   <si>
     <t>Id</t>
   </si>
@@ -552,6 +552,9 @@
     <t>Reversible</t>
   </si>
   <si>
+    <t>Rate units</t>
+  </si>
+  <si>
     <t>Flux min</t>
   </si>
   <si>
@@ -570,6 +573,9 @@
     <t>[c]: atp + h2o ==&gt; adp + pi + h</t>
   </si>
   <si>
+    <t>s^-1</t>
+  </si>
+  <si>
     <t>biomass_production</t>
   </si>
   <si>
@@ -613,9 +619,6 @@
   </si>
   <si>
     <t>k_cat_atp_hyd_rev * atp[c] / (atp[c] + K_m_atp_hyd_rev * Avogadro * volume_c)</t>
-  </si>
-  <si>
-    <t>s^-1</t>
   </si>
   <si>
     <t>atp_hydrolysis-forward</t>
@@ -812,12 +815,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="176" formatCode="0.000E+00"/>
+    <numFmt numFmtId="177" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="0.000E+00"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -852,23 +855,24 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -887,16 +891,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -904,7 +907,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -920,9 +930,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -930,6 +940,13 @@
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -943,7 +960,29 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -957,44 +996,8 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1015,7 +1018,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1027,7 +1072,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1039,49 +1084,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1093,43 +1096,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1147,25 +1150,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1177,13 +1168,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1195,7 +1186,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1227,24 +1230,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1256,6 +1241,36 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1275,17 +1290,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1301,153 +1310,147 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1477,10 +1480,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2014,14 +2017,14 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomRight" activeCell="F2" sqref="F2:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4"/>
@@ -2030,10 +2033,10 @@
     <col min="2" max="2" width="18.2916666666667" style="1"/>
     <col min="3" max="3" width="13.3416666666667" style="1"/>
     <col min="4" max="4" width="40.575" style="1"/>
-    <col min="5" max="1025" width="8.78333333333333" style="1"/>
+    <col min="5" max="1026" width="8.78333333333333" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:12">
+    <row r="1" ht="15.1" customHeight="1" spans="1:13">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2059,92 +2062,107 @@
         <v>154</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:9">
+    <row r="2" ht="15.1" customHeight="1" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E2" s="7">
         <v>1</v>
       </c>
-      <c r="F2" s="7"/>
+      <c r="F2" s="7" t="s">
+        <v>159</v>
+      </c>
       <c r="G2" s="7"/>
-      <c r="I2" s="9"/>
-    </row>
-    <row r="3" ht="15.1" customHeight="1" spans="1:9">
+      <c r="H2" s="7"/>
+      <c r="J2" s="9"/>
+    </row>
+    <row r="3" ht="15.1" customHeight="1" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="E3" s="7">
         <v>0</v>
       </c>
-      <c r="F3" s="7"/>
+      <c r="F3" s="7" t="s">
+        <v>159</v>
+      </c>
       <c r="G3" s="7"/>
-      <c r="I3" s="9"/>
-    </row>
-    <row r="4" ht="15.1" customHeight="1" spans="1:7">
+      <c r="H3" s="7"/>
+      <c r="J3" s="9"/>
+    </row>
+    <row r="4" ht="15.1" customHeight="1" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E4" s="7">
         <v>0</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="7" t="s">
+        <v>159</v>
+      </c>
       <c r="G4" s="7"/>
-    </row>
-    <row r="5" ht="15.1" customHeight="1" spans="1:5">
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" ht="15.1" customHeight="1" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>34</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="E5" s="1">
         <v>0</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -2185,10 +2203,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>69</v>
@@ -2214,102 +2232,102 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -2360,10 +2378,10 @@
         <v>120</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
@@ -2380,19 +2398,19 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>17</v>
@@ -2440,7 +2458,7 @@
         <v>120</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>18</v>
@@ -2491,13 +2509,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>132</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>120</v>
@@ -2530,12 +2548,12 @@
   <sheetPr/>
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F8" sqref="F8:F10"/>
+      <selection pane="bottomRight" activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1"/>
@@ -2554,10 +2572,10 @@
         <v>69</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>120</v>
@@ -2577,100 +2595,100 @@
     </row>
     <row r="2" customHeight="1" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D2" s="1">
         <v>0.3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D3" s="1">
         <v>0.0003</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:6">
       <c r="A4" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>195</v>
       </c>
       <c r="D4" s="1">
         <v>0.0003</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D6" s="1">
         <v>2000</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D7" s="1">
         <v>0.0003</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D8" s="1">
         <v>0.001</v>
@@ -2681,10 +2699,10 @@
     </row>
     <row r="9" customHeight="1" spans="1:6">
       <c r="A9" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>202</v>
       </c>
       <c r="D9" s="1">
         <v>0.001</v>
@@ -2695,10 +2713,10 @@
     </row>
     <row r="10" customHeight="1" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D10" s="1">
         <v>0.01</v>
@@ -2712,13 +2730,13 @@
         <v>57</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D11" s="1">
         <v>1100</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="12" customHeight="1" spans="1:6">
@@ -2726,31 +2744,31 @@
         <v>62</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D12" s="1">
         <v>1000</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="13" customHeight="1" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D13" s="4">
         <v>6.02214075862e+23</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F10">
+  <autoFilter ref="A1:F13">
     <extLst/>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2839,7 +2857,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>120</v>
@@ -2848,19 +2866,19 @@
         <v>69</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>18</v>
@@ -2911,46 +2929,46 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>69</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>18</v>
@@ -2961,66 +2979,66 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:16">
       <c r="A2" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F2" s="1">
         <v>2016</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K2" s="1">
         <v>44</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:16">
       <c r="A3" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="F3" s="1">
         <v>2017</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K3" s="1">
         <v>45</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating wc-files with new experiment worksheet
</commit_message>
<xml_diff>
--- a/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
+++ b/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
@@ -5,95 +5,96 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="19800" windowHeight="6840" tabRatio="993" activeTab="9"/>
+    <workbookView windowWidth="19800" windowHeight="6840" tabRatio="993" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
     <sheet name="Taxon" sheetId="2" r:id="rId2"/>
-    <sheet name="Submodels" sheetId="3" r:id="rId3"/>
-    <sheet name="Compartments" sheetId="4" r:id="rId4"/>
-    <sheet name="Species types" sheetId="5" r:id="rId5"/>
-    <sheet name="Species" sheetId="6" r:id="rId6"/>
-    <sheet name="Initial species concentrations" sheetId="7" r:id="rId7"/>
-    <sheet name="Observables" sheetId="8" r:id="rId8"/>
-    <sheet name="Functions" sheetId="9" r:id="rId9"/>
-    <sheet name="Reactions" sheetId="10" r:id="rId10"/>
-    <sheet name="Rate laws" sheetId="11" r:id="rId11"/>
-    <sheet name="dFBA objectives" sheetId="12" r:id="rId12"/>
-    <sheet name="dFBA net reactions" sheetId="13" r:id="rId13"/>
-    <sheet name="dFBA net species" sheetId="14" r:id="rId14"/>
-    <sheet name="Parameters" sheetId="15" r:id="rId15"/>
-    <sheet name="Stop conditions" sheetId="16" r:id="rId16"/>
-    <sheet name="Evidence" sheetId="17" r:id="rId17"/>
-    <sheet name="References" sheetId="18" r:id="rId18"/>
+    <sheet name="Environment" sheetId="19" r:id="rId3"/>
+    <sheet name="Submodels" sheetId="3" r:id="rId4"/>
+    <sheet name="Compartments" sheetId="4" r:id="rId5"/>
+    <sheet name="Species types" sheetId="5" r:id="rId6"/>
+    <sheet name="Species" sheetId="6" r:id="rId7"/>
+    <sheet name="Initial species concentrations" sheetId="7" r:id="rId8"/>
+    <sheet name="Observables" sheetId="8" r:id="rId9"/>
+    <sheet name="Functions" sheetId="9" r:id="rId10"/>
+    <sheet name="Reactions" sheetId="10" r:id="rId11"/>
+    <sheet name="Rate laws" sheetId="11" r:id="rId12"/>
+    <sheet name="dFBA objectives" sheetId="12" r:id="rId13"/>
+    <sheet name="dFBA net reactions" sheetId="13" r:id="rId14"/>
+    <sheet name="dFBA net species" sheetId="14" r:id="rId15"/>
+    <sheet name="Parameters" sheetId="15" r:id="rId16"/>
+    <sheet name="Stop conditions" sheetId="16" r:id="rId17"/>
+    <sheet name="Evidence" sheetId="17" r:id="rId18"/>
+    <sheet name="References" sheetId="18" r:id="rId19"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId19"/>
+    <externalReference r:id="rId20"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Compartments!$A$1:$G$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Species types'!$A$1:$K$11</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Initial species concentrations'!$C$1:$K$8</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'Rate laws'!$C$1:$H$6</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">Parameters!$A$1:$F$13</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">References!$A$1:$D$3</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="2">Submodels!#REF!</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2">Submodels!$A$1:$G$3</definedName>
-    <definedName name="excel_is_bugging_me" localSheetId="3">Compartments!$A$1:$G$3</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="3">Compartments!$A$1:$G$3</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="3">Compartments!$A$1:$G$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="3">Compartments!$A$1:$G$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="3">Compartments!$A$1:$G$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$G$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$G$3</definedName>
-    <definedName name="excel_is_bugging_me" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="6">'[1]#REF'!$C$1:$K$8</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="6">'[1]#REF'!$C$1:$K$8</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="6">'[1]#REF'!$C$1:$K$8</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="6">'[1]#REF'!$C$1:$K$8</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="6">'[1]#REF'!$C$1:$K$8</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="6">'[1]#REF'!$C$1:$K$8</definedName>
-    <definedName name="excel_is_bugging_me" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="10">'Rate laws'!$C$1:$H$6</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="10">'Rate laws'!$C$1:$H$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="10">'Rate laws'!$C$1:$H$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="10">'Rate laws'!$C$1:$H$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="10">'Rate laws'!$C$1:$H$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="10">'Rate laws'!$C$1:$H$6</definedName>
-    <definedName name="excel_is_bugging_me" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="excel_is_bugging_me" localSheetId="17">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="17">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="17">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="17">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="17">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="17">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="17">References!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Compartments!$A$1:$G$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Species types'!$A$1:$K$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Initial species concentrations'!$C$1:$K$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'Rate laws'!$C$1:$H$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">Parameters!$A$1:$F$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">References!$A$1:$D$3</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="3">Submodels!#REF!</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3">Submodels!$A$1:$G$3</definedName>
+    <definedName name="excel_is_bugging_me" localSheetId="4">Compartments!$A$1:$G$3</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="4">Compartments!$A$1:$G$3</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="4">Compartments!$A$1:$G$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="4">Compartments!$A$1:$G$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="4">Compartments!$A$1:$G$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$G$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$G$3</definedName>
+    <definedName name="excel_is_bugging_me" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="7">'[1]#REF'!$C$1:$K$8</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="7">'[1]#REF'!$C$1:$K$8</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="7">'[1]#REF'!$C$1:$K$8</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="7">'[1]#REF'!$C$1:$K$8</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="7">'[1]#REF'!$C$1:$K$8</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="7">'[1]#REF'!$C$1:$K$8</definedName>
+    <definedName name="excel_is_bugging_me" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="11">'Rate laws'!$C$1:$H$6</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="11">'Rate laws'!$C$1:$H$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="11">'Rate laws'!$C$1:$H$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="11">'Rate laws'!$C$1:$H$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="11">'Rate laws'!$C$1:$H$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="11">'Rate laws'!$C$1:$H$6</definedName>
+    <definedName name="excel_is_bugging_me" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="excel_is_bugging_me" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="242">
   <si>
     <t>Id</t>
   </si>
@@ -161,7 +162,7 @@
     <t>Updated</t>
   </si>
   <si>
-    <t>mpn_m129</t>
+    <t>taxon</t>
   </si>
   <si>
     <t>Mycoplasma pneumoniae M129</t>
@@ -177,6 +178,21 @@
   </si>
   <si>
     <t>References</t>
+  </si>
+  <si>
+    <t>env</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>Temperature units</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>pH</t>
   </si>
   <si>
     <t>Algorithm</t>
@@ -730,9 +746,6 @@
   </si>
   <si>
     <t>Temperature (C)</t>
-  </si>
-  <si>
-    <t>pH</t>
   </si>
   <si>
     <t>Growth media</t>
@@ -816,11 +829,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
     <numFmt numFmtId="176" formatCode="0.000E+00"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -855,9 +868,74 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -872,81 +950,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -958,9 +964,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -975,9 +980,16 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -988,18 +1000,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1018,25 +1031,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1049,42 +1062,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1108,6 +1085,60 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1120,13 +1151,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1144,43 +1175,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1198,7 +1193,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1223,54 +1236,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1293,19 +1263,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1314,147 +1288,186 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1488,6 +1501,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -2017,9 +2033,87 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="2" width="8.78333333333333" style="1"/>
+    <col min="3" max="3" width="11" style="1" customWidth="1"/>
+    <col min="4" max="1025" width="8.78333333333333" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customHeight="1" spans="1:8">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" customHeight="1" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" customHeight="1" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
@@ -2044,31 +2138,31 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>18</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>19</v>
@@ -2079,22 +2173,22 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="E2" s="7">
         <v>1</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -2102,22 +2196,22 @@
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="E3" s="7">
         <v>0</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -2125,44 +2219,44 @@
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="E4" s="7">
         <v>0</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="E5" s="1">
         <v>0</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -2175,7 +2269,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:K6"/>
@@ -2203,25 +2297,25 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>19</v>
@@ -2232,102 +2326,102 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:7">
       <c r="A4" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>173</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -2340,7 +2434,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:K2"/>
@@ -2369,25 +2463,25 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>144</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>19</v>
@@ -2398,19 +2492,19 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>17</v>
@@ -2426,7 +2520,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:I1"/>
@@ -2452,19 +2546,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>18</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>19</v>
@@ -2483,7 +2577,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:J1"/>
@@ -2509,22 +2603,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>18</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>19</v>
@@ -2543,7 +2637,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:J13"/>
@@ -2569,22 +2663,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>18</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>19</v>
@@ -2595,176 +2689,176 @@
     </row>
     <row r="2" customHeight="1" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="D2" s="1">
         <v>0.3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="D3" s="1">
         <v>0.0003</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="D4" s="1">
         <v>0.0003</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="D6" s="1">
         <v>2000</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:6">
       <c r="A7" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>196</v>
       </c>
       <c r="D7" s="1">
         <v>0.0003</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="D8" s="1">
         <v>0.001</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="D9" s="1">
         <v>0.001</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" customHeight="1" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="D10" s="1">
         <v>0.01</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" customHeight="1" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="D11" s="1">
         <v>1100</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
     </row>
     <row r="12" customHeight="1" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="D12" s="1">
         <v>1000</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
     </row>
     <row r="13" customHeight="1" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="D13" s="4">
         <v>6.02214075862e+23</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -2777,7 +2871,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:H1"/>
@@ -2803,16 +2897,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>19</v>
@@ -2831,7 +2925,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:N1"/>
@@ -2857,34 +2951,34 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>212</v>
+        <v>32</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>18</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>19</v>
@@ -2903,7 +2997,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:R3"/>
@@ -2929,46 +3023,46 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>18</v>
@@ -2979,66 +3073,66 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:16">
       <c r="A2" s="1" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="F2" s="1">
         <v>2016</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="K2" s="1">
         <v>44</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:16">
       <c r="A3" s="1" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="F3" s="1">
         <v>2017</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="K3" s="1">
         <v>45</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -3059,7 +3153,7 @@
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="D34" sqref="D34"/>
+      <selection pane="topRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5" outlineLevelCol="1"/>
@@ -3117,6 +3211,84 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection/>
+      <selection pane="topRight" activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelRow="7" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="18.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.375" style="1" customWidth="1"/>
+    <col min="3" max="1018" width="8.78333333333333" style="1"/>
+    <col min="1019" max="1019" width="8.78333333333333" style="12"/>
+    <col min="1020" max="16384" width="9" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" customHeight="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" customHeight="1" spans="1:1">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" customHeight="1" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" customHeight="1" spans="1:2">
+      <c r="A4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" customHeight="1" spans="1:2">
+      <c r="A5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="1">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="6" customHeight="1" spans="1:1">
+      <c r="A6" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" customHeight="1" spans="1:1">
+      <c r="A7" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" customHeight="1" spans="1:1">
+      <c r="A8" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:G3"/>
@@ -3145,13 +3317,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>19</v>
@@ -3162,30 +3334,30 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -3195,7 +3367,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:P3"/>
@@ -3221,40 +3393,40 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>18</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>19</v>
@@ -3265,28 +3437,28 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:15">
       <c r="A2" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="I2" s="4">
         <v>4.58e-17</v>
@@ -3295,39 +3467,39 @@
         <v>4.58e-18</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:15">
       <c r="A3" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="I3" s="1">
         <v>1</v>
@@ -3336,16 +3508,16 @@
         <v>0</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -3358,7 +3530,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:K11"/>
@@ -3386,25 +3558,25 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>19</v>
@@ -3415,16 +3587,16 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="E2" s="1">
         <v>424.1773</v>
@@ -3433,25 +3605,25 @@
         <v>-3</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="J2" s="10"/>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E3" s="1">
         <v>345.2053</v>
@@ -3460,25 +3632,25 @@
         <v>-2</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="J3" s="10"/>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="E4" s="1">
         <v>503.14946</v>
@@ -3487,25 +3659,25 @@
         <v>-4</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="J4" s="10"/>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="E5" s="1">
         <v>180.15588</v>
@@ -3514,22 +3686,22 @@
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="J5" s="10"/>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:10">
       <c r="A6" s="1" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E6" s="1">
         <v>1.00783</v>
@@ -3538,25 +3710,25 @@
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="J6" s="10"/>
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="E7" s="1">
         <v>18.0153</v>
@@ -3565,24 +3737,24 @@
         <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" ht="15.1" customHeight="1" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="E8" s="1">
         <v>95.9793</v>
@@ -3591,24 +3763,24 @@
         <v>-2</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" ht="15.1" customHeight="1" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="E9" s="1">
         <v>174.95</v>
@@ -3617,21 +3789,21 @@
         <v>-4</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" ht="15.1" customHeight="1" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="E10" s="1">
         <v>3298.98577</v>
@@ -3640,21 +3812,21 @@
         <v>-11</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" ht="15.1" customHeight="1" spans="1:9">
       <c r="A11" s="1" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="E11" s="1">
         <v>1042.32919</v>
@@ -3663,7 +3835,7 @@
         <v>-8</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
@@ -3678,7 +3850,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:I11"/>
@@ -3705,19 +3877,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>18</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>19</v>
@@ -3728,152 +3900,152 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="1" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="1" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" ht="15.1" customHeight="1" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="1" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" ht="15.1" customHeight="1" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" ht="15.1" customHeight="1" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="1" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" ht="15.1" customHeight="1" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="1" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -3886,7 +4058,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:K8"/>
@@ -3913,25 +4085,25 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>19</v>
@@ -3942,13 +4114,13 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="E2" s="10">
         <v>0.005</v>
@@ -3957,125 +4129,125 @@
         <v>0.0121655250605964</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:9">
       <c r="A3" s="1" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="E3" s="10">
         <v>0.005</v>
       </c>
       <c r="F3" s="10"/>
       <c r="G3" s="10" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:9">
       <c r="A4" s="1" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="E4" s="10">
         <v>0.005</v>
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:9">
       <c r="A5" s="1" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="E5" s="10">
         <v>0.01</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:9">
       <c r="A6" s="1" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="E6" s="1">
         <v>1e-7</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="10" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:9">
       <c r="A7" s="1" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="E7" s="10">
         <v>55</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="10" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
     </row>
     <row r="8" ht="15.1" customHeight="1" spans="1:9">
       <c r="A8" s="1" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="E8" s="4">
         <v>0.005</v>
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="10" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
@@ -4090,7 +4262,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:H1"/>
@@ -4116,100 +4288,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>18</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>19</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:H3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" outlineLevelCol="7"/>
-  <cols>
-    <col min="1" max="2" width="8.78333333333333" style="1"/>
-    <col min="3" max="3" width="11" style="1" customWidth="1"/>
-    <col min="4" max="1025" width="8.78333333333333" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" customHeight="1" spans="1:8">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" customHeight="1" spans="1:4">
-      <c r="A2" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" customHeight="1" spans="1:4">
-      <c r="A3" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating for renaming wc_lang DfbaNetReaction --> DfbaObjReaction, DfbaNetSpecies --> DfbaObjSpecies
</commit_message>
<xml_diff>
--- a/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
+++ b/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="19800" windowHeight="6840" tabRatio="993" activeTab="2"/>
+    <workbookView windowWidth="28200" windowHeight="14070" tabRatio="993" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,8 @@
     <sheet name="Reactions" sheetId="10" r:id="rId11"/>
     <sheet name="Rate laws" sheetId="11" r:id="rId12"/>
     <sheet name="dFBA objectives" sheetId="12" r:id="rId13"/>
-    <sheet name="dFBA net reactions" sheetId="13" r:id="rId14"/>
-    <sheet name="dFBA net species" sheetId="14" r:id="rId15"/>
+    <sheet name="dFBA objective reactions" sheetId="13" r:id="rId14"/>
+    <sheet name="dFBA objective species" sheetId="14" r:id="rId15"/>
     <sheet name="Parameters" sheetId="15" r:id="rId16"/>
     <sheet name="Stop conditions" sheetId="16" r:id="rId17"/>
     <sheet name="Evidence" sheetId="17" r:id="rId18"/>
@@ -679,7 +679,7 @@
     <t>Cell size units</t>
   </si>
   <si>
-    <t>dFBA net reaction</t>
+    <t>dFBA objective reaction</t>
   </si>
   <si>
     <t>Value</t>
@@ -828,12 +828,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="0.000E+00"/>
+    <numFmt numFmtId="176" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="0.000E+00"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -868,21 +868,22 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -895,24 +896,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -927,10 +919,41 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -941,16 +964,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -958,14 +980,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -979,40 +1008,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1031,7 +1031,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1043,13 +1055,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1067,13 +1079,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1091,37 +1109,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1133,19 +1139,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1163,7 +1163,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1175,43 +1211,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1234,17 +1234,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1256,6 +1245,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1284,11 +1282,37 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1307,163 +1331,139 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1493,10 +1493,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2582,12 +2582,12 @@
   <sheetPr/>
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -3215,7 +3215,7 @@
   <sheetPr/>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection/>
       <selection pane="topRight" activeCell="D6" sqref="D6"/>

</xml_diff>

<commit_message>
updating for changes to wc_lang.Evidence and wc_lang.Intrepretation
</commit_message>
<xml_diff>
--- a/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
+++ b/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="19800" windowHeight="6840" tabRatio="993" activeTab="2"/>
+    <workbookView windowWidth="19800" windowHeight="6945" tabRatio="993" firstSheet="11" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -26,21 +26,22 @@
     <sheet name="Parameters" sheetId="15" r:id="rId16"/>
     <sheet name="Stop conditions" sheetId="16" r:id="rId17"/>
     <sheet name="Evidence" sheetId="17" r:id="rId18"/>
-    <sheet name="References" sheetId="18" r:id="rId19"/>
+    <sheet name="Interpretations" sheetId="20" r:id="rId19"/>
+    <sheet name="References" sheetId="18" r:id="rId20"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId20"/>
+    <externalReference r:id="rId21"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Compartments!$A$1:$G$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Species types'!$A$1:$K$11</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Initial species concentrations'!$C$1:$K$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Species types'!$A$1:$L$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Initial species concentrations'!$C$1:$L$8</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">Reactions!$A$1:$D$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'Rate laws'!$C$1:$H$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">Parameters!$A$1:$F$13</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">References!$A$1:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">References!$A$1:$D$3</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="3">Submodels!#REF!</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3">Submodels!$A$1:$G$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3">Submodels!$A$1:$H$3</definedName>
     <definedName name="excel_is_bugging_me" localSheetId="4">Compartments!$A$1:$G$3</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="4">Compartments!$A$1:$G$3</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="4">Compartments!$A$1:$G$3</definedName>
@@ -48,13 +49,13 @@
     <definedName name="_FilterDatabase_0_0_0_0" localSheetId="4">Compartments!$A$1:$G$3</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$G$3</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$G$3</definedName>
-    <definedName name="excel_is_bugging_me" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="excel_is_bugging_me" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="7">'[1]#REF'!$C$1:$K$8</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="7">'[1]#REF'!$C$1:$K$8</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="7">'[1]#REF'!$C$1:$K$8</definedName>
@@ -81,20 +82,20 @@
     <definedName name="_FilterDatabase_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
-    <definedName name="excel_is_bugging_me" localSheetId="18">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="18">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="excel_is_bugging_me" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="249">
   <si>
     <t>Id</t>
   </si>
@@ -205,6 +206,9 @@
   </si>
   <si>
     <t>Evidence</t>
+  </si>
+  <si>
+    <t>Interpretations</t>
   </si>
   <si>
     <t>metabolism</t>
@@ -748,10 +752,25 @@
     <t>Genetic variant</t>
   </si>
   <si>
-    <t>Temperature (C)</t>
-  </si>
-  <si>
     <t>Growth media</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>Experiment type</t>
+  </si>
+  <si>
+    <t>Experiment design</t>
+  </si>
+  <si>
+    <t>Measurement method</t>
+  </si>
+  <si>
+    <t>Analysis method</t>
+  </si>
+  <si>
+    <t>Method</t>
   </si>
   <si>
     <t>Title</t>
@@ -831,12 +850,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="0.000E+00"/>
+    <numFmt numFmtId="176" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="0.000E+00"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -879,6 +898,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -887,16 +918,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -905,20 +939,6 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -931,10 +951,17 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -952,32 +979,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -985,6 +995,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -998,17 +1016,18 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1034,7 +1053,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1046,19 +1125,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1070,37 +1143,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1112,7 +1179,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1130,85 +1221,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1256,6 +1275,15 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
@@ -1276,26 +1304,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1307,6 +1315,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1337,140 +1356,140 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1481,6 +1500,9 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1496,10 +1518,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2036,24 +2058,24 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:D3"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelRow="2"/>
   <cols>
     <col min="1" max="2" width="8.78333333333333" style="1"/>
     <col min="3" max="3" width="11" style="1" customWidth="1"/>
-    <col min="4" max="1025" width="8.78333333333333" style="1"/>
+    <col min="4" max="1026" width="8.78333333333333" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:8">
+    <row r="1" customHeight="1" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2061,10 +2083,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>18</v>
@@ -2073,32 +2095,35 @@
         <v>36</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -2114,14 +2139,14 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F2" sqref="F2:F5"/>
+      <selection pane="bottomRight" activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4"/>
@@ -2130,10 +2155,10 @@
     <col min="2" max="2" width="18.2916666666667" style="1"/>
     <col min="3" max="3" width="13.3416666666667" style="1"/>
     <col min="4" max="4" width="40.575" style="1"/>
-    <col min="5" max="1026" width="8.78333333333333" style="1"/>
+    <col min="5" max="1027" width="8.78333333333333" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:13">
+    <row r="1" ht="15.1" customHeight="1" spans="1:14">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2141,25 +2166,25 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>18</v>
@@ -2168,98 +2193,101 @@
         <v>36</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="E2" s="7">
+        <v>38</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="E2" s="8">
         <v>1</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="J2" s="9"/>
+      <c r="F2" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="J2" s="10"/>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:10">
       <c r="A3" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E3" s="8">
+        <v>0</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="E3" s="7">
-        <v>0</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="J3" s="9"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="J3" s="10"/>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="E4" s="7">
+        <v>38</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="E4" s="8">
         <v>0</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
+      <c r="F4" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E5" s="1">
         <v>0</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>166</v>
+      <c r="F5" s="8" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -2275,24 +2303,24 @@
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomRight" activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5"/>
   <cols>
     <col min="1" max="5" width="8.78333333333333" style="1"/>
     <col min="6" max="6" width="68.5" style="1" customWidth="1"/>
-    <col min="7" max="1025" width="8.78333333333333" style="1"/>
+    <col min="7" max="1026" width="8.78333333333333" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:11">
+    <row r="1" ht="15.1" customHeight="1" spans="1:12">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2300,19 +2328,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
@@ -2321,110 +2349,113 @@
         <v>36</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="E2" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>180</v>
       </c>
+      <c r="E2" s="8" t="s">
+        <v>181</v>
+      </c>
       <c r="F2" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>180</v>
+        <v>164</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>181</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>180</v>
+        <v>171</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>181</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>180</v>
+        <v>174</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>181</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -2440,14 +2471,14 @@
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomRight" activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
@@ -2455,10 +2486,10 @@
     <col min="1" max="1" width="17" style="1" customWidth="1"/>
     <col min="2" max="4" width="9.10833333333333" style="1"/>
     <col min="5" max="6" width="12.25" style="1" customWidth="1"/>
-    <col min="7" max="1027" width="9.10833333333333" style="1"/>
+    <col min="7" max="1028" width="9.10833333333333" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:11">
+    <row r="1" ht="15.1" customHeight="1" spans="1:12">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2466,19 +2497,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
@@ -2487,27 +2518,30 @@
         <v>36</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>167</v>
+        <v>38</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>168</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>17</v>
@@ -2526,22 +2560,22 @@
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="P36" sqref="P36"/>
+      <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1025" width="8.78333333333333" style="1"/>
+    <col min="1" max="1026" width="8.78333333333333" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:9">
+    <row r="1" ht="15.1" customHeight="1" spans="1:10">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2549,13 +2583,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>18</v>
@@ -2564,9 +2598,12 @@
         <v>36</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2583,50 +2620,53 @@
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomRight" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1025" width="8.78333333333333" style="1"/>
+    <col min="1" max="1026" width="8.78333333333333" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:10">
-      <c r="A1" s="5" t="s">
+    <row r="1" ht="15.1" customHeight="1" spans="1:11">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="E1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="G1" s="5" t="s">
+      <c r="D1" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>18</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="6" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2643,22 +2683,22 @@
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K12" sqref="K12"/>
+      <selection pane="bottomRight" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1025" width="8.78333333333333" style="1"/>
+    <col min="1" max="1026" width="8.78333333333333" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:10">
+    <row r="1" customHeight="1" spans="1:11">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2666,16 +2706,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>18</v>
@@ -2684,21 +2724,24 @@
         <v>36</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" customHeight="1" spans="1:10">
+    <row r="2" customHeight="1" spans="1:11">
       <c r="A2" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D2" s="1">
         <v>0.3</v>
@@ -2706,162 +2749,162 @@
       <c r="F2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>200</v>
+      <c r="K2" s="1" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D3" s="1">
         <v>0.0003</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:6">
       <c r="A4" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>202</v>
       </c>
       <c r="D4" s="1">
         <v>0.0003</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D6" s="1">
         <v>2000</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D7" s="1">
         <v>0.0003</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D8" s="1">
         <v>0.001</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="1:6">
       <c r="A9" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="D9" s="1">
         <v>0.001</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" customHeight="1" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D10" s="1">
         <v>0.01</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" customHeight="1" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D11" s="1">
         <v>1100</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="12" customHeight="1" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D12" s="1">
         <v>1000</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="13" customHeight="1" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="D13" s="4">
+        <v>181</v>
+      </c>
+      <c r="D13" s="5">
         <v>6.02214075862e+23</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -2877,22 +2920,22 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1025" width="8.78333333333333" style="1"/>
+    <col min="1" max="1026" width="8.78333333333333" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:8">
+    <row r="1" ht="15.1" customHeight="1" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2900,10 +2943,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>18</v>
@@ -2912,9 +2955,12 @@
         <v>36</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2931,14 +2977,14 @@
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:V1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="N28" sqref="N28"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1:V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2946,7 +2992,7 @@
     <col min="1" max="1025" width="9.10833333333333" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:14">
+    <row r="1" ht="15.1" customHeight="1" spans="1:22">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2954,16 +3000,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>127</v>
+        <v>198</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>76</v>
+        <v>128</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>215</v>
+        <v>77</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>216</v>
@@ -2972,21 +3018,45 @@
         <v>217</v>
       </c>
       <c r="I1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="N1" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3003,148 +3073,98 @@
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E18" sqref="E18"/>
+      <selection pane="bottomRight" activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1025" width="8.78333333333333" style="1"/>
+    <col min="1" max="1" width="15.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.75" style="1" customWidth="1"/>
+    <col min="3" max="1022" width="9.10833333333333" style="1"/>
+    <col min="1023" max="1023" width="9.10833333333333"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:18">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="15.1" customHeight="1" spans="1:11">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="J1" s="2" t="s">
+      <c r="C1" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="Q1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="I1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:16">
-      <c r="A2" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="F2" s="1">
-        <v>2016</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="K2" s="1">
-        <v>44</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="3" ht="15.1" customHeight="1" spans="1:16">
-      <c r="A3" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="F3" s="1">
-        <v>2017</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="K3" s="1">
-        <v>45</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>242</v>
-      </c>
+      <c r="K1" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" ht="15.1" customHeight="1" spans="3:4">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" ht="15.1" customHeight="1" spans="3:4">
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" ht="15.1" customHeight="1" spans="3:4">
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" ht="15.1" customHeight="1" spans="3:4">
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" ht="15.1" customHeight="1" spans="3:4">
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" ht="15.1" customHeight="1" spans="3:4">
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" ht="15.1" customHeight="1" spans="3:4">
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" ht="15.1" customHeight="1" spans="3:4">
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D3">
-    <extLst/>
-  </autoFilter>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -3213,12 +3233,160 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:R3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2"/>
+  <cols>
+    <col min="1" max="1025" width="8.78333333333333" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.1" customHeight="1" spans="1:18">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" ht="15.1" customHeight="1" spans="1:16">
+      <c r="A2" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2016</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="K2" s="1">
+        <v>44</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="3" ht="15.1" customHeight="1" spans="1:16">
+      <c r="A3" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2017</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="K3" s="1">
+        <v>45</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D3">
+    <extLst/>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection/>
       <selection pane="topRight" activeCell="A6" sqref="A6:B6"/>
@@ -3229,8 +3397,8 @@
     <col min="1" max="1" width="18.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="5.375" style="1" customWidth="1"/>
     <col min="3" max="1018" width="8.78333333333333" style="1"/>
-    <col min="1019" max="1019" width="8.78333333333333" style="12"/>
-    <col min="1020" max="16384" width="9" style="12"/>
+    <col min="1019" max="1019" width="8.78333333333333" style="13"/>
+    <col min="1020" max="16384" width="9" style="13"/>
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:2">
@@ -3302,25 +3470,25 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="13" style="1"/>
     <col min="2" max="2" width="13.4416666666667" style="1"/>
     <col min="3" max="3" width="13.225" style="1"/>
-    <col min="4" max="1025" width="8.78333333333333" style="1"/>
+    <col min="4" max="1026" width="8.78333333333333" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:7">
+    <row r="1" ht="15.1" customHeight="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3337,38 +3505,41 @@
         <v>36</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -3381,57 +3552,57 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L2" sqref="L2:L3"/>
+      <selection pane="bottomRight" activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1030" width="8.78333333333333" style="1"/>
+    <col min="1" max="1031" width="8.78333333333333" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:16">
-      <c r="A1" s="11" t="s">
+    <row r="1" ht="15.1" customHeight="1" spans="1:17">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>18</v>
@@ -3440,77 +3611,80 @@
         <v>36</v>
       </c>
       <c r="O1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:15">
+    <row r="2" ht="15.1" customHeight="1" spans="1:16">
       <c r="A2" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="I2" s="4">
+        <v>63</v>
+      </c>
+      <c r="I2" s="5">
         <v>4.58e-17</v>
       </c>
       <c r="J2" s="1">
         <v>4.58e-18</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" ht="15.1" customHeight="1" spans="1:16">
+      <c r="A3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" ht="15.1" customHeight="1" spans="1:15">
-      <c r="A3" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="I3" s="1">
         <v>1</v>
@@ -3519,16 +3693,16 @@
         <v>0</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="O3" s="1" t="s">
         <v>71</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -3544,24 +3718,24 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomRight" activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="3" width="8.78333333333333" style="1"/>
     <col min="4" max="4" width="17.3083333333333" style="1"/>
-    <col min="5" max="1025" width="8.78333333333333" style="1"/>
+    <col min="5" max="1026" width="8.78333333333333" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:11">
+    <row r="1" ht="15.1" customHeight="1" spans="1:12">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3569,19 +3743,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
@@ -3590,24 +3764,27 @@
         <v>36</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:10">
+    <row r="2" ht="15.1" customHeight="1" spans="1:11">
       <c r="A2" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E2" s="1">
         <v>424.1773</v>
@@ -3616,25 +3793,25 @@
         <v>-3</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="J2" s="10"/>
-    </row>
-    <row r="3" ht="15.1" customHeight="1" spans="1:10">
+        <v>83</v>
+      </c>
+      <c r="K2" s="11"/>
+    </row>
+    <row r="3" ht="15.1" customHeight="1" spans="1:11">
       <c r="A3" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E3" s="1">
         <v>345.2053</v>
@@ -3643,25 +3820,25 @@
         <v>-2</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="J3" s="10"/>
-    </row>
-    <row r="4" ht="15.1" customHeight="1" spans="1:10">
+        <v>88</v>
+      </c>
+      <c r="K3" s="11"/>
+    </row>
+    <row r="4" ht="15.1" customHeight="1" spans="1:11">
       <c r="A4" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E4" s="1">
         <v>503.14946</v>
@@ -3670,25 +3847,25 @@
         <v>-4</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="J4" s="10"/>
-    </row>
-    <row r="5" ht="15.1" customHeight="1" spans="1:10">
+        <v>93</v>
+      </c>
+      <c r="K4" s="11"/>
+    </row>
+    <row r="5" ht="15.1" customHeight="1" spans="1:11">
       <c r="A5" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E5" s="1">
         <v>180.15588</v>
@@ -3697,22 +3874,22 @@
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="J5" s="10"/>
-    </row>
-    <row r="6" ht="15.1" customHeight="1" spans="1:10">
+        <v>82</v>
+      </c>
+      <c r="K5" s="11"/>
+    </row>
+    <row r="6" ht="15.1" customHeight="1" spans="1:11">
       <c r="A6" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E6" s="1">
         <v>1.00783</v>
@@ -3721,25 +3898,25 @@
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="J6" s="10"/>
+        <v>102</v>
+      </c>
+      <c r="K6" s="11"/>
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E7" s="1">
         <v>18.0153</v>
@@ -3748,24 +3925,24 @@
         <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" ht="15.1" customHeight="1" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E8" s="1">
         <v>95.9793</v>
@@ -3774,24 +3951,24 @@
         <v>-2</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" ht="15.1" customHeight="1" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E9" s="1">
         <v>174.95</v>
@@ -3800,21 +3977,21 @@
         <v>-4</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" ht="15.1" customHeight="1" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E10" s="1">
         <v>3298.98577</v>
@@ -3823,21 +4000,21 @@
         <v>-11</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="11" ht="15.1" customHeight="1" spans="1:9">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" ht="15.1" customHeight="1" spans="1:10">
       <c r="A11" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E11" s="1">
         <v>1042.32919</v>
@@ -3845,14 +4022,15 @@
       <c r="F11" s="1">
         <v>-8</v>
       </c>
-      <c r="G11" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
+      <c r="G11" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K11">
+  <autoFilter ref="A1:L11">
     <extLst/>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3864,23 +4042,23 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D32" sqref="D32"/>
+      <selection pane="bottomRight" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="9" width="15.9583333333333" style="1"/>
-    <col min="10" max="1025" width="9.10833333333333" style="1"/>
+    <col min="1" max="10" width="15.9583333333333" style="1"/>
+    <col min="11" max="1026" width="9.10833333333333" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:9">
+    <row r="1" ht="15.1" customHeight="1" spans="1:10">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3888,13 +4066,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>18</v>
@@ -3903,160 +4081,163 @@
         <v>36</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B2" s="9"/>
+        <v>129</v>
+      </c>
+      <c r="B2" s="10"/>
       <c r="C2" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:5">
       <c r="A3" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B4" s="9"/>
+        <v>132</v>
+      </c>
+      <c r="B4" s="10"/>
       <c r="C4" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B5" s="9"/>
+        <v>133</v>
+      </c>
+      <c r="B5" s="10"/>
       <c r="C5" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B6" s="9"/>
+        <v>134</v>
+      </c>
+      <c r="B6" s="10"/>
       <c r="C6" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B7" s="9"/>
+        <v>135</v>
+      </c>
+      <c r="B7" s="10"/>
       <c r="C7" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" ht="15.1" customHeight="1" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B8" s="9"/>
+        <v>136</v>
+      </c>
+      <c r="B8" s="10"/>
       <c r="C8" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" ht="15.1" customHeight="1" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B9" s="9"/>
+        <v>137</v>
+      </c>
+      <c r="B9" s="10"/>
       <c r="C9" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" ht="15.1" customHeight="1" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B10" s="9"/>
+        <v>138</v>
+      </c>
+      <c r="B10" s="10"/>
       <c r="C10" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" ht="15.1" customHeight="1" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B11" s="9"/>
+        <v>139</v>
+      </c>
+      <c r="B11" s="10"/>
       <c r="C11" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -4072,23 +4253,23 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomRight" activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7"/>
   <cols>
     <col min="1" max="1" width="16.625" style="1" customWidth="1"/>
-    <col min="2" max="1025" width="8.78333333333333" style="1"/>
+    <col min="2" max="1026" width="8.78333333333333" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:11">
+    <row r="1" ht="15.1" customHeight="1" spans="1:12">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4096,19 +4277,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
@@ -4117,154 +4298,163 @@
         <v>36</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E2" s="10">
+        <v>63</v>
+      </c>
+      <c r="E2" s="11">
         <v>0.005</v>
       </c>
       <c r="F2" s="1">
         <v>0.0121655250605964</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="3" ht="15.1" customHeight="1" spans="1:9">
+      <c r="G2" s="11" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" ht="15.1" customHeight="1" spans="1:10">
       <c r="A3" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="11">
+        <v>0.005</v>
+      </c>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E3" s="10">
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+    </row>
+    <row r="4" ht="15.1" customHeight="1" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="11">
         <v>0.005</v>
       </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-    </row>
-    <row r="4" ht="15.1" customHeight="1" spans="1:9">
-      <c r="A4" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E4" s="10">
-        <v>0.005</v>
-      </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-    </row>
-    <row r="5" ht="15.1" customHeight="1" spans="1:9">
+      <c r="F4" s="11"/>
+      <c r="G4" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+    </row>
+    <row r="5" ht="15.1" customHeight="1" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E5" s="10">
+        <v>63</v>
+      </c>
+      <c r="E5" s="11">
         <v>0.01</v>
       </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-    </row>
-    <row r="6" ht="15.1" customHeight="1" spans="1:9">
+      <c r="F5" s="11"/>
+      <c r="G5" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+    </row>
+    <row r="6" ht="15.1" customHeight="1" spans="1:10">
       <c r="A6" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E6" s="1">
         <v>1e-7</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-    </row>
-    <row r="7" ht="15.1" customHeight="1" spans="1:9">
+      <c r="F6" s="11"/>
+      <c r="G6" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+    </row>
+    <row r="7" ht="15.1" customHeight="1" spans="1:10">
       <c r="A7" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E7" s="10">
+        <v>63</v>
+      </c>
+      <c r="E7" s="11">
         <v>55</v>
       </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-    </row>
-    <row r="8" ht="15.1" customHeight="1" spans="1:9">
+      <c r="F7" s="11"/>
+      <c r="G7" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+    </row>
+    <row r="8" ht="15.1" customHeight="1" spans="1:10">
       <c r="A8" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E8" s="4">
+        <v>63</v>
+      </c>
+      <c r="E8" s="5">
         <v>0.005</v>
       </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
     </row>
   </sheetData>
-  <autoFilter ref="C1:K8">
+  <autoFilter ref="C1:L8">
     <extLst/>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -4276,22 +4466,22 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I26" sqref="I26"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1025" width="8.78333333333333" style="1"/>
+    <col min="1" max="1026" width="8.78333333333333" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:8">
+    <row r="1" ht="15.1" customHeight="1" spans="1:9">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4299,10 +4489,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>18</v>
@@ -4310,10 +4500,13 @@
       <c r="F1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updating for wc_lang ontologies
</commit_message>
<xml_diff>
--- a/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
+++ b/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="19800" windowHeight="6945" tabRatio="993" firstSheet="11" activeTab="16"/>
+    <workbookView windowWidth="28695" windowHeight="14070" tabRatio="993" firstSheet="6" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="248">
   <si>
     <t>Id</t>
   </si>
@@ -202,7 +202,7 @@
     <t>dimensionless</t>
   </si>
   <si>
-    <t>Algorithm</t>
+    <t>Framework</t>
   </si>
   <si>
     <t>Evidence</t>
@@ -217,7 +217,7 @@
     <t>Metabolism</t>
   </si>
   <si>
-    <t>dfba</t>
+    <t>dynamic_flux_balance_analysis</t>
   </si>
   <si>
     <t>go: GO:0008152</t>
@@ -229,7 +229,7 @@
     <t>RNA degradation</t>
   </si>
   <si>
-    <t>ssa</t>
+    <t>stochastic_simulation_algorithm</t>
   </si>
   <si>
     <t>go: GO:0006401</t>
@@ -271,13 +271,13 @@
     <t>Cell</t>
   </si>
   <si>
-    <t>cellular</t>
-  </si>
-  <si>
-    <t>fluid</t>
-  </si>
-  <si>
-    <t>3d</t>
+    <t>cellular_compartment</t>
+  </si>
+  <si>
+    <t>fluid_compartment</t>
+  </si>
+  <si>
+    <t>3D_compartment</t>
   </si>
   <si>
     <t>e</t>
@@ -286,7 +286,7 @@
     <t>g</t>
   </si>
   <si>
-    <t>normal</t>
+    <t>normal_distribution</t>
   </si>
   <si>
     <t>l</t>
@@ -304,7 +304,7 @@
     <t>Extracellular space</t>
   </si>
   <si>
-    <t>extracellular</t>
+    <t>extracellular_compartment</t>
   </si>
   <si>
     <t>density_e</t>
@@ -461,7 +461,7 @@
     <t>C100H111N50O61P10</t>
   </si>
   <si>
-    <t>rna</t>
+    <t>RNA</t>
   </si>
   <si>
     <t>bp: Rna</t>
@@ -639,9 +639,6 @@
   </si>
   <si>
     <t>backward</t>
-  </si>
-  <si>
-    <t>other</t>
   </si>
   <si>
     <t>k_cat_atp_hyd_rev * atp[c] / (atp[c] + K_m_atp_hyd_rev * Avogadro * volume_c)</t>
@@ -850,12 +847,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="0.000E+00"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="0.000E+00"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -903,13 +900,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -926,11 +916,33 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -959,21 +971,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -987,6 +1000,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -994,45 +1014,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1053,13 +1050,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1071,7 +1074,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1083,25 +1092,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1119,7 +1110,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1131,91 +1218,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1227,13 +1230,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1282,6 +1279,17 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
@@ -1319,17 +1327,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1356,132 +1353,132 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1489,7 +1486,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1519,6 +1516,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2310,7 +2310,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J1" sqref="J1"/>
+      <selection pane="bottomRight" activeCell="E2" sqref="E2:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5"/>
@@ -2368,11 +2368,9 @@
       <c r="D2" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="8"/>
+      <c r="F2" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>182</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>167</v>
@@ -2380,19 +2378,17 @@
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>164</v>
       </c>
       <c r="D3" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>167</v>
@@ -2400,19 +2396,17 @@
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>168</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>181</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="E4" s="8"/>
       <c r="F4" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>167</v>
@@ -2420,19 +2414,17 @@
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>171</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>181</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="E5" s="8"/>
       <c r="F5" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>167</v>
@@ -2440,19 +2432,17 @@
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>174</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>181</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="E6" s="8"/>
       <c r="F6" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>167</v>
@@ -2506,10 +2496,10 @@
         <v>128</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>192</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>193</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
@@ -2529,7 +2519,7 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>38</v>
@@ -2589,7 +2579,7 @@
         <v>128</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>18</v>
@@ -2643,13 +2633,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>140</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>128</v>
@@ -2690,7 +2680,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1"/>
@@ -2709,10 +2699,10 @@
         <v>77</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>197</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>198</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>128</v>
@@ -2735,14 +2725,12 @@
     </row>
     <row r="2" customHeight="1" spans="1:11">
       <c r="A2" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>181</v>
-      </c>
+      <c r="C2" s="1"/>
       <c r="D2" s="1">
         <v>0.3</v>
       </c>
@@ -2750,15 +2738,15 @@
         <v>34</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:6">
       <c r="A3" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>203</v>
       </c>
       <c r="D3" s="1">
         <v>0.0003</v>
@@ -2769,10 +2757,10 @@
     </row>
     <row r="4" customHeight="1" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D4" s="1">
         <v>0.0003</v>
@@ -2783,24 +2771,24 @@
     </row>
     <row r="5" customHeight="1" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D6" s="1">
         <v>2000</v>
@@ -2811,24 +2799,24 @@
     </row>
     <row r="7" customHeight="1" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D7" s="1">
         <v>0.0003</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:6">
       <c r="A8" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>210</v>
       </c>
       <c r="D8" s="1">
         <v>0.001</v>
@@ -2839,10 +2827,10 @@
     </row>
     <row r="9" customHeight="1" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D9" s="1">
         <v>0.001</v>
@@ -2853,10 +2841,10 @@
     </row>
     <row r="10" customHeight="1" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D10" s="1">
         <v>0.01</v>
@@ -2869,42 +2857,33 @@
       <c r="A11" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>181</v>
-      </c>
       <c r="D11" s="1">
         <v>1100</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="12" customHeight="1" spans="1:6">
       <c r="A12" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>181</v>
-      </c>
       <c r="D12" s="1">
         <v>1000</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="13" customHeight="1" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>181</v>
+        <v>213</v>
       </c>
       <c r="D13" s="5">
         <v>6.02214075862e+23</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -2922,7 +2901,7 @@
   <sheetPr/>
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
@@ -3000,10 +2979,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>197</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>198</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>128</v>
@@ -3012,10 +2991,10 @@
         <v>77</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>216</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>217</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>29</v>
@@ -3030,22 +3009,22 @@
         <v>33</v>
       </c>
       <c r="M1" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>222</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>223</v>
       </c>
       <c r="S1" s="3" t="s">
         <v>18</v>
@@ -3099,10 +3078,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>197</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>198</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>128</v>
@@ -3111,7 +3090,7 @@
         <v>77</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>18</v>
@@ -3238,12 +3217,12 @@
   <sheetPr/>
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E18" sqref="E18"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2"/>
@@ -3259,46 +3238,46 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>226</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>227</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>77</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>235</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>236</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>18</v>
@@ -3309,66 +3288,66 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:16">
       <c r="A2" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>238</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>239</v>
       </c>
       <c r="F2" s="1">
         <v>2016</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>241</v>
       </c>
       <c r="K2" s="1">
         <v>44</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>242</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:16">
       <c r="A3" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>246</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>247</v>
       </c>
       <c r="F3" s="1">
         <v>2017</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>241</v>
       </c>
       <c r="K3" s="1">
         <v>45</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -3397,8 +3376,8 @@
     <col min="1" max="1" width="18.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="5.375" style="1" customWidth="1"/>
     <col min="3" max="1018" width="8.78333333333333" style="1"/>
-    <col min="1019" max="1019" width="8.78333333333333" style="13"/>
-    <col min="1020" max="16384" width="9" style="13"/>
+    <col min="1019" max="1019" width="8.78333333333333" style="14"/>
+    <col min="1020" max="16384" width="9" style="14"/>
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:2">
@@ -3477,7 +3456,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="7"/>
@@ -3559,7 +3538,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="O1" sqref="O1"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2"/>
@@ -3568,7 +3547,7 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.1" customHeight="1" spans="1:17">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -3725,7 +3704,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J1" sqref="J1"/>
+      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -3798,7 +3777,7 @@
       <c r="H2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="K2" s="11"/>
+      <c r="K2" s="12"/>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:11">
       <c r="A3" s="1" t="s">
@@ -3825,7 +3804,7 @@
       <c r="H3" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="K3" s="11"/>
+      <c r="K3" s="12"/>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:11">
       <c r="A4" s="1" t="s">
@@ -3852,7 +3831,7 @@
       <c r="H4" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="K4" s="11"/>
+      <c r="K4" s="12"/>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:11">
       <c r="A5" s="1" t="s">
@@ -3876,7 +3855,7 @@
       <c r="G5" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="K5" s="11"/>
+      <c r="K5" s="12"/>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:11">
       <c r="A6" s="1" t="s">
@@ -3903,7 +3882,7 @@
       <c r="H6" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="K6" s="11"/>
+      <c r="K6" s="12"/>
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:8">
       <c r="A7" s="1" t="s">
@@ -4022,12 +4001,12 @@
       <c r="F11" s="1">
         <v>-8</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:L11">
@@ -4260,7 +4239,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J1" sqref="J1"/>
+      <selection pane="bottomRight" activeCell="D8" sqref="D2:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7"/>
@@ -4314,16 +4293,16 @@
       <c r="C2" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E2" s="12">
         <v>0.005</v>
       </c>
       <c r="F2" s="1">
         <v>0.0121655250605964</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="12" t="s">
         <v>145</v>
       </c>
     </row>
@@ -4334,19 +4313,19 @@
       <c r="C3" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="12">
         <v>0.005</v>
       </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11" t="s">
+      <c r="F3" s="12"/>
+      <c r="G3" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:10">
       <c r="A4" s="1" t="s">
@@ -4355,19 +4334,19 @@
       <c r="C4" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="12">
         <v>0.005</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11" t="s">
+      <c r="F4" s="12"/>
+      <c r="G4" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:10">
       <c r="A5" s="1" t="s">
@@ -4376,19 +4355,19 @@
       <c r="C5" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="12">
         <v>0.01</v>
       </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11" t="s">
+      <c r="F5" s="12"/>
+      <c r="G5" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:10">
       <c r="A6" s="1" t="s">
@@ -4397,19 +4376,19 @@
       <c r="C6" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="11" t="s">
         <v>63</v>
       </c>
       <c r="E6" s="1">
         <v>1e-7</v>
       </c>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11" t="s">
+      <c r="F6" s="12"/>
+      <c r="G6" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:10">
       <c r="A7" s="1" t="s">
@@ -4418,19 +4397,19 @@
       <c r="C7" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="12">
         <v>55</v>
       </c>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11" t="s">
+      <c r="F7" s="12"/>
+      <c r="G7" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
     </row>
     <row r="8" ht="15.1" customHeight="1" spans="1:10">
       <c r="A8" s="1" t="s">
@@ -4439,19 +4418,19 @@
       <c r="C8" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="11" t="s">
         <v>63</v>
       </c>
       <c r="E8" s="5">
         <v>0.005</v>
       </c>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11" t="s">
+      <c r="F8" s="12"/>
+      <c r="G8" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
     </row>
   </sheetData>
   <autoFilter ref="C1:L8">

</xml_diff>

<commit_message>
updating for refactoring wc_lang units
</commit_message>
<xml_diff>
--- a/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
+++ b/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="14070" tabRatio="993" firstSheet="6" activeTab="19"/>
+    <workbookView windowWidth="20295" windowHeight="6840" tabRatio="993" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -190,7 +190,7 @@
     <t>Temperature units</t>
   </si>
   <si>
-    <t>C</t>
+    <t>degC</t>
   </si>
   <si>
     <t>pH</t>
@@ -847,10 +847,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
+    <numFmt numFmtId="176" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="0.000E+00"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
@@ -900,9 +900,8 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -917,22 +916,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -946,6 +938,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -954,9 +953,52 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -971,55 +1013,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -1027,9 +1027,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1050,19 +1050,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1074,31 +1140,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1110,91 +1176,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1212,25 +1194,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1253,46 +1253,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1312,6 +1277,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1323,6 +1297,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1350,135 +1339,146 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2730,7 +2730,6 @@
       <c r="B2" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="C2" s="1"/>
       <c r="D2" s="1">
         <v>0.3</v>
       </c>
@@ -3217,7 +3216,7 @@
   <sheetPr/>
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
@@ -3365,10 +3364,10 @@
   <sheetPr/>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="A6" sqref="A6:B6"/>
+      <selection pane="topRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelCol="1"/>

</xml_diff>

<commit_message>
updating for wc_lang provenance
</commit_message>
<xml_diff>
--- a/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
+++ b/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="20295" windowHeight="6840" tabRatio="993" activeTab="2"/>
+    <workbookView windowWidth="28695" windowHeight="13965" tabRatio="993" firstSheet="6" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -28,9 +28,12 @@
     <sheet name="Evidence" sheetId="17" r:id="rId18"/>
     <sheet name="Interpretations" sheetId="20" r:id="rId19"/>
     <sheet name="References" sheetId="18" r:id="rId20"/>
+    <sheet name="Authors" sheetId="21" r:id="rId21"/>
+    <sheet name="Changes" sheetId="22" r:id="rId22"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId21"/>
+    <externalReference r:id="rId23"/>
+    <externalReference r:id="rId24"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Compartments!$A$1:$G$3</definedName>
@@ -89,13 +92,14 @@
     <definedName name="_FilterDatabase_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="Id">'[2]Rate laws'!$A:$A</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="262">
   <si>
     <t>Id</t>
   </si>
@@ -134,15 +138,6 @@
   </si>
   <si>
     <t>wc_lang version</t>
-  </si>
-  <si>
-    <t>Author</t>
-  </si>
-  <si>
-    <t>Author organization</t>
-  </si>
-  <si>
-    <t>Author email</t>
   </si>
   <si>
     <t>Time units</t>
@@ -773,6 +768,9 @@
     <t>Title</t>
   </si>
   <si>
+    <t>Author</t>
+  </si>
+  <si>
     <t>Editor</t>
   </si>
   <si>
@@ -840,6 +838,54 @@
   </si>
   <si>
     <t>D37-D42</t>
+  </si>
+  <si>
+    <t>Last name</t>
+  </si>
+  <si>
+    <t>First name</t>
+  </si>
+  <si>
+    <t>Middle name</t>
+  </si>
+  <si>
+    <t>Organization</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>ORCID</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>Target type</t>
+  </si>
+  <si>
+    <t>Reason</t>
+  </si>
+  <si>
+    <t>Reason type</t>
+  </si>
+  <si>
+    <t>Intention</t>
+  </si>
+  <si>
+    <t>Intention type</t>
+  </si>
+  <si>
+    <t>Authors</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -847,11 +893,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="176" formatCode="0.000E+00"/>
+    <numFmt numFmtId="177" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="0.000E+00"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="25">
@@ -895,23 +941,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -922,9 +964,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -939,7 +985,45 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -967,38 +1051,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1013,23 +1067,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1050,25 +1096,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1080,7 +1138,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1098,7 +1156,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1110,127 +1276,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1262,6 +1308,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1273,6 +1334,32 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1301,36 +1388,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1339,149 +1396,138 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1515,13 +1561,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1667,6 +1713,61 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Model"/>
+      <sheetName val="Taxon"/>
+      <sheetName val="Environment"/>
+      <sheetName val="Submodels"/>
+      <sheetName val="Compartments"/>
+      <sheetName val="Species types"/>
+      <sheetName val="Species"/>
+      <sheetName val="Initial species concentrations"/>
+      <sheetName val="Observables"/>
+      <sheetName val="Functions"/>
+      <sheetName val="Reactions"/>
+      <sheetName val="Rate laws"/>
+      <sheetName val="dFBA objectives"/>
+      <sheetName val="dFBA objective reactions"/>
+      <sheetName val="dFBA objective species"/>
+      <sheetName val="Parameters"/>
+      <sheetName val="Stop conditions"/>
+      <sheetName val="Evidence"/>
+      <sheetName val="Interpretations"/>
+      <sheetName val="References"/>
+      <sheetName val="Authors"/>
+      <sheetName val="Changes"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1930,12 +2031,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="F6" sqref="F6"/>
+      <selection pane="topRight" activeCell="A8" sqref="$A8:$XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="1"/>
@@ -2003,46 +2104,28 @@
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B8"/>
-    </row>
-    <row r="9" ht="15.1" customHeight="1" spans="1:2">
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" ht="15.1" customHeight="1" spans="1:1">
       <c r="A9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9"/>
-    </row>
-    <row r="10" ht="15.1" customHeight="1" spans="1:2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" ht="15.1" customHeight="1" spans="1:1">
       <c r="A10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10"/>
-    </row>
-    <row r="11" ht="15.1" customHeight="1" spans="1:2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" ht="15.1" customHeight="1" spans="1:1">
       <c r="A11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" ht="15.1" customHeight="1" spans="1:1">
       <c r="A12" s="2" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="13" ht="15.1" customHeight="1" spans="1:1">
-      <c r="A13" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" ht="15.1" customHeight="1" spans="1:1">
-      <c r="A14" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" ht="15.1" customHeight="1" spans="1:1">
-      <c r="A15" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -2083,47 +2166,47 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -2166,60 +2249,60 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>163</v>
-      </c>
       <c r="J1" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E2" s="8">
         <v>1</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
@@ -2227,22 +2310,22 @@
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E3" s="8">
         <v>0</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
@@ -2250,44 +2333,44 @@
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E4" s="8">
         <v>0</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E5" s="1">
         <v>0</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -2328,124 +2411,124 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -2487,54 +2570,54 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -2573,28 +2656,28 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -2633,31 +2716,31 @@
         <v>2</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -2696,193 +2779,193 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:11">
       <c r="A2" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D2" s="1">
         <v>0.3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D3" s="1">
         <v>0.0003</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D4" s="1">
         <v>0.0003</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D6" s="1">
         <v>2000</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D7" s="1">
         <v>0.0003</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D8" s="1">
         <v>0.001</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D9" s="1">
         <v>0.001</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" customHeight="1" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D10" s="1">
         <v>0.01</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" customHeight="1" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D11" s="1">
         <v>1100</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="12" customHeight="1" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D12" s="1">
         <v>1000</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="13" customHeight="1" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D13" s="5">
         <v>6.02214075862e+23</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -2921,25 +3004,25 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -2978,64 +3061,64 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="L1" s="3" t="s">
+      <c r="P1" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="T1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="M1" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="U1" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -3077,31 +3160,31 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="3:4">
@@ -3167,7 +3250,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:2">
@@ -3175,33 +3258,33 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:1">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:1">
       <c r="A6" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -3237,116 +3320,116 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>235</v>
-      </c>
       <c r="Q1" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:16">
       <c r="A2" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>236</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>238</v>
       </c>
       <c r="F2" s="1">
         <v>2016</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="K2" s="1">
         <v>44</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:16">
       <c r="A3" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>244</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>246</v>
       </c>
       <c r="F3" s="1">
         <v>2017</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="K3" s="1">
         <v>45</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -3359,12 +3442,151 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:M1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1"/>
+  <cols>
+    <col min="1" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customHeight="1" spans="1:13">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:P1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1"/>
+  <cols>
+    <col min="1" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customHeight="1" spans="1:16">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection/>
       <selection pane="topRight" activeCell="B5" sqref="B5"/>
@@ -3384,7 +3606,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:1">
@@ -3394,7 +3616,7 @@
     </row>
     <row r="3" customHeight="1" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B3" s="1">
         <v>37</v>
@@ -3402,15 +3624,15 @@
     </row>
     <row r="4" customHeight="1" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B5" s="1">
         <v>7.75</v>
@@ -3418,25 +3640,25 @@
     </row>
     <row r="6" customHeight="1" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:1">
       <c r="A7" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:1">
       <c r="A8" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="1:1">
       <c r="A9" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -3474,50 +3696,50 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:4">
       <c r="A2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:4">
       <c r="A3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -3553,75 +3775,75 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="M1" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:16">
       <c r="A2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="I2" s="5">
         <v>4.58e-17</v>
@@ -3630,39 +3852,39 @@
         <v>4.58e-18</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:16">
       <c r="A3" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="I3" s="1">
         <v>1</v>
@@ -3671,16 +3893,16 @@
         <v>0</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -3721,48 +3943,48 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="H1" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:11">
       <c r="A2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="E2" s="1">
         <v>424.1773</v>
@@ -3771,25 +3993,25 @@
         <v>-3</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="K2" s="12"/>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:11">
       <c r="A3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="E3" s="1">
         <v>345.2053</v>
@@ -3798,25 +4020,25 @@
         <v>-2</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="K3" s="12"/>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:11">
       <c r="A4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="E4" s="1">
         <v>503.14946</v>
@@ -3825,25 +4047,25 @@
         <v>-4</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="K4" s="12"/>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:11">
       <c r="A5" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="E5" s="1">
         <v>180.15588</v>
@@ -3852,22 +4074,22 @@
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K5" s="12"/>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:11">
       <c r="A6" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="E6" s="1">
         <v>1.00783</v>
@@ -3876,25 +4098,25 @@
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="K6" s="12"/>
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:8">
       <c r="A7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="E7" s="1">
         <v>18.0153</v>
@@ -3903,24 +4125,24 @@
         <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" ht="15.1" customHeight="1" spans="1:8">
       <c r="A8" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="E8" s="1">
         <v>95.9793</v>
@@ -3929,24 +4151,24 @@
         <v>-2</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" ht="15.1" customHeight="1" spans="1:7">
       <c r="A9" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="E9" s="1">
         <v>174.95</v>
@@ -3955,21 +4177,21 @@
         <v>-4</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" ht="15.1" customHeight="1" spans="1:8">
       <c r="A10" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>120</v>
       </c>
       <c r="E10" s="1">
         <v>3298.98577</v>
@@ -3978,21 +4200,21 @@
         <v>-11</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" ht="15.1" customHeight="1" spans="1:10">
       <c r="A11" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E11" s="1">
         <v>1042.32919</v>
@@ -4001,7 +4223,7 @@
         <v>-8</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
@@ -4044,178 +4266,178 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" ht="15.1" customHeight="1" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" ht="15.1" customHeight="1" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" ht="15.1" customHeight="1" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" ht="15.1" customHeight="1" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -4255,45 +4477,45 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>143</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E2" s="12">
         <v>0.005</v>
@@ -4302,25 +4524,25 @@
         <v>0.0121655250605964</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E3" s="12">
         <v>0.005</v>
       </c>
       <c r="F3" s="12"/>
       <c r="G3" s="12" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
@@ -4328,20 +4550,20 @@
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E4" s="12">
         <v>0.005</v>
       </c>
       <c r="F4" s="12"/>
       <c r="G4" s="12" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
@@ -4349,20 +4571,20 @@
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E5" s="12">
         <v>0.01</v>
       </c>
       <c r="F5" s="12"/>
       <c r="G5" s="12" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
@@ -4370,20 +4592,20 @@
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:10">
       <c r="A6" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E6" s="1">
         <v>1e-7</v>
       </c>
       <c r="F6" s="12"/>
       <c r="G6" s="12" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
@@ -4391,20 +4613,20 @@
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:10">
       <c r="A7" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E7" s="12">
         <v>55</v>
       </c>
       <c r="F7" s="12"/>
       <c r="G7" s="12" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
@@ -4412,20 +4634,20 @@
     </row>
     <row r="8" ht="15.1" customHeight="1" spans="1:10">
       <c r="A8" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E8" s="5">
         <v>0.005</v>
       </c>
       <c r="F8" s="12"/>
       <c r="G8" s="12" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
@@ -4467,25 +4689,25 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating for changes to wc-lang
</commit_message>
<xml_diff>
--- a/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
+++ b/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13965" tabRatio="993" firstSheet="7" activeTab="18"/>
+    <workbookView windowWidth="20295" windowHeight="6945" tabRatio="993" firstSheet="13" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="Table of contents" sheetId="23" r:id="rId1"/>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="279">
   <si>
     <t>Table</t>
   </si>
@@ -223,7 +223,7 @@
     <t>s</t>
   </si>
   <si>
-    <t>Database references</t>
+    <t>Identifiers</t>
   </si>
   <si>
     <t>Comments</t>
@@ -915,9 +915,6 @@
   </si>
   <si>
     <t>Address</t>
-  </si>
-  <si>
-    <t>ORCID</t>
   </si>
   <si>
     <t>Target</t>
@@ -949,12 +946,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="0.000E+00"/>
+    <numFmt numFmtId="176" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="177" formatCode="0.000E+00"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -1023,17 +1020,18 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1046,7 +1044,7 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1054,7 +1052,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1077,7 +1075,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1092,6 +1090,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1099,22 +1104,8 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1129,7 +1120,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1142,11 +1140,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1171,7 +1168,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1183,19 +1288,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1207,49 +1324,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1261,97 +1342,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1374,17 +1371,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1415,9 +1406,41 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1439,167 +1462,141 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1648,13 +1645,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5398,12 +5395,12 @@
   <sheetPr/>
   <dimension ref="A1:AMS2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A1" sqref="$A1:$XFD2"/>
+      <selection pane="bottomRight" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
@@ -5885,14 +5882,14 @@
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1"/>
@@ -5900,7 +5897,7 @@
     <col min="1" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:13">
+    <row r="1" customHeight="1" spans="1:12">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -5932,12 +5929,9 @@
         <v>270</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>271</v>
+        <v>40</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="M1" s="2" t="s">
         <v>41</v>
       </c>
     </row>
@@ -5976,25 +5970,25 @@
         <v>97</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>277</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>278</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>40</v>
@@ -6015,7 +6009,7 @@
         <v>23</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
moving pH from Environment to Compartment
</commit_message>
<xml_diff>
--- a/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
+++ b/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="20295" windowHeight="6945" tabRatio="993" firstSheet="13" activeTab="21"/>
+    <workbookView windowWidth="20295" windowHeight="6840" tabRatio="993" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Table of contents" sheetId="23" r:id="rId1"/>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="283">
   <si>
     <t>Table</t>
   </si>
@@ -262,103 +262,103 @@
     <t>degC</t>
   </si>
   <si>
+    <t>Framework</t>
+  </si>
+  <si>
+    <t>metabolism</t>
+  </si>
+  <si>
+    <t>Metabolism</t>
+  </si>
+  <si>
+    <t>dynamic_flux_balance_analysis</t>
+  </si>
+  <si>
+    <t>go: GO:0008152</t>
+  </si>
+  <si>
+    <t>rna_degradation</t>
+  </si>
+  <si>
+    <t>RNA degradation</t>
+  </si>
+  <si>
+    <t>stochastic_simulation_algorithm</t>
+  </si>
+  <si>
+    <t>go: GO:0006401</t>
+  </si>
+  <si>
+    <t>Initial volume</t>
+  </si>
+  <si>
     <t>pH</t>
   </si>
   <si>
+    <t>Biological type</t>
+  </si>
+  <si>
+    <t>Physical type</t>
+  </si>
+  <si>
+    <t>Geometry</t>
+  </si>
+  <si>
+    <t>Parent compartment</t>
+  </si>
+  <si>
+    <t>Mass units</t>
+  </si>
+  <si>
+    <t>Volume distribution</t>
+  </si>
+  <si>
+    <t>Volume mean</t>
+  </si>
+  <si>
+    <t>Volume standard deviation</t>
+  </si>
+  <si>
+    <t>Volume units</t>
+  </si>
+  <si>
+    <t>Initial density</t>
+  </si>
+  <si>
     <t>pH units</t>
   </si>
   <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>Cell</t>
+  </si>
+  <si>
+    <t>cellular_compartment</t>
+  </si>
+  <si>
+    <t>fluid_compartment</t>
+  </si>
+  <si>
+    <t>3D_compartment</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>normal_distribution</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>density_c</t>
+  </si>
+  <si>
     <t>dimensionless</t>
-  </si>
-  <si>
-    <t>Framework</t>
-  </si>
-  <si>
-    <t>metabolism</t>
-  </si>
-  <si>
-    <t>Metabolism</t>
-  </si>
-  <si>
-    <t>dynamic_flux_balance_analysis</t>
-  </si>
-  <si>
-    <t>go: GO:0008152</t>
-  </si>
-  <si>
-    <t>rna_degradation</t>
-  </si>
-  <si>
-    <t>RNA degradation</t>
-  </si>
-  <si>
-    <t>stochastic_simulation_algorithm</t>
-  </si>
-  <si>
-    <t>go: GO:0006401</t>
-  </si>
-  <si>
-    <t>Initial volume</t>
-  </si>
-  <si>
-    <t>Biological type</t>
-  </si>
-  <si>
-    <t>Physical type</t>
-  </si>
-  <si>
-    <t>Geometry</t>
-  </si>
-  <si>
-    <t>Parent compartment</t>
-  </si>
-  <si>
-    <t>Mass units</t>
-  </si>
-  <si>
-    <t>Distribution</t>
-  </si>
-  <si>
-    <t>Mean</t>
-  </si>
-  <si>
-    <t>Standard deviation</t>
-  </si>
-  <si>
-    <t>Units</t>
-  </si>
-  <si>
-    <t>Initial density</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>Cell</t>
-  </si>
-  <si>
-    <t>cellular_compartment</t>
-  </si>
-  <si>
-    <t>fluid_compartment</t>
-  </si>
-  <si>
-    <t>3D_compartment</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>normal_distribution</t>
-  </si>
-  <si>
-    <t>l</t>
-  </si>
-  <si>
-    <t>density_c</t>
   </si>
   <si>
     <t>cco: CCO-CYTOPLASM</t>
@@ -548,6 +548,9 @@
     <t>Compartment</t>
   </si>
   <si>
+    <t>Units</t>
+  </si>
+  <si>
     <t>adp[c]</t>
   </si>
   <si>
@@ -579,6 +582,15 @@
   </si>
   <si>
     <t>rna_dec_a[c]</t>
+  </si>
+  <si>
+    <t>Distribution</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Standard deviation</t>
   </si>
   <si>
     <t>dist-init-conc-adp[c]</t>
@@ -947,11 +959,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
     <numFmt numFmtId="176" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="177" formatCode="0.000E+00"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="0.000E+00"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -1006,17 +1018,32 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -1024,6 +1051,50 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1037,25 +1108,9 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1067,15 +1122,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1090,51 +1146,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1168,19 +1180,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1198,13 +1210,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1216,43 +1276,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1264,13 +1288,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1282,61 +1342,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1348,7 +1354,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1371,6 +1383,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1380,11 +1407,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1406,26 +1439,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1445,17 +1461,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1471,136 +1483,136 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1814,6 +1826,7 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
+      <sheetName val="Table of contents"/>
       <sheetName val="Model"/>
       <sheetName val="Taxon"/>
       <sheetName val="Environment"/>
@@ -1860,6 +1873,7 @@
       <sheetData sheetId="19"/>
       <sheetData sheetId="20"/>
       <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2406,10 +2420,10 @@
         <v>27</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>74</v>
+        <v>148</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>40</v>
@@ -2465,10 +2479,10 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>74</v>
+        <v>148</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>40</v>
@@ -2488,24 +2502,24 @@
     </row>
     <row r="2" customHeight="1" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -2548,7 +2562,7 @@
       <c r="E1" s="11"/>
       <c r="F1" s="11"/>
       <c r="G1" s="13" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="H1" s="13"/>
       <c r="I1" s="13"/>
@@ -3579,25 +3593,25 @@
         <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>74</v>
+        <v>148</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>40</v>
@@ -4630,22 +4644,22 @@
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="E3" s="10">
         <v>1</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
@@ -4653,22 +4667,22 @@
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E4" s="10">
         <v>0</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
@@ -4676,44 +4690,44 @@
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="E5" s="10">
         <v>0</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="E6" s="1">
         <v>0</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -4757,19 +4771,19 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>97</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>74</v>
+        <v>148</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>40</v>
@@ -4789,92 +4803,92 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="1" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="1" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="E4" s="10"/>
       <c r="F4" s="1" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:7">
       <c r="A5" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>202</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>198</v>
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="1" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="1" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -4910,7 +4924,7 @@
   <sheetData>
     <row r="1" spans="4:5">
       <c r="D1" s="8" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="E1" s="8"/>
     </row>
@@ -4922,19 +4936,19 @@
         <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>74</v>
+        <v>148</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>40</v>
@@ -4954,19 +4968,19 @@
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>39</v>
@@ -5011,13 +5025,13 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>74</v>
+        <v>148</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>40</v>
@@ -5071,16 +5085,16 @@
         <v>27</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>74</v>
+        <v>148</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>40</v>
@@ -5137,13 +5151,13 @@
         <v>97</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>74</v>
+        <v>148</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>40</v>
@@ -5163,142 +5177,142 @@
     </row>
     <row r="2" customHeight="1" spans="1:11">
       <c r="A2" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="D2" s="1">
         <v>0.3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="D3" s="1">
         <v>0.0003</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="D4" s="1">
         <v>0.0003</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:6">
       <c r="A6" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>217</v>
       </c>
       <c r="D6" s="1">
         <v>2000</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="D7" s="1">
         <v>0.0003</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="D8" s="1">
         <v>0.001</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="D9" s="1">
         <v>0.001</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" customHeight="1" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="D10" s="1">
         <v>0.01</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" customHeight="1" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D11" s="1">
         <v>1100</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
     </row>
     <row r="12" customHeight="1" spans="1:6">
@@ -5309,18 +5323,18 @@
         <v>1000</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
     </row>
     <row r="13" customHeight="1" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="D13" s="6">
         <v>6.02214075862e+23</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -5359,10 +5373,10 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>74</v>
+        <v>148</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>40</v>
@@ -5410,7 +5424,7 @@
   <sheetData>
     <row r="1" ht="15" customHeight="1" spans="7:1033">
       <c r="G1" s="5" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="H1" s="5"/>
       <c r="I1" s="5" t="s">
@@ -5438,13 +5452,13 @@
         <v>27</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>74</v>
+        <v>148</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>97</v>
@@ -5453,7 +5467,7 @@
         <v>4</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>50</v>
@@ -5462,28 +5476,28 @@
         <v>51</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>40</v>
@@ -5659,19 +5673,19 @@
         <v>27</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>74</v>
+        <v>148</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>97</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>40</v>
@@ -5757,46 +5771,46 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>97</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>40</v>
@@ -5807,66 +5821,66 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:16">
       <c r="A2" s="1" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="F2" s="1">
         <v>2016</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="K2" s="1">
         <v>44</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:16">
       <c r="A3" s="1" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="F3" s="1">
         <v>2017</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="K3" s="1">
         <v>45</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -5884,12 +5898,12 @@
   <sheetPr/>
   <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M18" sqref="M18"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1"/>
@@ -5905,28 +5919,28 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>40</v>
@@ -5970,25 +5984,25 @@
         <v>97</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>40</v>
@@ -6009,7 +6023,7 @@
         <v>23</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -6086,15 +6100,15 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="B5" sqref="B5"/>
+      <selection pane="topRight" activeCell="B5" sqref="$A5:$XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelRow="6" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="18.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="5.375" style="1" customWidth="1"/>
@@ -6132,34 +6146,18 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" customHeight="1" spans="1:2">
+    <row r="5" customHeight="1" spans="1:1">
       <c r="A5" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" s="1">
-        <v>7.75</v>
-      </c>
-    </row>
-    <row r="6" customHeight="1" spans="1:2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" customHeight="1" spans="1:1">
       <c r="A6" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:1">
       <c r="A7" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" customHeight="1" spans="1:1">
-      <c r="A8" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" customHeight="1" spans="1:1">
-      <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -6198,7 +6196,7 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>40</v>
@@ -6218,30 +6216,30 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:4">
       <c r="A2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:4">
       <c r="A3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -6254,22 +6252,22 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AMQ4"/>
+  <dimension ref="A1:AMS4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A1" sqref="$A1:$XFD2"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3"/>
   <cols>
-    <col min="1" max="1031" width="8.78333333333333" style="1"/>
+    <col min="1" max="1033" width="8.78333333333333" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" spans="1:1031">
+    <row r="1" ht="15" customHeight="1" spans="1:1033">
       <c r="A1" s="11"/>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -6278,14 +6276,16 @@
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
       <c r="H1" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I1" s="8"/>
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
       <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
+      <c r="M1" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="N1" s="8"/>
       <c r="O1" s="11"/>
       <c r="P1" s="11"/>
       <c r="Q1" s="11"/>
@@ -7300,11 +7300,13 @@
       <c r="AML1" s="11"/>
       <c r="AMM1" s="11"/>
       <c r="AMN1" s="11"/>
-      <c r="AMO1"/>
-      <c r="AMP1"/>
+      <c r="AMO1" s="11"/>
+      <c r="AMP1" s="11"/>
       <c r="AMQ1"/>
-    </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:1031">
+      <c r="AMR1"/>
+      <c r="AMS1"/>
+    </row>
+    <row r="2" ht="15.1" customHeight="1" spans="1:1033">
       <c r="A2" s="17" t="s">
         <v>25</v>
       </c>
@@ -7312,52 +7314,56 @@
         <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="M2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
       <c r="T2" s="11"/>
       <c r="U2" s="11"/>
       <c r="V2" s="11"/>
@@ -8367,34 +8373,36 @@
       <c r="AML2" s="11"/>
       <c r="AMM2" s="11"/>
       <c r="AMN2" s="11"/>
-      <c r="AMO2"/>
-      <c r="AMP2"/>
+      <c r="AMO2" s="11"/>
+      <c r="AMP2" s="11"/>
       <c r="AMQ2"/>
-    </row>
-    <row r="3" ht="15.1" customHeight="1" spans="1:16">
+      <c r="AMR2"/>
+      <c r="AMS2"/>
+    </row>
+    <row r="3" ht="15.1" customHeight="1" spans="1:18">
       <c r="A3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="I3" s="6">
         <v>4.58e-17</v>
@@ -8403,21 +8411,27 @@
         <v>4.58e-18</v>
       </c>
       <c r="K3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1">
+        <v>7.75</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="4" ht="15.1" customHeight="1" spans="1:16">
+    <row r="4" ht="15.1" customHeight="1" spans="1:18">
       <c r="A4" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>88</v>
@@ -8426,16 +8440,16 @@
         <v>89</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="G4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="I4" s="1">
         <v>1</v>
@@ -8444,15 +8458,21 @@
         <v>0</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="M4" s="1">
+        <v>7.75</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>92</v>
       </c>
     </row>
@@ -8460,8 +8480,9 @@
   <autoFilter ref="A2:G4">
     <extLst/>
   </autoFilter>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="H1:K1"/>
+    <mergeCell ref="M1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -8826,7 +8847,7 @@
         <v>147</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>74</v>
+        <v>148</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>40</v>
@@ -8846,152 +8867,152 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="1" t="s">
         <v>98</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B3" s="14"/>
       <c r="C3" s="1" t="s">
         <v>104</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B4" s="14"/>
       <c r="C4" s="1" t="s">
         <v>109</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B5" s="14"/>
       <c r="C5" s="1" t="s">
         <v>143</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B6" s="14"/>
       <c r="C6" s="1" t="s">
         <v>114</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B7" s="14"/>
       <c r="C7" s="1" t="s">
         <v>114</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" ht="15.1" customHeight="1" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B8" s="14"/>
       <c r="C8" s="1" t="s">
         <v>118</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" ht="15.1" customHeight="1" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B9" s="14"/>
       <c r="C9" s="1" t="s">
         <v>123</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" ht="15.1" customHeight="1" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B10" s="14"/>
       <c r="C10" s="1" t="s">
         <v>128</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" ht="15.1" customHeight="1" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B11" s="14"/>
       <c r="C11" s="1" t="s">
         <v>137</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -9034,16 +9055,16 @@
         <v>9</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>71</v>
+        <v>160</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>72</v>
+        <v>161</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>73</v>
+        <v>162</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>74</v>
+        <v>148</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>40</v>
@@ -9063,13 +9084,13 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E2" s="16">
         <v>0.005</v>
@@ -9078,25 +9099,25 @@
         <v>0.0121655250605964</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E3" s="16">
         <v>0.005</v>
       </c>
       <c r="F3" s="16"/>
       <c r="G3" s="16" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
@@ -9104,20 +9125,20 @@
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E4" s="16">
         <v>0.005</v>
       </c>
       <c r="F4" s="16"/>
       <c r="G4" s="16" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="H4" s="16"/>
       <c r="I4" s="16"/>
@@ -9125,20 +9146,20 @@
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E5" s="16">
         <v>0.01</v>
       </c>
       <c r="F5" s="16"/>
       <c r="G5" s="16" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="H5" s="16"/>
       <c r="I5" s="16"/>
@@ -9146,20 +9167,20 @@
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:10">
       <c r="A6" s="1" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E6" s="1">
         <v>1e-7</v>
       </c>
       <c r="F6" s="16"/>
       <c r="G6" s="16" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="H6" s="16"/>
       <c r="I6" s="16"/>
@@ -9167,20 +9188,20 @@
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:10">
       <c r="A7" s="1" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E7" s="16">
         <v>55</v>
       </c>
       <c r="F7" s="16"/>
       <c r="G7" s="16" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="H7" s="16"/>
       <c r="I7" s="16"/>
@@ -9188,20 +9209,20 @@
     </row>
     <row r="8" ht="15.1" customHeight="1" spans="1:10">
       <c r="A8" s="1" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E8" s="6">
         <v>0.005</v>
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="16" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="H8" s="16"/>
       <c r="I8" s="16"/>

</xml_diff>

<commit_message>
updating for wc_lang provenance changes
</commit_message>
<xml_diff>
--- a/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
+++ b/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="20295" windowHeight="6945" tabRatio="993" activeTab="6"/>
+    <workbookView windowWidth="28695" windowHeight="14070" tabRatio="993" firstSheet="9" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Table of contents" sheetId="23" r:id="rId1"/>
@@ -26,25 +26,26 @@
     <sheet name="dFBA objective species" sheetId="14" r:id="rId16"/>
     <sheet name="Parameters" sheetId="15" r:id="rId17"/>
     <sheet name="Stop conditions" sheetId="16" r:id="rId18"/>
-    <sheet name="Evidence" sheetId="17" r:id="rId19"/>
-    <sheet name="Interpretations" sheetId="20" r:id="rId20"/>
-    <sheet name="References" sheetId="18" r:id="rId21"/>
-    <sheet name="Authors" sheetId="21" r:id="rId22"/>
-    <sheet name="Changes" sheetId="22" r:id="rId23"/>
+    <sheet name="Observations" sheetId="17" r:id="rId19"/>
+    <sheet name="Observation sets" sheetId="24" r:id="rId20"/>
+    <sheet name="Conclusions" sheetId="20" r:id="rId21"/>
+    <sheet name="References" sheetId="18" r:id="rId22"/>
+    <sheet name="Authors" sheetId="21" r:id="rId23"/>
+    <sheet name="Changes" sheetId="22" r:id="rId24"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId24"/>
     <externalReference r:id="rId25"/>
+    <externalReference r:id="rId26"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Table of contents'!$A$1:$C$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Table of contents'!$A$1:$C$24</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Compartments!$A$2:$G$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Species types'!$A$2:$N$12</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Initial species concentrations'!$C$1:$L$8</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Reactions!$A$2:$D$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'Rate laws'!$C$1:$H$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">Parameters!$A$1:$F$13</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">References!$A$1:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">References!$A$1:$D$3</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="4">Submodels!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4">Submodels!$A$1:$H$3</definedName>
     <definedName name="excel_is_bugging_me" localSheetId="5">Compartments!$A$2:$G$4</definedName>
@@ -87,13 +88,13 @@
     <definedName name="_FilterDatabase_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
-    <definedName name="excel_is_bugging_me" localSheetId="20">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="20">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
+    <definedName name="excel_is_bugging_me" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
     <definedName name="Id">'[2]Rate laws'!$A:$A</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
@@ -101,7 +102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="286">
   <si>
     <t>Table</t>
   </si>
@@ -163,108 +164,114 @@
     <t>Stop conditions</t>
   </si>
   <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>Observation sets</t>
+  </si>
+  <si>
+    <t>Conclusions</t>
+  </si>
+  <si>
+    <t>References</t>
+  </si>
+  <si>
+    <t>Authors</t>
+  </si>
+  <si>
+    <t>Changes</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>wc_lang_tutorial_model</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>wc_lang tutorial model</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>0.0.1</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>https://github.com/org/repo</t>
+  </si>
+  <si>
+    <t>Branch</t>
+  </si>
+  <si>
+    <t>master</t>
+  </si>
+  <si>
+    <t>Revision</t>
+  </si>
+  <si>
+    <t>hash</t>
+  </si>
+  <si>
+    <t>wc_lang version</t>
+  </si>
+  <si>
+    <t>Time units</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>Identifiers</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Created</t>
+  </si>
+  <si>
+    <t>Updated</t>
+  </si>
+  <si>
+    <t>taxon</t>
+  </si>
+  <si>
+    <t>Mycoplasma pneumoniae M129</t>
+  </si>
+  <si>
+    <t>Rank</t>
+  </si>
+  <si>
+    <t>variety</t>
+  </si>
+  <si>
+    <t>taxonomy: 272634</t>
+  </si>
+  <si>
+    <t>env</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>Temperature units</t>
+  </si>
+  <si>
+    <t>degC</t>
+  </si>
+  <si>
+    <t>Framework</t>
+  </si>
+  <si>
     <t>Evidence</t>
   </si>
   <si>
-    <t>Interpretations</t>
-  </si>
-  <si>
-    <t>References</t>
-  </si>
-  <si>
-    <t>Authors</t>
-  </si>
-  <si>
-    <t>Changes</t>
-  </si>
-  <si>
-    <t>Id</t>
-  </si>
-  <si>
-    <t>wc_lang_tutorial_model</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>wc_lang tutorial model</t>
-  </si>
-  <si>
-    <t>Version</t>
-  </si>
-  <si>
-    <t>0.0.1</t>
-  </si>
-  <si>
-    <t>URL</t>
-  </si>
-  <si>
-    <t>https://github.com/org/repo</t>
-  </si>
-  <si>
-    <t>Branch</t>
-  </si>
-  <si>
-    <t>master</t>
-  </si>
-  <si>
-    <t>Revision</t>
-  </si>
-  <si>
-    <t>hash</t>
-  </si>
-  <si>
-    <t>wc_lang version</t>
-  </si>
-  <si>
-    <t>Time units</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>Identifiers</t>
-  </si>
-  <si>
-    <t>Comments</t>
-  </si>
-  <si>
-    <t>Created</t>
-  </si>
-  <si>
-    <t>Updated</t>
-  </si>
-  <si>
-    <t>taxon</t>
-  </si>
-  <si>
-    <t>Mycoplasma pneumoniae M129</t>
-  </si>
-  <si>
-    <t>Rank</t>
-  </si>
-  <si>
-    <t>variety</t>
-  </si>
-  <si>
-    <t>taxonomy: 272634</t>
-  </si>
-  <si>
-    <t>env</t>
-  </si>
-  <si>
-    <t>Temperature</t>
-  </si>
-  <si>
-    <t>Temperature units</t>
-  </si>
-  <si>
-    <t>degC</t>
-  </si>
-  <si>
-    <t>Framework</t>
-  </si>
-  <si>
     <t>metabolism</t>
   </si>
   <si>
@@ -808,10 +815,10 @@
     <t>Genotype</t>
   </si>
   <si>
-    <t>Measurement method</t>
-  </si>
-  <si>
-    <t>Analysis method</t>
+    <t>Data generation process</t>
+  </si>
+  <si>
+    <t>Data analysis process</t>
   </si>
   <si>
     <t>Variant</t>
@@ -832,7 +839,10 @@
     <t>Experiment design</t>
   </si>
   <si>
-    <t>Method</t>
+    <t>Process</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
   <si>
     <t>Title</t>
@@ -950,9 +960,6 @@
   </si>
   <si>
     <t>Intention type</t>
-  </si>
-  <si>
-    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -961,11 +968,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
     <numFmt numFmtId="176" formatCode="0.000E+00"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -1021,10 +1028,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -1042,28 +1062,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1079,7 +1079,52 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1093,9 +1138,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1117,45 +1162,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1182,7 +1189,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1194,7 +1231,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1206,13 +1291,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1224,7 +1327,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1236,133 +1369,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1385,10 +1392,51 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1399,6 +1447,15 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1432,189 +1489,139 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1849,8 +1856,9 @@
       <sheetName val="dFBA objective species"/>
       <sheetName val="Parameters"/>
       <sheetName val="Stop conditions"/>
-      <sheetName val="Evidence"/>
-      <sheetName val="Interpretations"/>
+      <sheetName val="Observations"/>
+      <sheetName val="Observation sets"/>
+      <sheetName val="Conclusions"/>
       <sheetName val="References"/>
       <sheetName val="Authors"/>
       <sheetName val="Changes"/>
@@ -1879,6 +1887,7 @@
       <sheetData sheetId="20"/>
       <sheetData sheetId="21"/>
       <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2142,12 +2151,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A19" sqref="A19:A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1" outlineLevelCol="2"/>
@@ -2335,7 +2344,7 @@
       </c>
       <c r="B20" s="22"/>
       <c r="C20" s="22">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" customHeight="1" spans="1:3">
@@ -2344,7 +2353,7 @@
       </c>
       <c r="B21" s="22"/>
       <c r="C21" s="22">
-        <v>21</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" customHeight="1" spans="1:3">
@@ -2353,7 +2362,7 @@
       </c>
       <c r="B22" s="22"/>
       <c r="C22" s="22">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" customHeight="1" spans="1:3">
@@ -2365,9 +2374,18 @@
         <v>0</v>
       </c>
     </row>
+    <row r="24" customHeight="1" spans="1:3">
+      <c r="A24" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0" objects="1" scenarios="1"/>
-  <autoFilter ref="A1:C23">
+  <autoFilter ref="A1:C24">
     <extLst/>
   </autoFilter>
   <hyperlinks>
@@ -2388,11 +2406,11 @@
     <hyperlink ref="A16" location="'dFBA objective species'!A1" display="dFBA objective species" tooltip="Click to view dfba objective species"/>
     <hyperlink ref="A17" location="'Parameters'!A1" display="Parameters" tooltip="Click to view parameters"/>
     <hyperlink ref="A18" location="'Stop conditions'!A1" display="Stop conditions" tooltip="Click to view stop conditions"/>
-    <hyperlink ref="A19" location="'Evidence'!A1" display="Evidence" tooltip="Click to view evidence"/>
-    <hyperlink ref="A20" location="'Interpretations'!A1" display="Interpretations" tooltip="Click to view interpretations"/>
-    <hyperlink ref="A21" location="'References'!A1" display="References" tooltip="Click to view references"/>
-    <hyperlink ref="A22" location="'Authors'!A1" display="Authors" tooltip="Click to view authors"/>
-    <hyperlink ref="A23" location="'Changes'!A1" display="Changes" tooltip="Click to view changes"/>
+    <hyperlink ref="A22" location="'References'!A1" display="References" tooltip="Click to view references"/>
+    <hyperlink ref="A23" location="'Authors'!A1" display="Authors" tooltip="Click to view authors"/>
+    <hyperlink ref="A24" location="'Changes'!A1" display="Changes" tooltip="Click to view changes"/>
+    <hyperlink ref="A19" location="'Evidence'!A1" display="Observations" tooltip="Click to view evidence"/>
+    <hyperlink ref="A21" location="'Interpretations'!A1" display="Conclusions" tooltip="Click to view interpretations"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -2419,31 +2437,31 @@
   <sheetData>
     <row r="1" ht="15.1" customHeight="1" spans="1:9">
       <c r="A1" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -2478,53 +2496,53 @@
   <sheetData>
     <row r="1" customHeight="1" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2567,7 +2585,7 @@
       <c r="E1" s="11"/>
       <c r="F1" s="11"/>
       <c r="G1" s="13" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="H1" s="13"/>
       <c r="I1" s="13"/>
@@ -3592,46 +3610,46 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:1027">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O2" s="11"/>
       <c r="P2" s="11"/>
@@ -4649,22 +4667,22 @@
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E3" s="10">
         <v>1</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
@@ -4672,22 +4690,22 @@
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="E4" s="10">
         <v>0</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
@@ -4695,44 +4713,44 @@
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="E5" s="10">
         <v>0</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="E6" s="1">
         <v>0</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -4770,130 +4788,130 @@
   <sheetData>
     <row r="1" ht="15.1" customHeight="1" spans="1:12">
       <c r="A1" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="1" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:7">
       <c r="A4" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>205</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>203</v>
       </c>
       <c r="E4" s="10"/>
       <c r="F4" s="1" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="1" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="1" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -4929,60 +4947,60 @@
   <sheetData>
     <row r="1" ht="15.1" customHeight="1" spans="1:12">
       <c r="A1" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -5015,34 +5033,34 @@
   <sheetData>
     <row r="1" ht="15.1" customHeight="1" spans="1:10">
       <c r="A1" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -5075,37 +5093,37 @@
   <sheetData>
     <row r="1" ht="15.1" customHeight="1" spans="1:11">
       <c r="A1" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -5138,199 +5156,199 @@
   <sheetData>
     <row r="1" customHeight="1" spans="1:11">
       <c r="A1" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:11">
       <c r="A2" s="1" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="D2" s="1">
         <v>0.3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="D3" s="1">
         <v>0.0003</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="D4" s="1">
         <v>0.0003</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:6">
       <c r="A5" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>223</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>221</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="D6" s="1">
         <v>2000</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="D7" s="1">
         <v>0.0003</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="D8" s="1">
         <v>0.001</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="D9" s="1">
         <v>0.001</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" customHeight="1" spans="1:6">
       <c r="A10" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>230</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>228</v>
       </c>
       <c r="D10" s="1">
         <v>0.01</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="11" customHeight="1" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D11" s="1">
         <v>1100</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="12" customHeight="1" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D12" s="1">
         <v>1000</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="13" customHeight="1" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D13" s="7">
         <v>6.02214075862e+23</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -5363,31 +5381,31 @@
   <sheetData>
     <row r="1" ht="15.1" customHeight="1" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -5403,24 +5421,24 @@
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AMU2"/>
+  <dimension ref="A1:AMT2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="Q1" sqref="Q1:T2"/>
+      <selection pane="bottomRight" activeCell="V1" sqref="V$1:V$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1027" width="9.10833333333333" style="1"/>
+    <col min="1" max="1026" width="9.10833333333333" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" spans="7:1035">
+    <row r="1" ht="15" customHeight="1" spans="7:1034">
       <c r="G1" s="6" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="H1" s="6"/>
       <c r="I1" s="6" t="s">
@@ -5432,13 +5450,14 @@
       <c r="M1" s="6"/>
       <c r="N1" s="6"/>
       <c r="Q1" s="5" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="R1" s="5"/>
       <c r="S1" s="5" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="T1" s="5"/>
+      <c r="AMM1" s="1"/>
       <c r="AMN1" s="1"/>
       <c r="AMO1" s="1"/>
       <c r="AMP1" s="1"/>
@@ -5446,81 +5465,78 @@
       <c r="AMR1" s="1"/>
       <c r="AMS1" s="1"/>
       <c r="AMT1" s="1"/>
-      <c r="AMU1" s="1"/>
-    </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:1035">
+    </row>
+    <row r="2" ht="15.1" customHeight="1" spans="1:1034">
       <c r="A2" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>22</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="AMM2" s="1"/>
       <c r="AMN2" s="1"/>
       <c r="AMO2" s="1"/>
       <c r="AMP2" s="1"/>
@@ -5528,7 +5544,6 @@
       <c r="AMR2" s="1"/>
       <c r="AMS2" s="1"/>
       <c r="AMT2" s="1"/>
-      <c r="AMU2" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -5564,86 +5579,86 @@
   <sheetData>
     <row r="1" ht="15.1" customHeight="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" ht="15.1" customHeight="1" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" ht="15.1" customHeight="1" spans="1:1">
       <c r="A9" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" ht="15.1" customHeight="1" spans="1:1">
       <c r="A10" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" ht="15.1" customHeight="1" spans="1:1">
       <c r="A11" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" ht="15.1" customHeight="1" spans="1:1">
       <c r="A12" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -5659,14 +5674,72 @@
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="1" width="14" style="1" customWidth="1"/>
+    <col min="2" max="3" width="13.3916666666667" style="1"/>
+    <col min="4" max="1017" width="9.10833333333333" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.1" customHeight="1" spans="1:6">
+      <c r="A1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" ht="15.1" customHeight="1"/>
+    <row r="3" ht="15.1" customHeight="1"/>
+    <row r="4" ht="15.1" customHeight="1"/>
+    <row r="5" ht="15.1" customHeight="1"/>
+    <row r="6" ht="15.1" customHeight="1"/>
+    <row r="7" ht="15.1" customHeight="1"/>
+    <row r="8" ht="15.1" customHeight="1"/>
+    <row r="9" ht="15.1" customHeight="1"/>
+  </sheetData>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G1" sqref="G1:H2"/>
+      <selection pane="bottomRight" activeCell="N2" sqref="N2:N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -5679,49 +5752,52 @@
   <sheetData>
     <row r="1" spans="7:8">
       <c r="G1" s="5" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:13">
+    <row r="2" ht="15.1" customHeight="1" spans="1:14">
       <c r="A2" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="3:4">
@@ -5769,7 +5845,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:R3"/>
@@ -5789,122 +5865,122 @@
   <sheetData>
     <row r="1" ht="15.1" customHeight="1" spans="1:18">
       <c r="A1" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:16">
       <c r="A2" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="F2" s="1">
         <v>2016</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="K2" s="1">
         <v>44</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:16">
       <c r="A3" s="1" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="F3" s="1">
         <v>2017</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="K3" s="1">
         <v>45</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -5917,7 +5993,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:L1"/>
@@ -5937,40 +6013,40 @@
   <sheetData>
     <row r="1" customHeight="1" spans="1:12">
       <c r="A1" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -5979,7 +6055,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:Q1"/>
@@ -5999,55 +6075,55 @@
   <sheetData>
     <row r="1" customHeight="1" spans="1:17">
       <c r="A1" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>283</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -6074,44 +6150,44 @@
   <sheetData>
     <row r="1" ht="15.1" customHeight="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:1">
       <c r="A5" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:1">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -6143,20 +6219,20 @@
   <sheetData>
     <row r="1" customHeight="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B3" s="1">
         <v>37</v>
@@ -6164,25 +6240,25 @@
     </row>
     <row r="4" customHeight="1" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:1">
       <c r="A5" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:1">
       <c r="A6" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:1">
       <c r="A7" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -6214,56 +6290,56 @@
   <sheetData>
     <row r="1" ht="15.1" customHeight="1" spans="1:8">
       <c r="A1" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -6300,14 +6376,14 @@
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
       <c r="H1" s="17" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I1" s="17"/>
       <c r="J1" s="17"/>
       <c r="K1" s="17"/>
       <c r="L1" s="11"/>
       <c r="M1" s="17" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="N1" s="17"/>
       <c r="O1" s="17"/>
@@ -7334,67 +7410,67 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:1035">
       <c r="A2" s="18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>71</v>
-      </c>
       <c r="P2" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="V2" s="11"/>
       <c r="W2" s="11"/>
@@ -8413,28 +8489,28 @@
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:20">
       <c r="A3" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="I3" s="7">
         <v>4.58e-17</v>
@@ -8443,13 +8519,13 @@
         <v>4.58e-18</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="N3" s="1">
         <v>7.75</v>
@@ -8458,36 +8534,36 @@
         <v>0.775</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:20">
       <c r="A4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="I4" s="1">
         <v>1</v>
@@ -8496,13 +8572,13 @@
         <v>0</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="N4" s="1">
         <v>7.75</v>
@@ -8511,13 +8587,13 @@
         <v>0.775</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -8539,7 +8615,7 @@
   <sheetPr/>
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
@@ -8556,7 +8632,7 @@
   <sheetData>
     <row r="1" spans="3:8">
       <c r="C1" s="17" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D1" s="17"/>
       <c r="E1" s="17"/>
@@ -8566,63 +8642,63 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:14">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:13">
       <c r="A3" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="G3" s="1">
         <v>424.1773</v>
@@ -8631,28 +8707,28 @@
         <v>-3</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="M3" s="16"/>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:13">
       <c r="A4" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G4" s="1">
         <v>345.2053</v>
@@ -8661,28 +8737,28 @@
         <v>-2</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="M4" s="16"/>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:13">
       <c r="A5" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="G5" s="1">
         <v>503.14946</v>
@@ -8691,28 +8767,28 @@
         <v>-4</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="M5" s="16"/>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:13">
       <c r="A6" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="G6" s="1">
         <v>180.15588</v>
@@ -8721,25 +8797,25 @@
         <v>0</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M6" s="16"/>
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:13">
       <c r="A7" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="G7" s="1">
         <v>1.00783</v>
@@ -8748,28 +8824,28 @@
         <v>1</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="M7" s="16"/>
     </row>
     <row r="8" ht="15.1" customHeight="1" spans="1:10">
       <c r="A8" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G8" s="1">
         <v>18.0153</v>
@@ -8778,27 +8854,27 @@
         <v>0</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" ht="15.1" customHeight="1" spans="1:10">
       <c r="A9" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G9" s="1">
         <v>95.9793</v>
@@ -8807,27 +8883,27 @@
         <v>-2</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" ht="15.1" customHeight="1" spans="1:9">
       <c r="A10" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G10" s="1">
         <v>174.95</v>
@@ -8836,27 +8912,27 @@
         <v>-3</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" ht="15.1" customHeight="1" spans="1:10">
       <c r="A11" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="G11" s="1">
         <v>3298.98577</v>
@@ -8865,22 +8941,21 @@
         <v>-11</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" ht="15.1" customHeight="1" spans="1:12">
       <c r="A12" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C12" s="1"/>
+        <v>150</v>
+      </c>
       <c r="F12" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="G12" s="1">
         <v>1042.32919</v>
@@ -8889,7 +8964,7 @@
         <v>-8</v>
       </c>
       <c r="I12" s="16" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="J12" s="16"/>
       <c r="K12" s="16"/>
@@ -8929,184 +9004,184 @@
   <sheetData>
     <row r="1" ht="15.1" customHeight="1" spans="1:10">
       <c r="A1" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B3" s="14"/>
       <c r="C3" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B4" s="14"/>
       <c r="C4" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B5" s="14"/>
       <c r="C5" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B6" s="14"/>
       <c r="C6" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B7" s="14"/>
       <c r="C7" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" ht="15.1" customHeight="1" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B8" s="14"/>
       <c r="C8" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" ht="15.1" customHeight="1" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B9" s="14"/>
       <c r="C9" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" ht="15.1" customHeight="1" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B10" s="14"/>
       <c r="C10" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" ht="15.1" customHeight="1" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B11" s="14"/>
       <c r="C11" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -9140,51 +9215,51 @@
   <sheetData>
     <row r="1" ht="15.1" customHeight="1" spans="1:12">
       <c r="A1" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E2" s="16">
         <v>0.005</v>
@@ -9193,25 +9268,25 @@
         <v>0.0121655250605964</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E3" s="16">
         <v>0.005</v>
       </c>
       <c r="F3" s="16"/>
       <c r="G3" s="16" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
@@ -9219,20 +9294,20 @@
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E4" s="16">
         <v>0.005</v>
       </c>
       <c r="F4" s="16"/>
       <c r="G4" s="16" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="H4" s="16"/>
       <c r="I4" s="16"/>
@@ -9240,20 +9315,20 @@
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E5" s="16">
         <v>0.01</v>
       </c>
       <c r="F5" s="16"/>
       <c r="G5" s="16" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="H5" s="16"/>
       <c r="I5" s="16"/>
@@ -9261,20 +9336,20 @@
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:10">
       <c r="A6" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E6" s="1">
         <v>1e-7</v>
       </c>
       <c r="F6" s="16"/>
       <c r="G6" s="16" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="H6" s="16"/>
       <c r="I6" s="16"/>
@@ -9282,20 +9357,20 @@
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:10">
       <c r="A7" s="1" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E7" s="16">
         <v>55</v>
       </c>
       <c r="F7" s="16"/>
       <c r="G7" s="16" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="H7" s="16"/>
       <c r="I7" s="16"/>
@@ -9303,20 +9378,20 @@
     </row>
     <row r="8" ht="15.1" customHeight="1" spans="1:10">
       <c r="A8" s="1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E8" s="7">
         <v>0.005</v>
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="16" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="H8" s="16"/>
       <c r="I8" s="16"/>

</xml_diff>

<commit_message>
updating for obj_tables and wc_lang
</commit_message>
<xml_diff>
--- a/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
+++ b/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="993" visibility="visible" windowHeight="13965" windowWidth="28695"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" windowWidth="28695" windowHeight="13965" tabRatio="993" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!!_Table of contents" sheetId="1" state="visible" r:id="rId1"/>
@@ -37,63 +37,63 @@
     <externalReference xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId26"/>
   </externalReferences>
   <definedNames>
-    <definedName localSheetId="4" name="_FilterDatabase_0">Submodels!#REF!</definedName>
-    <definedName localSheetId="5" name="excel_is_bugging_me">Compartments!$A$2:$G$4</definedName>
-    <definedName localSheetId="5" name="_FilterDatabase_0">Compartments!$A$2:$G$4</definedName>
-    <definedName localSheetId="5" name="_FilterDatabase_0_0">Compartments!$A$2:$G$4</definedName>
-    <definedName localSheetId="5" name="_FilterDatabase_0_0_0">Compartments!$A$2:$G$4</definedName>
-    <definedName localSheetId="5" name="_FilterDatabase_0_0_0_0">Compartments!$A$2:$G$4</definedName>
-    <definedName localSheetId="5" name="_FilterDatabase_0_0_0_0_0">Compartments!$A$2:$G$4</definedName>
-    <definedName localSheetId="5" name="_FilterDatabase_0_0_0_0_0_0">Compartments!$A$2:$G$4</definedName>
-    <definedName localSheetId="6" name="excel_is_bugging_me">'Species types'!$A$2:$N$7</definedName>
-    <definedName localSheetId="6" name="_FilterDatabase_0">'Species types'!$A$2:$N$7</definedName>
-    <definedName localSheetId="6" name="_FilterDatabase_0_0">'Species types'!$A$2:$N$7</definedName>
-    <definedName localSheetId="6" name="_FilterDatabase_0_0_0">'Species types'!$A$2:$N$7</definedName>
-    <definedName localSheetId="6" name="_FilterDatabase_0_0_0_0">'Species types'!$A$2:$N$7</definedName>
-    <definedName localSheetId="6" name="_FilterDatabase_0_0_0_0_0">'Species types'!$A$2:$N$7</definedName>
-    <definedName localSheetId="6" name="_FilterDatabase_0_0_0_0_0_0">'Species types'!$A$2:$N$7</definedName>
-    <definedName localSheetId="8" name="_FilterDatabase_0">'[1]#REF'!$C$1:$K$8</definedName>
-    <definedName localSheetId="8" name="_FilterDatabase_0_0">'[1]#REF'!$C$1:$K$8</definedName>
-    <definedName localSheetId="8" name="_FilterDatabase_0_0_0">'[1]#REF'!$C$1:$K$8</definedName>
-    <definedName localSheetId="8" name="_FilterDatabase_0_0_0_0">'[1]#REF'!$C$1:$K$8</definedName>
-    <definedName localSheetId="8" name="_FilterDatabase_0_0_0_0_0">'[1]#REF'!$C$1:$K$8</definedName>
-    <definedName localSheetId="8" name="_FilterDatabase_0_0_0_0_0_0">'[1]#REF'!$C$1:$K$8</definedName>
-    <definedName localSheetId="11" name="excel_is_bugging_me">Reactions!$A$2:$D$6</definedName>
-    <definedName localSheetId="11" name="_FilterDatabase_0">Reactions!$A$2:$D$6</definedName>
-    <definedName localSheetId="11" name="_FilterDatabase_0_0">Reactions!$A$2:$D$6</definedName>
-    <definedName localSheetId="11" name="_FilterDatabase_0_0_0">Reactions!$A$2:$D$6</definedName>
-    <definedName localSheetId="11" name="_FilterDatabase_0_0_0_0">Reactions!$A$2:$D$6</definedName>
-    <definedName localSheetId="11" name="_FilterDatabase_0_0_0_0_0">Reactions!$A$2:$D$6</definedName>
-    <definedName localSheetId="11" name="_FilterDatabase_0_0_0_0_0_0">Reactions!$A$2:$D$6</definedName>
-    <definedName localSheetId="12" name="_FilterDatabase_0">'Rate laws'!$C$1:$H$6</definedName>
-    <definedName localSheetId="12" name="_FilterDatabase_0_0">'Rate laws'!$C$1:$H$6</definedName>
-    <definedName localSheetId="12" name="_FilterDatabase_0_0_0">'Rate laws'!$C$1:$H$6</definedName>
-    <definedName localSheetId="12" name="_FilterDatabase_0_0_0_0">'Rate laws'!$C$1:$H$6</definedName>
-    <definedName localSheetId="12" name="_FilterDatabase_0_0_0_0_0">'Rate laws'!$C$1:$H$6</definedName>
-    <definedName localSheetId="12" name="_FilterDatabase_0_0_0_0_0_0">'Rate laws'!$C$1:$H$6</definedName>
-    <definedName localSheetId="16" name="excel_is_bugging_me">Parameters!$A$1:$F$1</definedName>
-    <definedName localSheetId="16" name="_FilterDatabase_0">Parameters!$A$1:$F$1</definedName>
-    <definedName localSheetId="16" name="_FilterDatabase_0_0">Parameters!$A$1:$F$1</definedName>
-    <definedName localSheetId="16" name="_FilterDatabase_0_0_0">Parameters!$A$1:$F$1</definedName>
-    <definedName localSheetId="16" name="_FilterDatabase_0_0_0_0">Parameters!$A$1:$F$1</definedName>
-    <definedName localSheetId="16" name="_FilterDatabase_0_0_0_0_0">Parameters!$A$1:$F$1</definedName>
-    <definedName localSheetId="16" name="_FilterDatabase_0_0_0_0_0_0">Parameters!$A$1:$F$1</definedName>
-    <definedName localSheetId="21" name="excel_is_bugging_me">References!$A$1:$D$1</definedName>
-    <definedName localSheetId="21" name="_FilterDatabase_0">References!$A$1:$D$1</definedName>
-    <definedName localSheetId="21" name="_FilterDatabase_0_0">References!$A$1:$D$1</definedName>
-    <definedName localSheetId="21" name="_FilterDatabase_0_0_0">References!$A$1:$D$1</definedName>
-    <definedName localSheetId="21" name="_FilterDatabase_0_0_0_0">References!$A$1:$D$1</definedName>
-    <definedName localSheetId="21" name="_FilterDatabase_0_0_0_0_0">References!$A$1:$D$1</definedName>
-    <definedName localSheetId="21" name="_FilterDatabase_0_0_0_0_0_0">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="4">Submodels!#REF!</definedName>
+    <definedName name="excel_is_bugging_me" localSheetId="5">Compartments!$A$2:$G$4</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="5">Compartments!$A$2:$G$4</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="5">Compartments!$A$2:$G$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="5">Compartments!$A$2:$G$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="5">Compartments!$A$2:$G$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$G$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$G$4</definedName>
+    <definedName name="excel_is_bugging_me" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="8">'[1]#REF'!$C$1:$K$8</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="8">'[1]#REF'!$C$1:$K$8</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="8">'[1]#REF'!$C$1:$K$8</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="8">'[1]#REF'!$C$1:$K$8</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="8">'[1]#REF'!$C$1:$K$8</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="8">'[1]#REF'!$C$1:$K$8</definedName>
+    <definedName name="excel_is_bugging_me" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="12">'Rate laws'!$C$1:$H$6</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="12">'Rate laws'!$C$1:$H$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="12">'Rate laws'!$C$1:$H$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="12">'Rate laws'!$C$1:$H$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="12">'Rate laws'!$C$1:$H$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="12">'Rate laws'!$C$1:$H$6</definedName>
+    <definedName name="excel_is_bugging_me" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="excel_is_bugging_me" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
     <definedName name="Id">'[2]Rate laws'!$A:$A</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'!!_Table of contents'!$A$1:$C$24</definedName>
-    <definedName hidden="1" localSheetId="5" name="_xlnm._FilterDatabase">'!!Compartments'!$A$2:$G$4</definedName>
-    <definedName hidden="1" localSheetId="6" name="_xlnm._FilterDatabase">'!!Species types'!$A$2:$N$12</definedName>
-    <definedName hidden="1" localSheetId="8" name="_xlnm._FilterDatabase">'!!Init species concentrations'!$C$1:$L$8</definedName>
-    <definedName hidden="1" localSheetId="11" name="_xlnm._FilterDatabase">'!!Reactions'!$A$2:$D$6</definedName>
-    <definedName hidden="1" localSheetId="12" name="_xlnm._FilterDatabase">'!!Rate laws'!$C$1:$H$6</definedName>
-    <definedName hidden="1" localSheetId="16" name="_xlnm._FilterDatabase">'!!Parameters'!$A$1:$F$13</definedName>
-    <definedName hidden="1" localSheetId="21" name="_xlnm._FilterDatabase">'!!References'!$A$1:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'!!_Table of contents'!$A$1:$C$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'!!Compartments'!$A$2:$G$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'!!Species types'!$A$2:$N$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'!!Init species concentrations'!$C$1:$L$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'!!Reactions'!$A$2:$D$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'!!Rate laws'!$C$1:$H$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">'!!Parameters'!$A$1:$F$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">'!!References'!$A$1:$D$3</definedName>
   </definedNames>
   <calcPr calcId="144525" fullCalcOnLoad="1"/>
 </workbook>
@@ -102,9 +102,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;" numFmtId="164"/>
-    <numFmt formatCode="0.000E+00" numFmtId="165"/>
-    <numFmt formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" numFmtId="166"/>
+    <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="165" formatCode="0.000E+00"/>
+    <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -623,266 +623,266 @@
     </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="33" fontId="9" numFmtId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="34" fontId="10" numFmtId="0">
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="6" fontId="9" numFmtId="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="21" fontId="9" numFmtId="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="5" fontId="10" numFmtId="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="31" fontId="10" numFmtId="0">
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="26" fontId="9" numFmtId="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="29" fontId="9" numFmtId="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="28" fontId="10" numFmtId="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="25" fontId="9" numFmtId="0">
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="9" fillId="0" fontId="22" numFmtId="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="20" fontId="10" numFmtId="0">
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="17" fontId="9" numFmtId="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="22" fontId="9" numFmtId="0">
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="30" fontId="10" numFmtId="0">
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="16" fontId="10" numFmtId="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="14" fontId="9" numFmtId="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="19" fontId="10" numFmtId="0">
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="18" fontId="10" numFmtId="0">
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="13" fontId="9" numFmtId="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="32" fontId="25" numFmtId="0">
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="12" fontId="9" numFmtId="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="10" fontId="18" numFmtId="0">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="27" fontId="10" numFmtId="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="7" fillId="0" fontId="20" numFmtId="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="6" fillId="11" fontId="19" numFmtId="0">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="6" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="166"/>
-    <xf applyAlignment="1" borderId="0" fillId="15" fontId="10" numFmtId="0">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="3" fillId="8" fontId="5" numFmtId="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="8" fillId="23" fontId="21" numFmtId="0">
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="8" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="14" numFmtId="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="8" fillId="11" fontId="26" numFmtId="0">
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="8" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="7" fontId="16" numFmtId="0">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="5" fillId="0" fontId="14" numFmtId="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="24" numFmtId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="24" fontId="10" numFmtId="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="13" numFmtId="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="15" numFmtId="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="12" numFmtId="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="11" numFmtId="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="1" borderId="4" fillId="9" fontId="17" numFmtId="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="4" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="4" fontId="9" numFmtId="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="23" numFmtId="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="25">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="11" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="35">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="35">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="35">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="35">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
+      <protection locked="0" hidden="0"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="52" name="60% - Accent6" xfId="1"/>
-    <cellStyle builtinId="51" name="40% - Accent6" xfId="2"/>
-    <cellStyle builtinId="48" name="60% - Accent5" xfId="3"/>
-    <cellStyle builtinId="49" name="Accent6" xfId="4"/>
-    <cellStyle builtinId="47" name="40% - Accent5" xfId="5"/>
-    <cellStyle builtinId="46" name="20% - Accent5" xfId="6"/>
-    <cellStyle builtinId="44" name="60% - Accent4" xfId="7"/>
-    <cellStyle builtinId="45" name="Accent5" xfId="8"/>
-    <cellStyle builtinId="43" name="40% - Accent4" xfId="9"/>
-    <cellStyle builtinId="41" name="Accent4" xfId="10"/>
-    <cellStyle builtinId="24" name="Linked Cell" xfId="11"/>
-    <cellStyle builtinId="39" name="40% - Accent3" xfId="12"/>
-    <cellStyle builtinId="36" name="60% - Accent2" xfId="13"/>
-    <cellStyle builtinId="37" name="Accent3" xfId="14"/>
-    <cellStyle builtinId="35" name="40% - Accent2" xfId="15"/>
-    <cellStyle builtinId="34" name="20% - Accent2" xfId="16"/>
-    <cellStyle builtinId="33" name="Accent2" xfId="17"/>
-    <cellStyle builtinId="31" name="40% - Accent1" xfId="18"/>
-    <cellStyle builtinId="30" name="20% - Accent1" xfId="19"/>
-    <cellStyle builtinId="29" name="Accent1" xfId="20"/>
-    <cellStyle builtinId="28" name="Neutral" xfId="21"/>
-    <cellStyle builtinId="32" name="60% - Accent1" xfId="22"/>
-    <cellStyle builtinId="27" name="Bad" xfId="23"/>
-    <cellStyle builtinId="42" name="20% - Accent4" xfId="24"/>
-    <cellStyle builtinId="25" name="Total" xfId="25"/>
-    <cellStyle builtinId="21" name="Output" xfId="26"/>
-    <cellStyle builtinId="4" name="Currency" xfId="27"/>
-    <cellStyle builtinId="38" name="20% - Accent3" xfId="28"/>
-    <cellStyle builtinId="10" name="Note" xfId="29"/>
-    <cellStyle builtinId="20" name="Input" xfId="30"/>
-    <cellStyle builtinId="19" name="Heading 4" xfId="31"/>
-    <cellStyle builtinId="22" name="Calculation" xfId="32"/>
-    <cellStyle builtinId="26" name="Good" xfId="33"/>
-    <cellStyle builtinId="18" name="Heading 3" xfId="34"/>
-    <cellStyle builtinId="53" name="CExplanatory Text" xfId="35"/>
-    <cellStyle builtinId="16" name="Heading 1" xfId="36"/>
-    <cellStyle builtinId="6" name="Comma [0]" xfId="37"/>
-    <cellStyle builtinId="50" name="20% - Accent6" xfId="38"/>
-    <cellStyle builtinId="15" name="Title" xfId="39"/>
-    <cellStyle builtinId="7" name="Currency [0]" xfId="40"/>
-    <cellStyle builtinId="11" name="Warning Text" xfId="41"/>
-    <cellStyle builtinId="9" name="Followed Hyperlink" xfId="42"/>
-    <cellStyle builtinId="17" name="Heading 2" xfId="43"/>
-    <cellStyle builtinId="3" name="Comma" xfId="44"/>
-    <cellStyle builtinId="23" name="Check Cell" xfId="45"/>
-    <cellStyle builtinId="40" name="60% - Accent3" xfId="46"/>
-    <cellStyle builtinId="5" name="Percent" xfId="47"/>
-    <cellStyle builtinId="8" name="Hyperlink" xfId="48"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -893,7 +893,7 @@
       <sheetName val="#REF"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData refreshError="1" sheetId="0"/>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1222,28 +1222,28 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A19" pane="bottomLeft" sqref="A19:A21"/>
+      <selection pane="bottomLeft" activeCell="A19" sqref="A19:A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="9" defaultRowHeight="15" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1"/>
   <cols>
-    <col customWidth="1" max="3" min="1" style="20" width="15.7083333333333"/>
-    <col customWidth="1" hidden="1" max="16384" min="4" style="20" width="9"/>
+    <col width="15.7083333333333" customWidth="1" style="20" min="1" max="3"/>
+    <col hidden="1" width="9" customWidth="1" style="20" min="4" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!!ObjTables ObjTablesVersion='0.0.8'</t>
+          <t>!!!ObjTables objTablesVersion='0.0.8'</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Schema' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Schema' objTablesVersion='0.0.8' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -1520,30 +1520,30 @@
   </sheetData>
   <autoFilter ref="A1:C24"/>
   <hyperlinks>
-    <hyperlink display="Model" location="'Model'!A1" ref="A2" tooltip="Click to view model"/>
-    <hyperlink display="Taxon" location="'Taxon'!A1" ref="A3" tooltip="Click to view taxon"/>
-    <hyperlink display="Environment" location="'Environment'!A1" ref="A4" tooltip="Click to view environment"/>
-    <hyperlink display="Submodels" location="'Submodels'!A1" ref="A5" tooltip="Click to view submodels"/>
-    <hyperlink display="Compartments" location="'Compartments'!A1" ref="A6" tooltip="Click to view compartments"/>
-    <hyperlink display="Species types" location="'Species types'!A1" ref="A7" tooltip="Click to view species types"/>
-    <hyperlink display="Species" location="'Species'!A1" ref="A8" tooltip="Click to view species"/>
-    <hyperlink display="Initial species concentrations" location="'Initial species concentrations'!A1" ref="A9" tooltip="Click to view initial species concentrations"/>
-    <hyperlink display="Observables" location="'Observables'!A1" ref="A10" tooltip="Click to view observables"/>
-    <hyperlink display="Functions" location="'Functions'!A1" ref="A11" tooltip="Click to view functions"/>
-    <hyperlink display="Reactions" location="'Reactions'!A1" ref="A12" tooltip="Click to view reactions"/>
-    <hyperlink display="Rate laws" location="'Rate laws'!A1" ref="A13" tooltip="Click to view rate laws"/>
-    <hyperlink display="dFBA objectives" location="'dFBA objectives'!A1" ref="A14" tooltip="Click to view dfba objectives"/>
-    <hyperlink display="dFBA objective reactions" location="'dFBA objective reactions'!A1" ref="A15" tooltip="Click to view dfba objective reactions"/>
-    <hyperlink display="dFBA objective species" location="'dFBA objective species'!A1" ref="A16" tooltip="Click to view dfba objective species"/>
-    <hyperlink display="Parameters" location="'Parameters'!A1" ref="A17" tooltip="Click to view parameters"/>
-    <hyperlink display="Stop conditions" location="'Stop conditions'!A1" ref="A18" tooltip="Click to view stop conditions"/>
-    <hyperlink display="Observations" location="'Evidence'!A1" ref="A19" tooltip="Click to view evidence"/>
-    <hyperlink display="Conclusions" location="'Interpretations'!A1" ref="A21" tooltip="Click to view interpretations"/>
-    <hyperlink display="References" location="'References'!A1" ref="A22" tooltip="Click to view references"/>
-    <hyperlink display="Authors" location="'Authors'!A1" ref="A23" tooltip="Click to view authors"/>
-    <hyperlink display="Changes" location="'Changes'!A1" ref="A24" tooltip="Click to view changes"/>
+    <hyperlink ref="A2" location="'Model'!A1" tooltip="Click to view model" display="Model"/>
+    <hyperlink ref="A3" location="'Taxon'!A1" tooltip="Click to view taxon" display="Taxon"/>
+    <hyperlink ref="A4" location="'Environment'!A1" tooltip="Click to view environment" display="Environment"/>
+    <hyperlink ref="A5" location="'Submodels'!A1" tooltip="Click to view submodels" display="Submodels"/>
+    <hyperlink ref="A6" location="'Compartments'!A1" tooltip="Click to view compartments" display="Compartments"/>
+    <hyperlink ref="A7" location="'Species types'!A1" tooltip="Click to view species types" display="Species types"/>
+    <hyperlink ref="A8" location="'Species'!A1" tooltip="Click to view species" display="Species"/>
+    <hyperlink ref="A9" location="'Initial species concentrations'!A1" tooltip="Click to view initial species concentrations" display="Initial species concentrations"/>
+    <hyperlink ref="A10" location="'Observables'!A1" tooltip="Click to view observables" display="Observables"/>
+    <hyperlink ref="A11" location="'Functions'!A1" tooltip="Click to view functions" display="Functions"/>
+    <hyperlink ref="A12" location="'Reactions'!A1" tooltip="Click to view reactions" display="Reactions"/>
+    <hyperlink ref="A13" location="'Rate laws'!A1" tooltip="Click to view rate laws" display="Rate laws"/>
+    <hyperlink ref="A14" location="'dFBA objectives'!A1" tooltip="Click to view dfba objectives" display="dFBA objectives"/>
+    <hyperlink ref="A15" location="'dFBA objective reactions'!A1" tooltip="Click to view dfba objective reactions" display="dFBA objective reactions"/>
+    <hyperlink ref="A16" location="'dFBA objective species'!A1" tooltip="Click to view dfba objective species" display="dFBA objective species"/>
+    <hyperlink ref="A17" location="'Parameters'!A1" tooltip="Click to view parameters" display="Parameters"/>
+    <hyperlink ref="A18" location="'Stop conditions'!A1" tooltip="Click to view stop conditions" display="Stop conditions"/>
+    <hyperlink ref="A19" location="'Evidence'!A1" tooltip="Click to view evidence" display="Observations"/>
+    <hyperlink ref="A21" location="'Interpretations'!A1" tooltip="Click to view interpretations" display="Conclusions"/>
+    <hyperlink ref="A22" location="'References'!A1" tooltip="Click to view references" display="References"/>
+    <hyperlink ref="A23" location="'Authors'!A1" tooltip="Click to view authors" display="Authors"/>
+    <hyperlink ref="A24" location="'Changes'!A1" tooltip="Click to view changes" display="Changes"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1556,22 +1556,22 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="B2" xSplit="1" ySplit="1"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="topRight" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
-      <selection activeCell="G1" pane="bottomRight" sqref="G1"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col customWidth="1" max="1026" min="1" style="15" width="8.78333333333333"/>
+    <col width="8.78333333333333" customWidth="1" style="15" min="1" max="1026"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15.1" r="1">
+    <row r="1" ht="15.1" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='Observable' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Data' id='Observable' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -1623,8 +1623,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" paperSize="1" useFirstPageNumber="1" verticalDpi="300"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup orientation="portrait" paperSize="1" firstPageNumber="0" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
@@ -1645,24 +1645,24 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="B2" xSplit="1" ySplit="1"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="topRight" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
-      <selection activeCell="G1" pane="bottomRight" sqref="G1"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelRow="2"/>
   <cols>
-    <col customWidth="1" max="2" min="1" style="15" width="8.78333333333333"/>
-    <col customWidth="1" max="3" min="3" style="15" width="11"/>
-    <col customWidth="1" max="1026" min="4" style="15" width="8.78333333333333"/>
+    <col width="8.78333333333333" customWidth="1" style="15" min="1" max="2"/>
+    <col width="11" customWidth="1" style="15" min="3" max="3"/>
+    <col width="8.78333333333333" customWidth="1" style="15" min="4" max="1026"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='Function' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Data' id='Function' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -1748,8 +1748,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" paperSize="1" useFirstPageNumber="1" verticalDpi="300"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup orientation="portrait" paperSize="1" firstPageNumber="0" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
@@ -1770,30 +1770,30 @@
   <dimension ref="A1:AMM7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="E2" xSplit="1" ySplit="2"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="topRight" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
-      <selection activeCell="G2" pane="bottomRight" sqref="G2"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="15" width="17.6416666666667"/>
-    <col customWidth="1" max="2" min="2" style="15" width="18.2916666666667"/>
-    <col customWidth="1" max="3" min="3" style="15" width="13.3416666666667"/>
-    <col customWidth="1" max="4" min="4" style="15" width="40.575"/>
-    <col customWidth="1" max="1027" min="5" style="15" width="8.78333333333333"/>
+    <col width="17.6416666666667" customWidth="1" style="15" min="1" max="1"/>
+    <col width="18.2916666666667" customWidth="1" style="15" min="2" max="2"/>
+    <col width="13.3416666666667" customWidth="1" style="15" min="3" max="3"/>
+    <col width="40.575" customWidth="1" style="15" min="4" max="4"/>
+    <col width="8.78333333333333" customWidth="1" style="15" min="5" max="1027"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='Reaction' ObjTablesVersion='0.0.8'</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="15.1" r="2">
+          <t>!!ObjTables type='Data' id='Reaction' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15.1" customHeight="1">
       <c r="A2" s="11" t="n"/>
       <c r="B2" s="11" t="n"/>
       <c r="C2" s="11" t="n"/>
@@ -2824,7 +2824,7 @@
       <c r="AML2" s="11" t="n"/>
       <c r="AMM2" s="11" t="n"/>
     </row>
-    <row customHeight="1" ht="15.1" r="3">
+    <row r="3" ht="15.1" customHeight="1">
       <c r="A3" s="18" t="inlineStr">
         <is>
           <t>!Id</t>
@@ -3909,7 +3909,7 @@
       <c r="AML3" s="11" t="n"/>
       <c r="AMM3" s="11" t="n"/>
     </row>
-    <row customHeight="1" ht="15.1" r="4">
+    <row r="4" ht="15.1" customHeight="1">
       <c r="A4" s="15" t="inlineStr">
         <is>
           <t>atp_hydrolysis</t>
@@ -3942,7 +3942,7 @@
       <c r="H4" s="10" t="n"/>
       <c r="J4" s="24" t="n"/>
     </row>
-    <row customHeight="1" ht="15.1" r="5">
+    <row r="5" ht="15.1" customHeight="1">
       <c r="A5" s="15" t="inlineStr">
         <is>
           <t>biomass_production</t>
@@ -3975,7 +3975,7 @@
       <c r="H5" s="10" t="n"/>
       <c r="J5" s="24" t="n"/>
     </row>
-    <row customHeight="1" ht="15.1" r="6">
+    <row r="6" ht="15.1" customHeight="1">
       <c r="A6" s="15" t="inlineStr">
         <is>
           <t>glc_import</t>
@@ -4042,8 +4042,8 @@
   <mergeCells count="1">
     <mergeCell ref="G2:I2"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" paperSize="1" useFirstPageNumber="1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup orientation="portrait" paperSize="1" firstPageNumber="0" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
@@ -4056,28 +4056,28 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="B2" xSplit="1" ySplit="1"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="topRight" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
-      <selection activeCell="E2" pane="bottomRight" sqref="E2:E6"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="E2" sqref="E2:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5"/>
   <cols>
-    <col customWidth="1" max="5" min="1" style="15" width="8.78333333333333"/>
-    <col customWidth="1" max="6" min="6" style="15" width="68.5"/>
-    <col customWidth="1" max="1026" min="7" style="15" width="8.78333333333333"/>
+    <col width="8.78333333333333" customWidth="1" style="15" min="1" max="5"/>
+    <col width="68.5" customWidth="1" style="15" min="6" max="6"/>
+    <col width="8.78333333333333" customWidth="1" style="15" min="7" max="1026"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15.1" r="1">
+    <row r="1" ht="15.1" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='RateLaw' ObjTablesVersion='0.0.8'</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="15.1" r="2">
+          <t>!!ObjTables type='Data' id='RateLaw' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15.1" customHeight="1">
       <c r="A2" s="18" t="inlineStr">
         <is>
           <t>!Id</t>
@@ -4139,7 +4139,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.1" r="3">
+    <row r="3" ht="15.1" customHeight="1">
       <c r="A3" s="15" t="inlineStr">
         <is>
           <t>atp_hydrolysis-backward</t>
@@ -4167,7 +4167,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.1" r="4">
+    <row r="4" ht="15.1" customHeight="1">
       <c r="A4" s="15" t="inlineStr">
         <is>
           <t>atp_hydrolysis-forward</t>
@@ -4195,7 +4195,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.1" r="5">
+    <row r="5" ht="15.1" customHeight="1">
       <c r="A5" s="15" t="inlineStr">
         <is>
           <t>biomass_production-forward</t>
@@ -4223,7 +4223,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.1" r="6">
+    <row r="6" ht="15.1" customHeight="1">
       <c r="A6" s="15" t="inlineStr">
         <is>
           <t>glc_import-forward</t>
@@ -4281,8 +4281,8 @@
     </row>
   </sheetData>
   <autoFilter ref="C1:H6"/>
-  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" paperSize="1" useFirstPageNumber="1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup orientation="portrait" paperSize="1" firstPageNumber="0" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
@@ -4295,29 +4295,29 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="B2" xSplit="1" ySplit="1"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="topRight" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomRight" sqref="$A1:$XFD1"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="$A1:$XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="15" width="17"/>
-    <col customWidth="1" max="4" min="2" style="15" width="9.108333333333331"/>
-    <col customWidth="1" max="6" min="5" style="15" width="12.25"/>
-    <col customWidth="1" max="1028" min="7" style="15" width="9.108333333333331"/>
+    <col width="17" customWidth="1" style="15" min="1" max="1"/>
+    <col width="9.108333333333331" customWidth="1" style="15" min="2" max="4"/>
+    <col width="12.25" customWidth="1" style="15" min="5" max="6"/>
+    <col width="9.108333333333331" customWidth="1" style="15" min="7" max="1028"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15.1" r="1">
+    <row r="1" ht="15.1" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='DfbaObjective' ObjTablesVersion='0.0.8'</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="15.1" r="2">
+          <t>!!ObjTables type='Data' id='DfbaObjective' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15.1" customHeight="1">
       <c r="A2" s="18" t="inlineStr">
         <is>
           <t>!Id</t>
@@ -4412,8 +4412,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" paperSize="1" useFirstPageNumber="1" verticalDpi="300"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup orientation="portrait" paperSize="1" firstPageNumber="0" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
@@ -4434,22 +4434,22 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="B2" xSplit="1" ySplit="1"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="topRight" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
-      <selection activeCell="H1" pane="bottomRight" sqref="H1"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col customWidth="1" max="1026" min="1" style="15" width="8.78333333333333"/>
+    <col width="8.78333333333333" customWidth="1" style="15" min="1" max="1026"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15.1" r="1">
+    <row r="1" ht="15.1" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='DfbaObjReaction' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Data' id='DfbaObjReaction' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -4506,8 +4506,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" paperSize="1" useFirstPageNumber="1" verticalDpi="300"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup orientation="portrait" paperSize="1" firstPageNumber="0" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
@@ -4528,22 +4528,22 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="B2" xSplit="1" ySplit="1"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="topRight" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
-      <selection activeCell="I1" pane="bottomRight" sqref="I1"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col customWidth="1" max="1026" min="1" style="15" width="8.78333333333333"/>
+    <col width="8.78333333333333" customWidth="1" style="15" min="1" max="1026"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15.1" r="1">
+    <row r="1" ht="15.1" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='DfbaObjSpecies' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Data' id='DfbaObjSpecies' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -4605,8 +4605,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" paperSize="1" useFirstPageNumber="1" verticalDpi="300"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup orientation="portrait" paperSize="1" firstPageNumber="0" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
@@ -4627,22 +4627,22 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="B2" xSplit="1" ySplit="1"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="topRight" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
-      <selection activeCell="C13" pane="bottomRight" sqref="C13"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" max="1026" min="1" style="15" width="8.78333333333333"/>
+    <col width="8.78333333333333" customWidth="1" style="15" min="1" max="1026"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='Parameter' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Data' id='Parameter' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -4935,8 +4935,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:F13"/>
-  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" paperSize="1" useFirstPageNumber="1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup orientation="portrait" paperSize="1" firstPageNumber="0" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
@@ -4949,22 +4949,22 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="B2" xSplit="1" ySplit="1"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="topRight" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
-      <selection activeCell="G1" pane="bottomRight" sqref="G1"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col customWidth="1" max="1026" min="1" style="15" width="8.78333333333333"/>
+    <col width="8.78333333333333" customWidth="1" style="15" min="1" max="1026"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15.1" r="1">
+    <row r="1" ht="15.1" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='StopCondition' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Data' id='StopCondition' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -5016,8 +5016,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" paperSize="1" useFirstPageNumber="1" verticalDpi="300"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup orientation="portrait" paperSize="1" firstPageNumber="0" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
@@ -5038,26 +5038,26 @@
   <dimension ref="A1:AMT3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="B2" xSplit="1" ySplit="2"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="topRight" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
-      <selection activeCell="V1" pane="bottomRight" sqref="V$1:V$1048576"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="V1" sqref="V$1:V$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
   <cols>
-    <col customWidth="1" max="1026" min="1" style="15" width="9.108333333333331"/>
+    <col width="9.108333333333331" customWidth="1" style="15" min="1" max="1026"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15" r="1">
+    <row r="1" ht="15" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='Observation' ObjTablesVersion='0.0.8'</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="15.1" r="2">
+          <t>!!ObjTables type='Data' id='Observation' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15.1" customHeight="1">
       <c r="G2" s="6" t="inlineStr">
         <is>
           <t>!Genotype</t>
@@ -5219,8 +5219,8 @@
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="S2:T2"/>
   </mergeCells>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" paperSize="1" useFirstPageNumber="1" verticalDpi="300"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup orientation="portrait" paperSize="1" firstPageNumber="0" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
@@ -5241,24 +5241,24 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="topRight" state="frozen" topLeftCell="B1" xSplit="1"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A8" pane="topRight" sqref="$A8:$XFD10"/>
+      <selection pane="topRight" activeCell="A8" sqref="$A8:$XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col customWidth="1" max="1025" min="1" style="15" width="8.78333333333333"/>
+    <col width="8.78333333333333" customWidth="1" style="15" min="1" max="1025"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15.1" r="1">
+    <row r="1" ht="15.1" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='Model' ObjTablesVersion='0.0.8'</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="15.1" r="2">
+          <t>!!ObjTables type='Data' id='Model' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='column'</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15.1" customHeight="1">
       <c r="A2" s="18" t="inlineStr">
         <is>
           <t>!Id</t>
@@ -5270,7 +5270,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.1" r="3">
+    <row r="3" ht="15.1" customHeight="1">
       <c r="A3" s="18" t="inlineStr">
         <is>
           <t>!Name</t>
@@ -5282,7 +5282,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.1" r="4">
+    <row r="4" ht="15.1" customHeight="1">
       <c r="A4" s="18" t="inlineStr">
         <is>
           <t>!Version</t>
@@ -5294,7 +5294,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.1" r="5">
+    <row r="5" ht="15.1" customHeight="1">
       <c r="A5" s="18" t="inlineStr">
         <is>
           <t>!URL</t>
@@ -5306,7 +5306,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.1" r="6">
+    <row r="6" ht="15.1" customHeight="1">
       <c r="A6" s="18" t="inlineStr">
         <is>
           <t>!Branch</t>
@@ -5318,7 +5318,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.1" r="7">
+    <row r="7" ht="15.1" customHeight="1">
       <c r="A7" s="18" t="inlineStr">
         <is>
           <t>!Revision</t>
@@ -5330,7 +5330,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.1" r="8">
+    <row r="8" ht="15.1" customHeight="1">
       <c r="A8" s="18" t="inlineStr">
         <is>
           <t>!wc_lang version</t>
@@ -5342,7 +5342,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.1" r="9">
+    <row r="9" ht="15.1" customHeight="1">
       <c r="A9" s="18" t="inlineStr">
         <is>
           <t>!Time units</t>
@@ -5354,21 +5354,21 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.1" r="10">
+    <row r="10" ht="15.1" customHeight="1">
       <c r="A10" s="18" t="inlineStr">
         <is>
           <t>!Identifiers</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.1" r="11">
+    <row r="11" ht="15.1" customHeight="1">
       <c r="A11" s="18" t="inlineStr">
         <is>
           <t>!Comments</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.1" r="12">
+    <row r="12" ht="15.1" customHeight="1">
       <c r="A12" s="18" t="inlineStr">
         <is>
           <t>!Created</t>
@@ -5384,10 +5384,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" display="https://github.com/org/repo" ref="B4" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B4" display="https://github.com/org/repo" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" paperSize="1" useFirstPageNumber="1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup orientation="portrait" paperSize="1" firstPageNumber="0" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
@@ -5400,28 +5400,28 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="B2" xSplit="1" ySplit="1"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="topRight" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomRight" sqref="A1"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="15" width="14"/>
-    <col customWidth="1" max="3" min="2" style="15" width="13.3916666666667"/>
-    <col customWidth="1" max="1017" min="4" style="15" width="9.108333333333331"/>
+    <col width="14" customWidth="1" style="15" min="1" max="1"/>
+    <col width="13.3916666666667" customWidth="1" style="15" min="2" max="3"/>
+    <col width="9.108333333333331" customWidth="1" style="15" min="4" max="1017"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15.1" r="1">
+    <row r="1" ht="15.1" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='ObservationSet' ObjTablesVersion='0.0.8'</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="15.1" r="2">
+          <t>!!ObjTables type='Data' id='ObservationSet' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15.1" customHeight="1">
       <c r="A2" s="3" t="inlineStr">
         <is>
           <t>!Id</t>
@@ -5453,16 +5453,16 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.1" r="3"/>
-    <row customHeight="1" ht="15.1" r="4"/>
-    <row customHeight="1" ht="15.1" r="5"/>
-    <row customHeight="1" ht="15.1" r="6"/>
-    <row customHeight="1" ht="15.1" r="7"/>
-    <row customHeight="1" ht="15.1" r="8"/>
-    <row customHeight="1" ht="15.1" r="9"/>
+    <row r="3" ht="15.1" customHeight="1"/>
+    <row r="4" ht="15.1" customHeight="1"/>
+    <row r="5" ht="15.1" customHeight="1"/>
+    <row r="6" ht="15.1" customHeight="1"/>
+    <row r="7" ht="15.1" customHeight="1"/>
+    <row r="8" ht="15.1" customHeight="1"/>
+    <row r="9" ht="15.1" customHeight="1"/>
   </sheetData>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" paperSize="1" useFirstPageNumber="1" verticalDpi="300"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup orientation="portrait" paperSize="1" firstPageNumber="0" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
@@ -5483,36 +5483,36 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="B2" xSplit="1" ySplit="2"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="topRight" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
-      <selection activeCell="N2" pane="bottomRight" sqref="N2:N3"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="N2" sqref="N2:N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="15" width="15.125"/>
-    <col customWidth="1" max="2" min="2" style="15" width="14.75"/>
-    <col customWidth="1" max="1023" min="3" style="15" width="9.108333333333331"/>
-    <col customWidth="1" max="1024" min="1024" width="9.108333333333331"/>
+    <col width="15.125" customWidth="1" style="15" min="1" max="1"/>
+    <col width="14.75" customWidth="1" style="15" min="2" max="2"/>
+    <col width="9.108333333333331" customWidth="1" style="15" min="3" max="1023"/>
+    <col width="9.108333333333331" customWidth="1" min="1024" max="1024"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='Conclusion' ObjTablesVersion='0.0.8'</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="15.1" r="2">
+          <t>!!ObjTables type='Data' id='Conclusion' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15.1" customHeight="1">
       <c r="G2" s="5" t="inlineStr">
         <is>
           <t>!Process</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.1" r="3">
+    <row r="3" ht="15.1" customHeight="1">
       <c r="A3" s="3" t="inlineStr">
         <is>
           <t>!Id</t>
@@ -5584,31 +5584,31 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.1" r="4">
+    <row r="4" ht="15.1" customHeight="1">
       <c r="C4" s="4" t="n"/>
       <c r="D4" s="4" t="n"/>
     </row>
-    <row customHeight="1" ht="15.1" r="5">
+    <row r="5" ht="15.1" customHeight="1">
       <c r="C5" s="4" t="n"/>
       <c r="D5" s="4" t="n"/>
     </row>
-    <row customHeight="1" ht="15.1" r="6">
+    <row r="6" ht="15.1" customHeight="1">
       <c r="C6" s="4" t="n"/>
       <c r="D6" s="4" t="n"/>
     </row>
-    <row customHeight="1" ht="15.1" r="7">
+    <row r="7" ht="15.1" customHeight="1">
       <c r="C7" s="4" t="n"/>
       <c r="D7" s="4" t="n"/>
     </row>
-    <row customHeight="1" ht="15.1" r="8">
+    <row r="8" ht="15.1" customHeight="1">
       <c r="C8" s="4" t="n"/>
       <c r="D8" s="4" t="n"/>
     </row>
-    <row customHeight="1" ht="15.1" r="9">
+    <row r="9" ht="15.1" customHeight="1">
       <c r="C9" s="4" t="n"/>
       <c r="D9" s="4" t="n"/>
     </row>
-    <row customHeight="1" ht="15.1" r="10">
+    <row r="10" ht="15.1" customHeight="1">
       <c r="C10" s="4" t="n"/>
       <c r="D10" s="4" t="n"/>
     </row>
@@ -5620,8 +5620,8 @@
   <mergeCells count="1">
     <mergeCell ref="G2:H2"/>
   </mergeCells>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" paperSize="1" useFirstPageNumber="1" verticalDpi="300"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup orientation="portrait" paperSize="1" firstPageNumber="0" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
@@ -5642,26 +5642,26 @@
   <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="B2" xSplit="1" ySplit="1"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="topRight" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
-      <selection activeCell="G2" pane="bottomRight" sqref="G2"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2"/>
   <cols>
-    <col customWidth="1" max="1025" min="1" style="15" width="8.78333333333333"/>
+    <col width="8.78333333333333" customWidth="1" style="15" min="1" max="1025"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15.1" r="1">
+    <row r="1" ht="15.1" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='Reference' ObjTablesVersion='0.0.8'</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="15.1" r="2">
+          <t>!!ObjTables type='Data' id='Reference' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15.1" customHeight="1">
       <c r="A2" s="18" t="inlineStr">
         <is>
           <t>!Id</t>
@@ -5753,7 +5753,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.1" r="3">
+    <row r="3" ht="15.1" customHeight="1">
       <c r="A3" s="15" t="inlineStr">
         <is>
           <t>ref_0001</t>
@@ -5851,8 +5851,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:D3"/>
-  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" paperSize="1" useFirstPageNumber="1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup orientation="portrait" paperSize="1" firstPageNumber="0" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
@@ -5865,22 +5865,22 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="C2" xSplit="2" ySplit="1"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="topRight" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomRight" sqref="A1"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" max="16384" min="1" style="15" width="9"/>
+    <col width="9" customWidth="1" style="15" min="1" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='Author' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Data' id='Author' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -5947,7 +5947,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -5960,22 +5960,22 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="B2" xSplit="1" ySplit="1"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="topRight" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
-      <selection activeCell="E1" pane="bottomRight" sqref="E1"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" max="16384" min="1" style="15" width="9"/>
+    <col width="9" customWidth="1" style="15" min="1" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='Change' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Data' id='Change' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -6067,7 +6067,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -6080,24 +6080,24 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="topRight" state="frozen" topLeftCell="B1" xSplit="1"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="B2" pane="topRight" sqref="B2"/>
+      <selection pane="topRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5"/>
   <cols>
-    <col customWidth="1" max="1025" min="1" style="15" width="8.78333333333333"/>
+    <col width="8.78333333333333" customWidth="1" style="15" min="1" max="1025"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15.1" r="1">
+    <row r="1" ht="15.1" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='Taxon' ObjTablesVersion='0.0.8'</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="15.1" r="2">
+          <t>!!ObjTables type='Data' id='Taxon' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='column'</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15.1" customHeight="1">
       <c r="A2" s="18" t="inlineStr">
         <is>
           <t>!Id</t>
@@ -6109,7 +6109,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.1" r="3">
+    <row r="3" ht="15.1" customHeight="1">
       <c r="A3" s="18" t="inlineStr">
         <is>
           <t>!Name</t>
@@ -6121,7 +6121,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.1" r="4">
+    <row r="4" ht="15.1" customHeight="1">
       <c r="A4" s="18" t="inlineStr">
         <is>
           <t>!Rank</t>
@@ -6133,7 +6133,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.1" r="5">
+    <row r="5" ht="15.1" customHeight="1">
       <c r="A5" s="18" t="inlineStr">
         <is>
           <t>!Identifiers</t>
@@ -6145,7 +6145,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.1" r="6">
+    <row r="6" ht="15.1" customHeight="1">
       <c r="A6" s="18" t="inlineStr">
         <is>
           <t>!Comments</t>
@@ -6160,8 +6160,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" paperSize="1" useFirstPageNumber="1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup orientation="portrait" paperSize="1" firstPageNumber="0" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
@@ -6174,24 +6174,24 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="topRight" state="frozen" topLeftCell="B1" xSplit="1"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="B5" pane="topRight" sqref="$A5:$XFD6"/>
+      <selection pane="topRight" activeCell="B5" sqref="$A5:$XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="6"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelRow="6"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="15" width="18.5"/>
-    <col customWidth="1" max="2" min="2" style="15" width="5.375"/>
-    <col customWidth="1" max="1018" min="3" style="15" width="8.78333333333333"/>
-    <col customWidth="1" max="1019" min="1019" style="19" width="8.78333333333333"/>
-    <col customWidth="1" max="16384" min="1020" style="19" width="9"/>
+    <col width="18.5" customWidth="1" style="15" min="1" max="1"/>
+    <col width="5.375" customWidth="1" style="15" min="2" max="2"/>
+    <col width="8.78333333333333" customWidth="1" style="15" min="3" max="1018"/>
+    <col width="8.78333333333333" customWidth="1" style="19" min="1019" max="1019"/>
+    <col width="9" customWidth="1" style="19" min="1020" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='Environment' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Data' id='Environment' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='column'</t>
         </is>
       </c>
     </row>
@@ -6258,7 +6258,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -6271,29 +6271,29 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="B2" xSplit="1" ySplit="1"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="topRight" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
-      <selection activeCell="C1" pane="bottomRight" sqref="C1:C3"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="15" width="13"/>
-    <col customWidth="1" max="2" min="2" style="15" width="13.4416666666667"/>
-    <col customWidth="1" max="3" min="3" style="15" width="13.225"/>
-    <col customWidth="1" max="1026" min="4" style="15" width="8.78333333333333"/>
+    <col width="13" customWidth="1" style="15" min="1" max="1"/>
+    <col width="13.4416666666667" customWidth="1" style="15" min="2" max="2"/>
+    <col width="13.225" customWidth="1" style="15" min="3" max="3"/>
+    <col width="8.78333333333333" customWidth="1" style="15" min="4" max="1026"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15.1" r="1">
+    <row r="1" ht="15.1" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='Submodel' ObjTablesVersion='0.0.8'</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="15.1" r="2">
+          <t>!!ObjTables type='Data' id='Submodel' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15.1" customHeight="1">
       <c r="A2" s="18" t="inlineStr">
         <is>
           <t>!Id</t>
@@ -6335,7 +6335,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.1" r="3">
+    <row r="3" ht="15.1" customHeight="1">
       <c r="A3" s="15" t="inlineStr">
         <is>
           <t>metabolism</t>
@@ -6380,8 +6380,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" paperSize="1" useFirstPageNumber="1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup orientation="portrait" paperSize="1" firstPageNumber="0" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
@@ -6394,26 +6394,26 @@
   <dimension ref="A1:AMR5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="B2" xSplit="1" ySplit="2"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="topRight" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
-      <selection activeCell="M1" pane="bottomRight" sqref="M1:P4"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="M1" sqref="M1:P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3"/>
   <cols>
-    <col customWidth="1" max="1035" min="1" style="15" width="8.78333333333333"/>
+    <col width="8.78333333333333" customWidth="1" style="15" min="1" max="1035"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15" r="1">
+    <row r="1" ht="15" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='Compartment' ObjTablesVersion='0.0.8'</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="15.1" r="2">
+          <t>!!ObjTables type='Data' id='Compartment' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15.1" customHeight="1">
       <c r="A2" s="11" t="n"/>
       <c r="B2" s="11" t="n"/>
       <c r="C2" s="11" t="n"/>
@@ -7449,7 +7449,7 @@
       <c r="AMQ2" s="11" t="n"/>
       <c r="AMR2" s="11" t="n"/>
     </row>
-    <row customHeight="1" ht="15.1" r="3">
+    <row r="3" ht="15.1" customHeight="1">
       <c r="A3" s="18" t="inlineStr">
         <is>
           <t>!Id</t>
@@ -8567,7 +8567,7 @@
       <c r="AMQ3" s="11" t="n"/>
       <c r="AMR3" s="11" t="n"/>
     </row>
-    <row customHeight="1" ht="15.1" r="4">
+    <row r="4" ht="15.1" customHeight="1">
       <c r="A4" s="15" t="inlineStr">
         <is>
           <t>c</t>
@@ -8736,8 +8736,8 @@
     <mergeCell ref="H2:K2"/>
     <mergeCell ref="M2:P2"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" paperSize="1" useFirstPageNumber="1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup orientation="portrait" paperSize="1" firstPageNumber="0" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
@@ -8750,35 +8750,35 @@
   <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="B2" xSplit="1" ySplit="2"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="topRight" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
-      <selection activeCell="E11" pane="bottomRight" sqref="E11"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col customWidth="1" max="5" min="1" style="15" width="8.78333333333333"/>
-    <col customWidth="1" max="6" min="6" style="15" width="17.3083333333333"/>
-    <col customWidth="1" max="1028" min="7" style="15" width="8.78333333333333"/>
+    <col width="8.78333333333333" customWidth="1" style="15" min="1" max="5"/>
+    <col width="17.3083333333333" customWidth="1" style="15" min="6" max="6"/>
+    <col width="8.78333333333333" customWidth="1" style="15" min="7" max="1028"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='SpeciesType' ObjTablesVersion='0.0.8'</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="15.1" r="2">
+          <t>!!ObjTables type='Data' id='SpeciesType' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15.1" customHeight="1">
       <c r="C2" s="17" t="inlineStr">
         <is>
           <t>!Structure</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.1" r="3">
+    <row r="3" ht="15.1" customHeight="1">
       <c r="A3" s="18" t="inlineStr">
         <is>
           <t>!Id</t>
@@ -8850,7 +8850,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.1" r="4">
+    <row r="4" ht="15.1" customHeight="1">
       <c r="A4" s="15" t="inlineStr">
         <is>
           <t>adp</t>
@@ -8894,7 +8894,7 @@
       </c>
       <c r="M4" s="23" t="n"/>
     </row>
-    <row customHeight="1" ht="15.1" r="5">
+    <row r="5" ht="15.1" customHeight="1">
       <c r="A5" s="15" t="inlineStr">
         <is>
           <t>amp</t>
@@ -8938,7 +8938,7 @@
       </c>
       <c r="M5" s="23" t="n"/>
     </row>
-    <row customHeight="1" ht="15.1" r="6">
+    <row r="6" ht="15.1" customHeight="1">
       <c r="A6" s="15" t="inlineStr">
         <is>
           <t>atp</t>
@@ -8982,7 +8982,7 @@
       </c>
       <c r="M6" s="23" t="n"/>
     </row>
-    <row customHeight="1" ht="15.1" r="7">
+    <row r="7" ht="15.1" customHeight="1">
       <c r="A7" s="15" t="inlineStr">
         <is>
           <t>glc</t>
@@ -9021,7 +9021,7 @@
       </c>
       <c r="M7" s="23" t="n"/>
     </row>
-    <row customHeight="1" ht="15.1" r="8">
+    <row r="8" ht="15.1" customHeight="1">
       <c r="A8" s="15" t="inlineStr">
         <is>
           <t>h</t>
@@ -9065,7 +9065,7 @@
       </c>
       <c r="M8" s="23" t="n"/>
     </row>
-    <row customHeight="1" ht="15.1" r="9">
+    <row r="9" ht="15.1" customHeight="1">
       <c r="A9" s="15" t="inlineStr">
         <is>
           <t>h2o</t>
@@ -9108,7 +9108,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.1" r="10">
+    <row r="10" ht="15.1" customHeight="1">
       <c r="A10" s="15" t="inlineStr">
         <is>
           <t>pi</t>
@@ -9151,7 +9151,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.1" r="11">
+    <row r="11" ht="15.1" customHeight="1">
       <c r="A11" s="15" t="inlineStr">
         <is>
           <t>ppi</t>
@@ -9189,7 +9189,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.1" r="12">
+    <row r="12" ht="15.1" customHeight="1">
       <c r="A12" s="15" t="inlineStr">
         <is>
           <t>rna_dec_a</t>
@@ -9273,8 +9273,8 @@
   <mergeCells count="1">
     <mergeCell ref="C2:H2"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" paperSize="1" useFirstPageNumber="1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup orientation="portrait" paperSize="1" firstPageNumber="0" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
@@ -9287,27 +9287,27 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="B2" xSplit="1" ySplit="1"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="topRight" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
-      <selection activeCell="H14" pane="bottomRight" sqref="H14"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col customWidth="1" max="10" min="1" style="15" width="15.9583333333333"/>
-    <col customWidth="1" max="1026" min="11" style="15" width="9.108333333333331"/>
+    <col width="15.9583333333333" customWidth="1" style="15" min="1" max="10"/>
+    <col width="9.108333333333331" customWidth="1" style="15" min="11" max="1026"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15.1" r="1">
+    <row r="1" ht="15.1" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='Species' ObjTablesVersion='0.0.8'</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="15.1" r="2">
+          <t>!!ObjTables type='Data' id='Species' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15.1" customHeight="1">
       <c r="A2" s="18" t="inlineStr">
         <is>
           <t>!Id</t>
@@ -9359,7 +9359,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.1" r="3">
+    <row r="3" ht="15.1" customHeight="1">
       <c r="A3" s="15" t="inlineStr">
         <is>
           <t>adp[c]</t>
@@ -9382,7 +9382,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.1" r="4">
+    <row r="4" ht="15.1" customHeight="1">
       <c r="A4" s="15" t="inlineStr">
         <is>
           <t>amp[c]</t>
@@ -9405,7 +9405,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.1" r="5">
+    <row r="5" ht="15.1" customHeight="1">
       <c r="A5" s="15" t="inlineStr">
         <is>
           <t>atp[c]</t>
@@ -9428,7 +9428,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.1" r="6">
+    <row r="6" ht="15.1" customHeight="1">
       <c r="A6" s="15" t="inlineStr">
         <is>
           <t>biomass[c]</t>
@@ -9451,7 +9451,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.1" r="7">
+    <row r="7" ht="15.1" customHeight="1">
       <c r="A7" s="15" t="inlineStr">
         <is>
           <t>glc[c]</t>
@@ -9474,7 +9474,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.1" r="8">
+    <row r="8" ht="15.1" customHeight="1">
       <c r="A8" s="15" t="inlineStr">
         <is>
           <t>glc[e]</t>
@@ -9497,7 +9497,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.1" r="9">
+    <row r="9" ht="15.1" customHeight="1">
       <c r="A9" s="15" t="inlineStr">
         <is>
           <t>h[c]</t>
@@ -9520,7 +9520,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.1" r="10">
+    <row r="10" ht="15.1" customHeight="1">
       <c r="A10" s="15" t="inlineStr">
         <is>
           <t>h2o[c]</t>
@@ -9543,7 +9543,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.1" r="11">
+    <row r="11" ht="15.1" customHeight="1">
       <c r="A11" s="15" t="inlineStr">
         <is>
           <t>pi[c]</t>
@@ -9590,8 +9590,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" paperSize="1" useFirstPageNumber="1" verticalDpi="300"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup orientation="portrait" paperSize="1" firstPageNumber="0" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
@@ -9612,27 +9612,27 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="B2" xSplit="1" ySplit="1"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="topRight" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
-      <selection activeCell="D8" pane="bottomRight" sqref="D2:D8"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="D8" sqref="D2:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="15" width="16.625"/>
-    <col customWidth="1" max="1026" min="2" style="15" width="8.78333333333333"/>
+    <col width="16.625" customWidth="1" style="15" min="1" max="1"/>
+    <col width="8.78333333333333" customWidth="1" style="15" min="2" max="1026"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15.1" r="1">
+    <row r="1" ht="15.1" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='DistributionInitConcentration' ObjTablesVersion='0.0.8'</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="15.1" r="2">
+          <t>!!ObjTables type='Data' id='DistributionInitConcentration' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15.1" customHeight="1">
       <c r="A2" s="18" t="inlineStr">
         <is>
           <t>!Id</t>
@@ -9694,7 +9694,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.1" r="3">
+    <row r="3" ht="15.1" customHeight="1">
       <c r="A3" s="15" t="inlineStr">
         <is>
           <t>dist-init-conc-adp[c]</t>
@@ -9722,7 +9722,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.1" r="4">
+    <row r="4" ht="15.1" customHeight="1">
       <c r="A4" s="15" t="inlineStr">
         <is>
           <t>dist-init-conc-atp[c]</t>
@@ -9751,7 +9751,7 @@
       <c r="I4" s="23" t="n"/>
       <c r="J4" s="23" t="n"/>
     </row>
-    <row customHeight="1" ht="15.1" r="5">
+    <row r="5" ht="15.1" customHeight="1">
       <c r="A5" s="15" t="inlineStr">
         <is>
           <t>dist-init-conc-glc[c]</t>
@@ -9780,7 +9780,7 @@
       <c r="I5" s="23" t="n"/>
       <c r="J5" s="23" t="n"/>
     </row>
-    <row customHeight="1" ht="15.1" r="6">
+    <row r="6" ht="15.1" customHeight="1">
       <c r="A6" s="15" t="inlineStr">
         <is>
           <t>dist-init-conc-glc[e]</t>
@@ -9809,7 +9809,7 @@
       <c r="I6" s="23" t="n"/>
       <c r="J6" s="23" t="n"/>
     </row>
-    <row customHeight="1" ht="15.1" r="7">
+    <row r="7" ht="15.1" customHeight="1">
       <c r="A7" s="15" t="inlineStr">
         <is>
           <t>dist-init-conc-h[c]</t>
@@ -9838,7 +9838,7 @@
       <c r="I7" s="23" t="n"/>
       <c r="J7" s="23" t="n"/>
     </row>
-    <row customHeight="1" ht="15.1" r="8">
+    <row r="8" ht="15.1" customHeight="1">
       <c r="A8" s="15" t="inlineStr">
         <is>
           <t>dist-init-conc-h2o[c]</t>
@@ -9898,7 +9898,7 @@
     </row>
   </sheetData>
   <autoFilter ref="C1:L8"/>
-  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" paperSize="1" useFirstPageNumber="1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup orientation="portrait" paperSize="1" firstPageNumber="0" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updating for changes to obj_tables
</commit_message>
<xml_diff>
--- a/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
+++ b/intro_to_wc_modeling/wc_modeling/wc_lang_tutorial/examples/example_model.xlsx
@@ -1571,7 +1571,7 @@
     <row r="1" ht="15.1" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables type='Data' id='Observable' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
+          <t>!!ObjTables type='Data' class='Observable' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -1662,7 +1662,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables type='Data' id='Function' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
+          <t>!!ObjTables type='Data' class='Function' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -1789,7 +1789,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables type='Data' id='Reaction' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
+          <t>!!ObjTables type='Data' class='Reaction' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -4073,7 +4073,7 @@
     <row r="1" ht="15.1" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables type='Data' id='RateLaw' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
+          <t>!!ObjTables type='Data' class='RateLaw' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -4313,7 +4313,7 @@
     <row r="1" ht="15.1" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables type='Data' id='DfbaObjective' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
+          <t>!!ObjTables type='Data' class='DfbaObjective' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -4449,7 +4449,7 @@
     <row r="1" ht="15.1" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables type='Data' id='DfbaObjReaction' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
+          <t>!!ObjTables type='Data' class='DfbaObjReaction' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -4543,7 +4543,7 @@
     <row r="1" ht="15.1" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables type='Data' id='DfbaObjSpecies' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
+          <t>!!ObjTables type='Data' class='DfbaObjSpecies' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -4642,7 +4642,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables type='Data' id='Parameter' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
+          <t>!!ObjTables type='Data' class='Parameter' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -4964,7 +4964,7 @@
     <row r="1" ht="15.1" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables type='Data' id='StopCondition' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
+          <t>!!ObjTables type='Data' class='StopCondition' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -5053,7 +5053,7 @@
     <row r="1" ht="15" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables type='Data' id='Observation' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
+          <t>!!ObjTables type='Data' class='Observation' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -5254,7 +5254,7 @@
     <row r="1" ht="15.1" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables type='Data' id='Model' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='column'</t>
+          <t>!!ObjTables type='Data' class='Model' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='column'</t>
         </is>
       </c>
     </row>
@@ -5417,7 +5417,7 @@
     <row r="1" ht="15.1" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables type='Data' id='ObservationSet' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
+          <t>!!ObjTables type='Data' class='ObservationSet' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -5501,7 +5501,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables type='Data' id='Conclusion' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
+          <t>!!ObjTables type='Data' class='Conclusion' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -5657,7 +5657,7 @@
     <row r="1" ht="15.1" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables type='Data' id='Reference' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
+          <t>!!ObjTables type='Data' class='Reference' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -5880,7 +5880,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables type='Data' id='Author' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
+          <t>!!ObjTables type='Data' class='Author' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -5975,7 +5975,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables type='Data' id='Change' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
+          <t>!!ObjTables type='Data' class='Change' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -6093,7 +6093,7 @@
     <row r="1" ht="15.1" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables type='Data' id='Taxon' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='column'</t>
+          <t>!!ObjTables type='Data' class='Taxon' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='column'</t>
         </is>
       </c>
     </row>
@@ -6191,7 +6191,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables type='Data' id='Environment' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='column'</t>
+          <t>!!ObjTables type='Data' class='Environment' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='column'</t>
         </is>
       </c>
     </row>
@@ -6289,7 +6289,7 @@
     <row r="1" ht="15.1" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables type='Data' id='Submodel' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
+          <t>!!ObjTables type='Data' class='Submodel' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -6409,7 +6409,7 @@
     <row r="1" ht="15" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables type='Data' id='Compartment' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
+          <t>!!ObjTables type='Data' class='Compartment' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -8767,7 +8767,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables type='Data' id='SpeciesType' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
+          <t>!!ObjTables type='Data' class='SpeciesType' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -9303,7 +9303,7 @@
     <row r="1" ht="15.1" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables type='Data' id='Species' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
+          <t>!!ObjTables type='Data' class='Species' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -9628,7 +9628,7 @@
     <row r="1" ht="15.1" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables type='Data' id='DistributionInitConcentration' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
+          <t>!!ObjTables type='Data' class='DistributionInitConcentration' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>

</xml_diff>